<commit_message>
Update tiền ăn, rút tiền sport 1 160 Zeus + 270 Hecquyn
</commit_message>
<xml_diff>
--- a/Project/TongHopQuy2.xlsx
+++ b/Project/TongHopQuy2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ViTechSolution_LTD\Team_Log\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ViTechSolution_LTD\04.Team_Log\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50508D57-BB63-4BE5-BD3C-7F842F6CC6D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393E4AB6-BC22-4930-A3BD-A3C5F8076AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tổng hợp quỹ công ty" sheetId="6" r:id="rId1"/>
@@ -18,45 +18,46 @@
     <sheet name="SPORT1_P1.5" sheetId="3" r:id="rId3"/>
     <sheet name="Sport1_Thu" sheetId="13" r:id="rId4"/>
     <sheet name="160_Zeus" sheetId="12" r:id="rId5"/>
-    <sheet name="SPORT1_P2" sheetId="4" r:id="rId6"/>
-    <sheet name="SMARTHOME" sheetId="5" r:id="rId7"/>
-    <sheet name="Chi Phí Công ty" sheetId="8" r:id="rId8"/>
-    <sheet name="270_Hecquyn" sheetId="10" r:id="rId9"/>
+    <sheet name="270_Hecquyn" sheetId="10" r:id="rId6"/>
+    <sheet name="SPORT1_P2" sheetId="4" r:id="rId7"/>
+    <sheet name="SMARTHOME" sheetId="5" r:id="rId8"/>
+    <sheet name="Chi Phí Công ty" sheetId="8" r:id="rId9"/>
+    <sheet name="Quản lý tài khoản CT" sheetId="14" r:id="rId10"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId10"/>
+    <externalReference r:id="rId11"/>
   </externalReferences>
   <definedNames>
-    <definedName name="chi_phi_cong_ty">'Chi Phí Công ty'!$G$75</definedName>
+    <definedName name="chi_phi_cong_ty">'Chi Phí Công ty'!$G$77</definedName>
     <definedName name="Pega">PEGA!$G$46</definedName>
     <definedName name="RowTitleRegion1..C7" localSheetId="4">#REF!</definedName>
+    <definedName name="RowTitleRegion1..C7" localSheetId="5">#REF!</definedName>
     <definedName name="RowTitleRegion1..C7" localSheetId="8">#REF!</definedName>
+    <definedName name="RowTitleRegion1..C7" localSheetId="1">#REF!</definedName>
     <definedName name="RowTitleRegion1..C7" localSheetId="7">#REF!</definedName>
-    <definedName name="RowTitleRegion1..C7" localSheetId="1">#REF!</definedName>
+    <definedName name="RowTitleRegion1..C7" localSheetId="2">#REF!</definedName>
     <definedName name="RowTitleRegion1..C7" localSheetId="6">#REF!</definedName>
-    <definedName name="RowTitleRegion1..C7" localSheetId="2">#REF!</definedName>
-    <definedName name="RowTitleRegion1..C7" localSheetId="5">#REF!</definedName>
     <definedName name="RowTitleRegion1..C7">#REF!</definedName>
     <definedName name="RowTitleRegion2..G5" localSheetId="4">#REF!</definedName>
+    <definedName name="RowTitleRegion2..G5" localSheetId="5">#REF!</definedName>
     <definedName name="RowTitleRegion2..G5" localSheetId="8">#REF!</definedName>
+    <definedName name="RowTitleRegion2..G5" localSheetId="1">#REF!</definedName>
     <definedName name="RowTitleRegion2..G5" localSheetId="7">#REF!</definedName>
-    <definedName name="RowTitleRegion2..G5" localSheetId="1">#REF!</definedName>
+    <definedName name="RowTitleRegion2..G5" localSheetId="2">#REF!</definedName>
     <definedName name="RowTitleRegion2..G5" localSheetId="6">#REF!</definedName>
-    <definedName name="RowTitleRegion2..G5" localSheetId="2">#REF!</definedName>
-    <definedName name="RowTitleRegion2..G5" localSheetId="5">#REF!</definedName>
     <definedName name="RowTitleRegion2..G5">#REF!</definedName>
     <definedName name="RowTitleRegion3..G26" localSheetId="4">[1]Effort_08062020!#REF!</definedName>
+    <definedName name="RowTitleRegion3..G26" localSheetId="5">[1]Effort_08062020!#REF!</definedName>
     <definedName name="RowTitleRegion3..G26" localSheetId="8">[1]Effort_08062020!#REF!</definedName>
+    <definedName name="RowTitleRegion3..G26" localSheetId="1">[1]Effort_08062020!#REF!</definedName>
     <definedName name="RowTitleRegion3..G26" localSheetId="7">[1]Effort_08062020!#REF!</definedName>
-    <definedName name="RowTitleRegion3..G26" localSheetId="1">[1]Effort_08062020!#REF!</definedName>
+    <definedName name="RowTitleRegion3..G26" localSheetId="2">[1]Effort_08062020!#REF!</definedName>
     <definedName name="RowTitleRegion3..G26" localSheetId="6">[1]Effort_08062020!#REF!</definedName>
-    <definedName name="RowTitleRegion3..G26" localSheetId="2">[1]Effort_08062020!#REF!</definedName>
-    <definedName name="RowTitleRegion3..G26" localSheetId="5">[1]Effort_08062020!#REF!</definedName>
     <definedName name="RowTitleRegion3..G26">[1]Effort_08062020!#REF!</definedName>
-    <definedName name="smarthome" localSheetId="7">'Chi Phí Công ty'!$G$75</definedName>
+    <definedName name="smarthome" localSheetId="8">'Chi Phí Công ty'!$G$77</definedName>
     <definedName name="smarthome">SMARTHOME!$G$32</definedName>
     <definedName name="sport1_p1.5" localSheetId="4">'160_Zeus'!$G$43</definedName>
-    <definedName name="sport1_p1.5" localSheetId="8">'270_Hecquyn'!$G$42</definedName>
+    <definedName name="sport1_p1.5" localSheetId="5">'270_Hecquyn'!$G$42</definedName>
     <definedName name="sport1_p1.5">SPORT1_P1.5!$G$59</definedName>
     <definedName name="sport1_p2">SPORT1_P2!$G$32</definedName>
   </definedNames>
@@ -70,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="190">
   <si>
     <t>STT</t>
   </si>
@@ -586,6 +587,62 @@
   </si>
   <si>
     <t>300 hddt mới</t>
+  </si>
+  <si>
+    <t>Thời gian</t>
+  </si>
+  <si>
+    <t>Nội dung thu vào</t>
+  </si>
+  <si>
+    <t>Nội dung rút ra</t>
+  </si>
+  <si>
+    <t>Số tiền</t>
+  </si>
+  <si>
+    <t>Thanh toán : 
+200xMS51 : 160_Zeus
+300 con STM32f102, Đặt mạch test: 270 Hecquyn</t>
+  </si>
+  <si>
+    <t>Thuế VAT  + 50% 72 mạch zeus</t>
+  </si>
+  <si>
+    <t>Tiền đặt linh kiện PEGA</t>
+  </si>
+  <si>
+    <t>Tổng rút ra</t>
+  </si>
+  <si>
+    <t>Anh Khơ rút</t>
+  </si>
+  <si>
+    <t>Tuấn rút</t>
+  </si>
+  <si>
+    <t>Rút thêm</t>
+  </si>
+  <si>
+    <t>tiền cơm ngày 12/06</t>
+  </si>
+  <si>
+    <t>Tiền cơm ngày 13/06</t>
+  </si>
+  <si>
+    <t>Cọc 50%</t>
+  </si>
+  <si>
+    <t>Ck 50 % đặt mạch anh Thịnh</t>
+  </si>
+  <si>
+    <t>Vào tk cá nhân ACB</t>
+  </si>
+  <si>
+    <t>Rút thêm 25tr tiền đặt mạch Zeus + Hecquyn</t>
+  </si>
+  <si>
+    <t>Chuyển vào tk cá nhân TPBank Tuấn</t>
   </si>
 </sst>
 </file>
@@ -686,7 +743,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -726,6 +783,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -810,7 +873,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1030,21 +1093,6 @@
     </xf>
     <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1063,6 +1111,26 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="13" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1391,12 +1459,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="8:11" ht="20.25">
-      <c r="H2" s="81" t="s">
+      <c r="H2" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="93"/>
+      <c r="K2" s="93"/>
     </row>
     <row r="3" spans="8:11" ht="15.75">
       <c r="H3" s="6" t="s">
@@ -1421,7 +1489,7 @@
       </c>
       <c r="J4" s="11">
         <f>chi_phi_cong_ty</f>
-        <v>-31728700</v>
+        <v>-32058700</v>
       </c>
       <c r="K4" s="8"/>
     </row>
@@ -1492,7 +1560,7 @@
       <c r="I12" s="9"/>
       <c r="J12" s="12">
         <f>SUM(J4:J11)</f>
-        <v>-71168766.400000006</v>
+        <v>-71498766.400000006</v>
       </c>
       <c r="K12" s="13" t="s">
         <v>7</v>
@@ -1503,6 +1571,128 @@
     <mergeCell ref="H2:K2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36E1739C-0CA9-4D70-99CB-9453E6E8DAF2}">
+  <dimension ref="A1:H14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="42.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" style="81" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="29.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="90" t="s">
+        <v>172</v>
+      </c>
+      <c r="B1" s="90" t="s">
+        <v>173</v>
+      </c>
+      <c r="C1" s="90" t="s">
+        <v>174</v>
+      </c>
+      <c r="D1" s="92" t="s">
+        <v>175</v>
+      </c>
+      <c r="E1" s="90" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="60">
+      <c r="C2" s="91" t="s">
+        <v>176</v>
+      </c>
+      <c r="D2" s="81">
+        <v>14064000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="C3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D3" s="81">
+        <v>8295653.599999994</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="C4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D4" s="81">
+        <v>22200000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="C5" t="s">
+        <v>182</v>
+      </c>
+      <c r="D5" s="81">
+        <v>40346</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="C7" t="s">
+        <v>188</v>
+      </c>
+      <c r="D7" s="81">
+        <v>25000000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="D11" s="81">
+        <f>SUM(D2:D9)</f>
+        <v>69599999.599999994</v>
+      </c>
+      <c r="E11" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="D12" s="81">
+        <v>25000000</v>
+      </c>
+      <c r="E12" t="s">
+        <v>180</v>
+      </c>
+      <c r="F12" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="D13" s="81">
+        <v>25000000</v>
+      </c>
+      <c r="E13" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="D14" s="81">
+        <f>D11-D13</f>
+        <v>44599999.599999994</v>
+      </c>
+      <c r="E14" t="s">
+        <v>181</v>
+      </c>
+      <c r="F14" t="s">
+        <v>187</v>
+      </c>
+      <c r="H14" s="81"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1529,16 +1719,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:10" ht="20.25">
-      <c r="C2" s="81" t="s">
+      <c r="C2" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="93"/>
     </row>
     <row r="3" spans="3:10" ht="15.75">
       <c r="C3" s="6" t="s">
@@ -1568,12 +1758,12 @@
     </row>
     <row r="4" spans="3:10" ht="15.75" customHeight="1">
       <c r="C4" s="7"/>
-      <c r="D4" s="82" t="s">
+      <c r="D4" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="83"/>
-      <c r="F4" s="83"/>
-      <c r="G4" s="84"/>
+      <c r="E4" s="95"/>
+      <c r="F4" s="95"/>
+      <c r="G4" s="96"/>
       <c r="H4" s="26"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
@@ -1640,12 +1830,12 @@
     </row>
     <row r="9" spans="3:10" ht="15">
       <c r="C9" s="8"/>
-      <c r="D9" s="82" t="s">
+      <c r="D9" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="83"/>
-      <c r="F9" s="83"/>
-      <c r="G9" s="84"/>
+      <c r="E9" s="95"/>
+      <c r="F9" s="95"/>
+      <c r="G9" s="96"/>
       <c r="H9" s="26"/>
       <c r="I9" s="14"/>
       <c r="J9" s="15"/>
@@ -1997,7 +2187,7 @@
         <v>2685000</v>
       </c>
       <c r="G25" s="11">
-        <f>E25*F25</f>
+        <f t="shared" ref="G25:G30" si="3">E25*F25</f>
         <v>2685000</v>
       </c>
       <c r="H25" s="70" t="s">
@@ -2018,7 +2208,7 @@
         <v>4298000</v>
       </c>
       <c r="G26" s="11">
-        <f>E26*F26</f>
+        <f t="shared" si="3"/>
         <v>4298000</v>
       </c>
       <c r="H26" s="70" t="s">
@@ -2039,7 +2229,7 @@
         <v>220000</v>
       </c>
       <c r="G27" s="78">
-        <f>E27*F27</f>
+        <f t="shared" si="3"/>
         <v>220000</v>
       </c>
       <c r="H27" s="79" t="s">
@@ -2060,7 +2250,7 @@
         <v>52000</v>
       </c>
       <c r="G28" s="78">
-        <f>E28*F28</f>
+        <f t="shared" si="3"/>
         <v>52000</v>
       </c>
       <c r="H28" s="79" t="s">
@@ -2081,7 +2271,7 @@
         <v>1200000</v>
       </c>
       <c r="G29" s="78">
-        <f>E29*F29</f>
+        <f t="shared" si="3"/>
         <v>1200000</v>
       </c>
       <c r="H29" s="79" t="s">
@@ -2102,7 +2292,7 @@
         <v>160000</v>
       </c>
       <c r="G30" s="78">
-        <f>E30*F30</f>
+        <f t="shared" si="3"/>
         <v>160000</v>
       </c>
       <c r="H30" s="79" t="s">
@@ -2146,12 +2336,12 @@
     </row>
     <row r="34" spans="3:10" ht="15">
       <c r="C34" s="8"/>
-      <c r="D34" s="82" t="s">
+      <c r="D34" s="94" t="s">
         <v>12</v>
       </c>
-      <c r="E34" s="83"/>
-      <c r="F34" s="83"/>
-      <c r="G34" s="84"/>
+      <c r="E34" s="95"/>
+      <c r="F34" s="95"/>
+      <c r="G34" s="96"/>
       <c r="H34" s="26"/>
       <c r="I34" s="11"/>
       <c r="J34" s="9"/>
@@ -2186,12 +2376,12 @@
     </row>
     <row r="37" spans="3:10" ht="15">
       <c r="C37" s="8"/>
-      <c r="D37" s="82" t="s">
+      <c r="D37" s="94" t="s">
         <v>27</v>
       </c>
-      <c r="E37" s="83"/>
-      <c r="F37" s="83"/>
-      <c r="G37" s="84"/>
+      <c r="E37" s="95"/>
+      <c r="F37" s="95"/>
+      <c r="G37" s="96"/>
       <c r="H37" s="27"/>
       <c r="I37" s="11"/>
       <c r="J37" s="8"/>
@@ -2328,7 +2518,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06BE7A19-D435-4A51-A018-E212475E8992}">
   <dimension ref="C2:M59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C4" sqref="C4:J8"/>
     </sheetView>
   </sheetViews>
@@ -2349,16 +2539,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:10" ht="20.25">
-      <c r="C2" s="81" t="s">
+      <c r="C2" s="93" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="93"/>
     </row>
     <row r="3" spans="3:10" ht="15.75">
       <c r="C3" s="6" t="s">
@@ -2388,12 +2578,12 @@
     </row>
     <row r="4" spans="3:10" ht="15.75" customHeight="1">
       <c r="C4" s="7"/>
-      <c r="D4" s="85" t="s">
+      <c r="D4" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="85"/>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
+      <c r="E4" s="97"/>
+      <c r="F4" s="97"/>
+      <c r="G4" s="97"/>
       <c r="H4" s="54"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
@@ -2478,12 +2668,12 @@
     </row>
     <row r="9" spans="3:10" ht="15">
       <c r="C9" s="8"/>
-      <c r="D9" s="85" t="s">
+      <c r="D9" s="97" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="85"/>
-      <c r="F9" s="85"/>
-      <c r="G9" s="85"/>
+      <c r="E9" s="97"/>
+      <c r="F9" s="97"/>
+      <c r="G9" s="97"/>
       <c r="H9" s="54"/>
       <c r="I9" s="14"/>
       <c r="J9" s="15"/>
@@ -2897,12 +3087,12 @@
     </row>
     <row r="30" spans="3:13" ht="15">
       <c r="C30" s="8"/>
-      <c r="D30" s="85" t="s">
+      <c r="D30" s="97" t="s">
         <v>30</v>
       </c>
-      <c r="E30" s="85"/>
-      <c r="F30" s="85"/>
-      <c r="G30" s="85"/>
+      <c r="E30" s="97"/>
+      <c r="F30" s="97"/>
+      <c r="G30" s="97"/>
       <c r="H30" s="54"/>
       <c r="I30" s="11"/>
       <c r="J30" s="9"/>
@@ -2929,10 +3119,10 @@
       </c>
       <c r="I31" s="11"/>
       <c r="J31" s="9"/>
-      <c r="L31" s="87" t="s">
+      <c r="L31" s="82" t="s">
         <v>158</v>
       </c>
-      <c r="M31" s="88">
+      <c r="M31" s="83">
         <f>SUM(G33:G37)+G44</f>
         <v>4145000</v>
       </c>
@@ -2959,10 +3149,10 @@
       </c>
       <c r="I32" s="11"/>
       <c r="J32" s="9"/>
-      <c r="L32" s="87" t="s">
-        <v>9</v>
-      </c>
-      <c r="M32" s="88">
+      <c r="L32" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="M32" s="83">
         <f>G31+G32+G39+G40+G41</f>
         <v>1677000</v>
       </c>
@@ -3286,24 +3476,24 @@
       <c r="D49" s="30"/>
       <c r="E49" s="38"/>
       <c r="F49" s="29"/>
-      <c r="G49" s="92">
+      <c r="G49" s="87">
         <f>G8-G48</f>
         <v>5121999.599999994</v>
       </c>
-      <c r="H49" s="93"/>
-      <c r="I49" s="94"/>
+      <c r="H49" s="88"/>
+      <c r="I49" s="89"/>
       <c r="J49" s="31" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="50" spans="3:10" ht="15">
       <c r="C50" s="8"/>
-      <c r="D50" s="85" t="s">
+      <c r="D50" s="97" t="s">
         <v>27</v>
       </c>
-      <c r="E50" s="85"/>
-      <c r="F50" s="85"/>
-      <c r="G50" s="85"/>
+      <c r="E50" s="97"/>
+      <c r="F50" s="97"/>
+      <c r="G50" s="97"/>
       <c r="H50" s="57"/>
       <c r="I50" s="11"/>
       <c r="J50" s="8"/>
@@ -3439,35 +3629,35 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D3E46B6-EEA2-499C-B73A-039F7F75D799}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="24.28515625" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" style="86" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" style="81" customWidth="1"/>
     <col min="4" max="4" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="85" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="90" t="s">
+      <c r="B1" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="91" t="s">
+      <c r="C1" s="86" t="s">
         <v>162</v>
       </c>
-      <c r="D1" s="90" t="s">
+      <c r="D1" s="85" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="84" t="s">
         <v>159</v>
       </c>
       <c r="B2" s="30">
@@ -3480,7 +3670,7 @@
       <c r="D2" s="30"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="89" t="s">
+      <c r="A3" s="84" t="s">
         <v>160</v>
       </c>
       <c r="B3" s="30">
@@ -3493,7 +3683,7 @@
       <c r="D3" s="30"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="89" t="s">
+      <c r="A4" s="84" t="s">
         <v>156</v>
       </c>
       <c r="B4" s="30">
@@ -3505,7 +3695,7 @@
       <c r="D4" s="30"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="89" t="s">
+      <c r="A5" s="84" t="s">
         <v>157</v>
       </c>
       <c r="B5" s="30"/>
@@ -3518,13 +3708,13 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="89"/>
+      <c r="A6" s="84"/>
       <c r="B6" s="30"/>
       <c r="C6" s="29"/>
       <c r="D6" s="30"/>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="89" t="s">
+      <c r="A7" s="84" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="30"/>
@@ -3532,6 +3722,12 @@
         <v>75919214</v>
       </c>
       <c r="D7" s="30"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="D13" s="81">
+        <f>SUM(C4:C5)</f>
+        <v>8295653.599999994</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3544,7 +3740,7 @@
   <dimension ref="C2:J43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3562,16 +3758,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:10" ht="20.25">
-      <c r="C2" s="81" t="s">
+      <c r="C2" s="93" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="93"/>
     </row>
     <row r="3" spans="3:10" ht="15.75">
       <c r="C3" s="6" t="s">
@@ -3601,12 +3797,12 @@
     </row>
     <row r="4" spans="3:10" ht="15.75" customHeight="1">
       <c r="C4" s="7"/>
-      <c r="D4" s="85" t="s">
+      <c r="D4" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="85"/>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
+      <c r="E4" s="97"/>
+      <c r="F4" s="97"/>
+      <c r="G4" s="97"/>
       <c r="H4" s="80"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
@@ -3692,7 +3888,7 @@
       <c r="F9" s="48"/>
       <c r="G9" s="49">
         <f>G8-G33</f>
-        <v>33528910</v>
+        <v>30528910</v>
       </c>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
@@ -3702,12 +3898,12 @@
     </row>
     <row r="10" spans="3:10" ht="15">
       <c r="C10" s="8"/>
-      <c r="D10" s="85" t="s">
+      <c r="D10" s="97" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="85"/>
-      <c r="F10" s="85"/>
-      <c r="G10" s="85"/>
+      <c r="E10" s="97"/>
+      <c r="F10" s="97"/>
+      <c r="G10" s="97"/>
       <c r="H10" s="76"/>
       <c r="I10" s="14"/>
       <c r="J10" s="15"/>
@@ -3749,12 +3945,12 @@
     </row>
     <row r="14" spans="3:10" ht="15">
       <c r="C14" s="8"/>
-      <c r="D14" s="85" t="s">
+      <c r="D14" s="97" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="85"/>
-      <c r="F14" s="85"/>
-      <c r="G14" s="85"/>
+      <c r="E14" s="97"/>
+      <c r="F14" s="97"/>
+      <c r="G14" s="97"/>
       <c r="H14" s="76"/>
       <c r="I14" s="11"/>
       <c r="J14" s="9"/>
@@ -3782,11 +3978,22 @@
     </row>
     <row r="16" spans="3:10" ht="15">
       <c r="C16" s="8"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="30"/>
+      <c r="D16" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="E16" s="38">
+        <v>1</v>
+      </c>
+      <c r="F16" s="29">
+        <v>3000000</v>
+      </c>
+      <c r="G16" s="29">
+        <f t="shared" ref="G16:G18" si="0">F16*E16</f>
+        <v>3000000</v>
+      </c>
+      <c r="H16" s="30" t="s">
+        <v>51</v>
+      </c>
       <c r="I16" s="11"/>
       <c r="J16" s="9"/>
     </row>
@@ -3795,7 +4002,10 @@
       <c r="D17" s="1"/>
       <c r="E17" s="3"/>
       <c r="F17" s="39"/>
-      <c r="G17" s="29"/>
+      <c r="G17" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H17" s="30"/>
       <c r="I17" s="11"/>
       <c r="J17" s="9"/>
@@ -3805,7 +4015,10 @@
       <c r="D18" s="1"/>
       <c r="E18" s="3"/>
       <c r="F18" s="39"/>
-      <c r="G18" s="29"/>
+      <c r="G18" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H18" s="30"/>
       <c r="I18" s="11"/>
       <c r="J18" s="9"/>
@@ -3957,7 +4170,7 @@
       <c r="F33" s="29"/>
       <c r="G33" s="55">
         <f>SUM(G15:G32)</f>
-        <v>4800000</v>
+        <v>7800000</v>
       </c>
       <c r="H33" s="56"/>
       <c r="I33" s="35"/>
@@ -3967,12 +4180,12 @@
     </row>
     <row r="34" spans="3:10" ht="15">
       <c r="C34" s="8"/>
-      <c r="D34" s="85" t="s">
+      <c r="D34" s="97" t="s">
         <v>27</v>
       </c>
-      <c r="E34" s="85"/>
-      <c r="F34" s="85"/>
-      <c r="G34" s="85"/>
+      <c r="E34" s="97"/>
+      <c r="F34" s="97"/>
+      <c r="G34" s="97"/>
       <c r="H34" s="57"/>
       <c r="I34" s="11"/>
       <c r="J34" s="8"/>
@@ -4085,7 +4298,7 @@
       <c r="F43" s="48"/>
       <c r="G43" s="49">
         <f>G8-G13-G33</f>
-        <v>33528910</v>
+        <v>30528910</v>
       </c>
       <c r="H43" s="12"/>
       <c r="I43" s="20"/>
@@ -4107,11 +4320,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F413B64-656B-492A-8F7D-8434699F234E}">
-  <dimension ref="C2:J32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A00FBF6-6528-4077-97A8-E7F8FA86DD30}">
+  <dimension ref="C2:J42"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4129,16 +4342,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:10" ht="20.25">
-      <c r="C2" s="81" t="s">
-        <v>66</v>
-      </c>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
+      <c r="C2" s="93" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="93"/>
     </row>
     <row r="3" spans="3:10" ht="15.75">
       <c r="C3" s="6" t="s">
@@ -4168,12 +4381,606 @@
     </row>
     <row r="4" spans="3:10" ht="15.75" customHeight="1">
       <c r="C4" s="7"/>
-      <c r="D4" s="85" t="s">
+      <c r="D4" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="85"/>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
+      <c r="E4" s="97"/>
+      <c r="F4" s="97"/>
+      <c r="G4" s="97"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+    </row>
+    <row r="5" spans="3:10" ht="20.25">
+      <c r="C5" s="7"/>
+      <c r="D5" s="97" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="97"/>
+      <c r="F5" s="97"/>
+      <c r="G5" s="97"/>
+      <c r="H5" s="80"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+    </row>
+    <row r="6" spans="3:10">
+      <c r="C6" s="8">
+        <v>1</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="10">
+        <v>1</v>
+      </c>
+      <c r="F6" s="48">
+        <v>29294650.400000002</v>
+      </c>
+      <c r="G6" s="48">
+        <f>F6*E6</f>
+        <v>29294650.400000002</v>
+      </c>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="8"/>
+    </row>
+    <row r="7" spans="3:10">
+      <c r="C7" s="8">
+        <v>2</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E7" s="10">
+        <v>1</v>
+      </c>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48">
+        <f>F7*E7</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="9"/>
+    </row>
+    <row r="8" spans="3:10">
+      <c r="C8" s="8">
+        <v>3</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="E8" s="10">
+        <v>1</v>
+      </c>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48">
+        <f>F8*E8</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="9"/>
+    </row>
+    <row r="9" spans="3:10" ht="15">
+      <c r="C9" s="8"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="49">
+        <f>SUM(G6:G8)</f>
+        <v>29294650.400000002</v>
+      </c>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" ht="15">
+      <c r="C10" s="8"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="9"/>
+    </row>
+    <row r="11" spans="3:10" ht="15">
+      <c r="C11" s="8"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="9"/>
+    </row>
+    <row r="12" spans="3:10" ht="15">
+      <c r="C12" s="8"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="55">
+        <f>SUM(G10:G10)</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="56"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10" ht="15">
+      <c r="C13" s="8"/>
+      <c r="D13" s="97" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="97"/>
+      <c r="F13" s="97"/>
+      <c r="G13" s="97"/>
+      <c r="H13" s="74"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="9"/>
+    </row>
+    <row r="14" spans="3:10" ht="15">
+      <c r="C14" s="8"/>
+      <c r="D14" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="E14" s="38">
+        <v>1</v>
+      </c>
+      <c r="F14" s="29">
+        <v>9064000</v>
+      </c>
+      <c r="G14" s="29">
+        <f>F14*E14</f>
+        <v>9064000</v>
+      </c>
+      <c r="H14" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" s="11"/>
+      <c r="J14" s="9"/>
+    </row>
+    <row r="15" spans="3:10" ht="15">
+      <c r="C15" s="8"/>
+      <c r="D15" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="E15" s="38">
+        <v>1</v>
+      </c>
+      <c r="F15" s="29">
+        <v>200000</v>
+      </c>
+      <c r="G15" s="29">
+        <f>F15*E15</f>
+        <v>200000</v>
+      </c>
+      <c r="H15" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" s="11"/>
+      <c r="J15" s="9"/>
+    </row>
+    <row r="16" spans="3:10" ht="15">
+      <c r="C16" s="8"/>
+      <c r="D16" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E16" s="3">
+        <v>1</v>
+      </c>
+      <c r="F16" s="39">
+        <v>21000000</v>
+      </c>
+      <c r="G16" s="29">
+        <f t="shared" ref="G16:G23" si="0">F16*E16</f>
+        <v>21000000</v>
+      </c>
+      <c r="H16" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="I16" s="11"/>
+      <c r="J16" s="9"/>
+    </row>
+    <row r="17" spans="3:10" ht="15">
+      <c r="C17" s="8"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H17" s="30"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="9"/>
+    </row>
+    <row r="18" spans="3:10" ht="15">
+      <c r="C18" s="8"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H18" s="30"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="9"/>
+    </row>
+    <row r="19" spans="3:10" ht="15">
+      <c r="C19" s="8"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H19" s="30"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="9"/>
+    </row>
+    <row r="20" spans="3:10" s="46" customFormat="1" ht="15">
+      <c r="C20" s="8"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H20" s="45"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="41"/>
+    </row>
+    <row r="21" spans="3:10" ht="15">
+      <c r="C21" s="8"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="15"/>
+    </row>
+    <row r="22" spans="3:10" ht="15">
+      <c r="C22" s="8"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H22" s="30"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="9"/>
+    </row>
+    <row r="23" spans="3:10" ht="15">
+      <c r="C23" s="8"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H23" s="30"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="9"/>
+    </row>
+    <row r="24" spans="3:10" ht="15">
+      <c r="C24" s="8"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="9"/>
+    </row>
+    <row r="25" spans="3:10" ht="15">
+      <c r="C25" s="8"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="9"/>
+    </row>
+    <row r="26" spans="3:10" ht="15">
+      <c r="C26" s="8"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="9"/>
+    </row>
+    <row r="27" spans="3:10" ht="15">
+      <c r="C27" s="8"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="9"/>
+    </row>
+    <row r="28" spans="3:10" ht="15">
+      <c r="C28" s="8"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="9"/>
+    </row>
+    <row r="29" spans="3:10" ht="15">
+      <c r="C29" s="8"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="9"/>
+    </row>
+    <row r="30" spans="3:10" ht="15">
+      <c r="C30" s="8"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="9"/>
+    </row>
+    <row r="31" spans="3:10" ht="15">
+      <c r="C31" s="8"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="75"/>
+    </row>
+    <row r="32" spans="3:10" ht="15">
+      <c r="C32" s="8"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="38"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="55">
+        <f>SUM(G14:G31)</f>
+        <v>30264000</v>
+      </c>
+      <c r="H32" s="56"/>
+      <c r="I32" s="35"/>
+      <c r="J32" s="33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="3:10" ht="15">
+      <c r="C33" s="8"/>
+      <c r="D33" s="97" t="s">
+        <v>27</v>
+      </c>
+      <c r="E33" s="97"/>
+      <c r="F33" s="97"/>
+      <c r="G33" s="97"/>
+      <c r="H33" s="57"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="8"/>
+    </row>
+    <row r="34" spans="3:10" ht="15">
+      <c r="C34" s="8">
+        <v>1</v>
+      </c>
+      <c r="D34" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="10"/>
+      <c r="F34" s="48"/>
+      <c r="G34" s="50"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="14"/>
+      <c r="J34" s="34"/>
+    </row>
+    <row r="35" spans="3:10" ht="15">
+      <c r="C35" s="8">
+        <v>2</v>
+      </c>
+      <c r="D35" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="10"/>
+      <c r="F35" s="48"/>
+      <c r="G35" s="50"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="22"/>
+    </row>
+    <row r="36" spans="3:10" ht="15">
+      <c r="C36" s="8">
+        <v>3</v>
+      </c>
+      <c r="D36" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" s="10"/>
+      <c r="F36" s="48"/>
+      <c r="G36" s="50"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="22"/>
+    </row>
+    <row r="37" spans="3:10" ht="15">
+      <c r="C37" s="8">
+        <v>4</v>
+      </c>
+      <c r="D37" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" s="10"/>
+      <c r="F37" s="48"/>
+      <c r="G37" s="50"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="22"/>
+    </row>
+    <row r="38" spans="3:10" ht="15">
+      <c r="C38" s="8"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="48"/>
+      <c r="G38" s="50"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="22"/>
+    </row>
+    <row r="39" spans="3:10" ht="15">
+      <c r="C39" s="8"/>
+      <c r="D39" s="36"/>
+      <c r="E39" s="37"/>
+      <c r="F39" s="53"/>
+      <c r="G39" s="51">
+        <f>SUM(G34:G38)</f>
+        <v>0</v>
+      </c>
+      <c r="H39" s="32"/>
+      <c r="I39" s="32"/>
+      <c r="J39" s="33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="3:10">
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="48"/>
+      <c r="G40" s="48"/>
+      <c r="H40" s="23"/>
+      <c r="I40" s="23"/>
+      <c r="J40" s="8"/>
+    </row>
+    <row r="41" spans="3:10" ht="15">
+      <c r="C41" s="8"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="48"/>
+      <c r="G41" s="58"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
+    </row>
+    <row r="42" spans="3:10" ht="15">
+      <c r="C42" s="8"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="48"/>
+      <c r="G42" s="49">
+        <f>G8-G12-G32</f>
+        <v>-30264000</v>
+      </c>
+      <c r="H42" s="12"/>
+      <c r="I42" s="20"/>
+      <c r="J42" s="31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="D33:G33"/>
+    <mergeCell ref="D5:G5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F413B64-656B-492A-8F7D-8434699F234E}">
+  <dimension ref="C2:J32"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="5"/>
+    <col min="3" max="3" width="8.42578125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="37.85546875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="24" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="52" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.42578125" style="52" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="25" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" style="25" customWidth="1"/>
+    <col min="10" max="10" width="33.5703125" style="5" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:10" ht="20.25">
+      <c r="C2" s="93" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="93"/>
+    </row>
+    <row r="3" spans="3:10" ht="15.75">
+      <c r="C3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="3:10" ht="15.75" customHeight="1">
+      <c r="C4" s="7"/>
+      <c r="D4" s="97" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="97"/>
+      <c r="F4" s="97"/>
+      <c r="G4" s="97"/>
       <c r="H4" s="54"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
@@ -4231,12 +5038,12 @@
     </row>
     <row r="9" spans="3:10" ht="15">
       <c r="C9" s="8"/>
-      <c r="D9" s="85" t="s">
+      <c r="D9" s="97" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="85"/>
-      <c r="F9" s="85"/>
-      <c r="G9" s="85"/>
+      <c r="E9" s="97"/>
+      <c r="F9" s="97"/>
+      <c r="G9" s="97"/>
       <c r="H9" s="54"/>
       <c r="I9" s="14"/>
       <c r="J9" s="15"/>
@@ -4398,11 +5205,22 @@
     </row>
     <row r="17" spans="3:10" ht="15">
       <c r="C17" s="8"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="30"/>
+      <c r="D17" s="30" t="s">
+        <v>186</v>
+      </c>
+      <c r="E17" s="38">
+        <v>1</v>
+      </c>
+      <c r="F17" s="29">
+        <v>5000000</v>
+      </c>
+      <c r="G17" s="29">
+        <f>F17*E17</f>
+        <v>5000000</v>
+      </c>
+      <c r="H17" s="30" t="s">
+        <v>51</v>
+      </c>
       <c r="I17" s="11"/>
       <c r="J17" s="9"/>
     </row>
@@ -4433,12 +5251,12 @@
     </row>
     <row r="20" spans="3:10" ht="15">
       <c r="C20" s="8"/>
-      <c r="D20" s="85" t="s">
+      <c r="D20" s="97" t="s">
         <v>30</v>
       </c>
-      <c r="E20" s="85"/>
-      <c r="F20" s="85"/>
-      <c r="G20" s="85"/>
+      <c r="E20" s="97"/>
+      <c r="F20" s="97"/>
+      <c r="G20" s="97"/>
       <c r="H20" s="54"/>
       <c r="I20" s="11"/>
       <c r="J20" s="9"/>
@@ -4470,12 +5288,12 @@
     </row>
     <row r="23" spans="3:10" ht="15">
       <c r="C23" s="8"/>
-      <c r="D23" s="85" t="s">
+      <c r="D23" s="97" t="s">
         <v>27</v>
       </c>
-      <c r="E23" s="85"/>
-      <c r="F23" s="85"/>
-      <c r="G23" s="85"/>
+      <c r="E23" s="97"/>
+      <c r="F23" s="97"/>
+      <c r="G23" s="97"/>
       <c r="H23" s="57"/>
       <c r="I23" s="11"/>
       <c r="J23" s="8"/>
@@ -4617,7 +5435,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F130950-C7C5-472A-9BC1-443D40499FE8}">
   <dimension ref="C2:J32"/>
   <sheetViews>
@@ -4640,16 +5458,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:10" ht="20.25">
-      <c r="C2" s="81" t="s">
+      <c r="C2" s="93" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="93"/>
     </row>
     <row r="3" spans="3:10" ht="15.75">
       <c r="C3" s="6" t="s">
@@ -4679,12 +5497,12 @@
     </row>
     <row r="4" spans="3:10" ht="15.75" customHeight="1">
       <c r="C4" s="7"/>
-      <c r="D4" s="85" t="s">
+      <c r="D4" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="85"/>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
+      <c r="E4" s="97"/>
+      <c r="F4" s="97"/>
+      <c r="G4" s="97"/>
       <c r="H4" s="54"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
@@ -4742,12 +5560,12 @@
     </row>
     <row r="9" spans="3:10" ht="15">
       <c r="C9" s="8"/>
-      <c r="D9" s="85" t="s">
+      <c r="D9" s="97" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="85"/>
-      <c r="F9" s="85"/>
-      <c r="G9" s="85"/>
+      <c r="E9" s="97"/>
+      <c r="F9" s="97"/>
+      <c r="G9" s="97"/>
       <c r="H9" s="54"/>
       <c r="I9" s="14"/>
       <c r="J9" s="15"/>
@@ -4919,12 +5737,12 @@
     </row>
     <row r="20" spans="3:10" ht="15">
       <c r="C20" s="8"/>
-      <c r="D20" s="85" t="s">
+      <c r="D20" s="97" t="s">
         <v>30</v>
       </c>
-      <c r="E20" s="85"/>
-      <c r="F20" s="85"/>
-      <c r="G20" s="85"/>
+      <c r="E20" s="97"/>
+      <c r="F20" s="97"/>
+      <c r="G20" s="97"/>
       <c r="H20" s="54"/>
       <c r="I20" s="11"/>
       <c r="J20" s="9"/>
@@ -4956,12 +5774,12 @@
     </row>
     <row r="23" spans="3:10" ht="15">
       <c r="C23" s="8"/>
-      <c r="D23" s="85" t="s">
+      <c r="D23" s="97" t="s">
         <v>27</v>
       </c>
-      <c r="E23" s="85"/>
-      <c r="F23" s="85"/>
-      <c r="G23" s="85"/>
+      <c r="E23" s="97"/>
+      <c r="F23" s="97"/>
+      <c r="G23" s="97"/>
       <c r="H23" s="57"/>
       <c r="I23" s="11"/>
       <c r="J23" s="8"/>
@@ -5095,12 +5913,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73990C79-75DF-434D-B272-2581D279AD79}">
-  <dimension ref="C2:J75"/>
+  <dimension ref="C2:J77"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H65" sqref="H65"/>
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J51" sqref="J51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -5118,16 +5936,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:10" ht="20.25">
-      <c r="C2" s="81" t="s">
+      <c r="C2" s="93" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="93"/>
     </row>
     <row r="3" spans="3:10" ht="15.75">
       <c r="C3" s="6" t="s">
@@ -5157,12 +5975,12 @@
     </row>
     <row r="4" spans="3:10" ht="15.75" customHeight="1">
       <c r="C4" s="7"/>
-      <c r="D4" s="85" t="s">
+      <c r="D4" s="97" t="s">
         <v>83</v>
       </c>
-      <c r="E4" s="85"/>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
+      <c r="E4" s="97"/>
+      <c r="F4" s="97"/>
+      <c r="G4" s="97"/>
       <c r="H4" s="60"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
@@ -5220,12 +6038,12 @@
     </row>
     <row r="9" spans="3:10" ht="15">
       <c r="C9" s="8"/>
-      <c r="D9" s="85" t="s">
+      <c r="D9" s="97" t="s">
         <v>76</v>
       </c>
-      <c r="E9" s="85"/>
-      <c r="F9" s="85"/>
-      <c r="G9" s="85"/>
+      <c r="E9" s="97"/>
+      <c r="F9" s="97"/>
+      <c r="G9" s="97"/>
       <c r="H9" s="60"/>
       <c r="I9" s="14"/>
       <c r="J9" s="15"/>
@@ -5426,12 +6244,12 @@
     </row>
     <row r="20" spans="3:10" ht="15">
       <c r="C20" s="8"/>
-      <c r="D20" s="85" t="s">
+      <c r="D20" s="97" t="s">
         <v>84</v>
       </c>
-      <c r="E20" s="85"/>
-      <c r="F20" s="85"/>
-      <c r="G20" s="85"/>
+      <c r="E20" s="97"/>
+      <c r="F20" s="97"/>
+      <c r="G20" s="97"/>
       <c r="H20" s="60"/>
       <c r="I20" s="11"/>
       <c r="J20" s="9"/>
@@ -5473,7 +6291,7 @@
         <v>120000</v>
       </c>
       <c r="G22" s="29">
-        <f t="shared" ref="G22:G48" si="1">E22*F22</f>
+        <f t="shared" ref="G22:G50" si="1">E22*F22</f>
         <v>120000</v>
       </c>
       <c r="H22" s="30" t="s">
@@ -6070,305 +6888,305 @@
     </row>
     <row r="49" spans="3:10" ht="15">
       <c r="C49" s="8"/>
-      <c r="D49" s="30"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="29"/>
-      <c r="G49" s="29"/>
-      <c r="H49" s="9"/>
+      <c r="D49" s="30" t="s">
+        <v>183</v>
+      </c>
+      <c r="E49" s="3">
+        <v>1</v>
+      </c>
+      <c r="F49" s="29">
+        <v>250000</v>
+      </c>
+      <c r="G49" s="29">
+        <f t="shared" si="1"/>
+        <v>250000</v>
+      </c>
+      <c r="H49" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="I49" s="8"/>
       <c r="J49" s="8"/>
     </row>
     <row r="50" spans="3:10" ht="15">
       <c r="C50" s="8"/>
-      <c r="D50" s="30"/>
-      <c r="E50" s="38"/>
-      <c r="F50" s="29"/>
-      <c r="G50" s="55">
-        <f>SUM(G21:G49)</f>
-        <v>4098000</v>
-      </c>
-      <c r="H50" s="56"/>
-      <c r="I50" s="35"/>
-      <c r="J50" s="33" t="s">
-        <v>7</v>
-      </c>
+      <c r="D50" s="30" t="s">
+        <v>184</v>
+      </c>
+      <c r="E50" s="3">
+        <v>1</v>
+      </c>
+      <c r="F50" s="29">
+        <v>80000</v>
+      </c>
+      <c r="G50" s="29">
+        <f t="shared" si="1"/>
+        <v>80000</v>
+      </c>
+      <c r="H50" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I50" s="8"/>
+      <c r="J50" s="8"/>
     </row>
     <row r="51" spans="3:10" ht="15">
       <c r="C51" s="8"/>
-      <c r="D51" s="85" t="s">
+      <c r="D51" s="30"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="29"/>
+      <c r="G51" s="29"/>
+      <c r="H51" s="9"/>
+      <c r="I51" s="8"/>
+      <c r="J51" s="8"/>
+    </row>
+    <row r="52" spans="3:10" ht="15">
+      <c r="C52" s="8"/>
+      <c r="D52" s="30"/>
+      <c r="E52" s="38"/>
+      <c r="F52" s="29"/>
+      <c r="G52" s="55">
+        <f>SUM(G21:G50)</f>
+        <v>4428000</v>
+      </c>
+      <c r="H52" s="56"/>
+      <c r="I52" s="35"/>
+      <c r="J52" s="33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="3:10" ht="15">
+      <c r="C53" s="8"/>
+      <c r="D53" s="97" t="s">
         <v>106</v>
       </c>
-      <c r="E51" s="85"/>
-      <c r="F51" s="85"/>
-      <c r="G51" s="85"/>
-      <c r="H51" s="57"/>
-      <c r="I51" s="11"/>
-      <c r="J51" s="8"/>
-    </row>
-    <row r="52" spans="3:10" ht="15">
-      <c r="C52" s="8">
-        <v>1</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E52" s="3">
-        <v>1</v>
-      </c>
-      <c r="F52" s="39">
-        <v>1800000</v>
-      </c>
-      <c r="G52" s="59">
-        <f>F52*E52</f>
-        <v>1800000</v>
-      </c>
-      <c r="H52" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="I52" s="14"/>
-      <c r="J52" s="34"/>
-    </row>
-    <row r="53" spans="3:10" ht="15">
-      <c r="C53" s="8">
-        <v>2</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E53" s="3">
-        <v>1</v>
-      </c>
-      <c r="F53" s="39">
-        <v>5000000</v>
-      </c>
-      <c r="G53" s="59">
-        <f>F53*E53</f>
-        <v>5000000</v>
-      </c>
-      <c r="H53" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="I53" s="14"/>
-      <c r="J53" s="22"/>
+      <c r="E53" s="97"/>
+      <c r="F53" s="97"/>
+      <c r="G53" s="97"/>
+      <c r="H53" s="57"/>
+      <c r="I53" s="11"/>
+      <c r="J53" s="8"/>
     </row>
     <row r="54" spans="3:10" ht="15">
       <c r="C54" s="8">
-        <v>3</v>
-      </c>
-      <c r="D54" s="30" t="s">
-        <v>109</v>
-      </c>
-      <c r="E54" s="30">
-        <v>1</v>
-      </c>
-      <c r="F54" s="29">
-        <v>2590000</v>
+        <v>1</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E54" s="3">
+        <v>1</v>
+      </c>
+      <c r="F54" s="39">
+        <v>1800000</v>
       </c>
       <c r="G54" s="59">
         <f>F54*E54</f>
-        <v>2590000</v>
+        <v>1800000</v>
       </c>
       <c r="H54" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="I54" s="11"/>
-      <c r="J54" s="22"/>
+        <v>22</v>
+      </c>
+      <c r="I54" s="14"/>
+      <c r="J54" s="34"/>
     </row>
     <row r="55" spans="3:10" ht="15">
-      <c r="C55" s="8"/>
-      <c r="D55" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="E55" s="10">
-        <v>1</v>
-      </c>
-      <c r="F55" s="48">
-        <v>410000</v>
+      <c r="C55" s="8">
+        <v>2</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E55" s="3">
+        <v>1</v>
+      </c>
+      <c r="F55" s="39">
+        <v>5000000</v>
       </c>
       <c r="G55" s="59">
         <f>F55*E55</f>
-        <v>410000</v>
-      </c>
-      <c r="H55" s="14" t="s">
+        <v>5000000</v>
+      </c>
+      <c r="H55" s="30" t="s">
         <v>22</v>
       </c>
       <c r="I55" s="14"/>
       <c r="J55" s="22"/>
     </row>
     <row r="56" spans="3:10" ht="15">
-      <c r="C56" s="8"/>
-      <c r="D56" s="21"/>
-      <c r="E56" s="10"/>
-      <c r="F56" s="48"/>
-      <c r="G56" s="50"/>
-      <c r="H56" s="14"/>
-      <c r="I56" s="14"/>
+      <c r="C56" s="8">
+        <v>3</v>
+      </c>
+      <c r="D56" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="E56" s="30">
+        <v>1</v>
+      </c>
+      <c r="F56" s="29">
+        <v>2590000</v>
+      </c>
+      <c r="G56" s="59">
+        <f>F56*E56</f>
+        <v>2590000</v>
+      </c>
+      <c r="H56" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="I56" s="11"/>
       <c r="J56" s="22"/>
     </row>
     <row r="57" spans="3:10" ht="15">
       <c r="C57" s="8"/>
-      <c r="D57" s="36"/>
-      <c r="E57" s="37"/>
-      <c r="F57" s="53"/>
-      <c r="G57" s="51">
-        <f>SUM(G52:G55)</f>
-        <v>9800000</v>
-      </c>
-      <c r="H57" s="32"/>
-      <c r="I57" s="32"/>
-      <c r="J57" s="33" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="58" spans="3:10">
+      <c r="D57" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="E57" s="10">
+        <v>1</v>
+      </c>
+      <c r="F57" s="48">
+        <v>410000</v>
+      </c>
+      <c r="G57" s="59">
+        <f>F57*E57</f>
+        <v>410000</v>
+      </c>
+      <c r="H57" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I57" s="14"/>
+      <c r="J57" s="22"/>
+    </row>
+    <row r="58" spans="3:10" ht="15">
       <c r="C58" s="8"/>
-      <c r="D58" s="8"/>
+      <c r="D58" s="21"/>
       <c r="E58" s="10"/>
       <c r="F58" s="48"/>
-      <c r="G58" s="48"/>
-      <c r="H58" s="23"/>
-      <c r="I58" s="23"/>
-      <c r="J58" s="8"/>
+      <c r="G58" s="50"/>
+      <c r="H58" s="14"/>
+      <c r="I58" s="14"/>
+      <c r="J58" s="22"/>
     </row>
     <row r="59" spans="3:10" ht="15">
       <c r="C59" s="8"/>
-      <c r="D59" s="85" t="s">
+      <c r="D59" s="36"/>
+      <c r="E59" s="37"/>
+      <c r="F59" s="53"/>
+      <c r="G59" s="51">
+        <f>SUM(G54:G57)</f>
+        <v>9800000</v>
+      </c>
+      <c r="H59" s="32"/>
+      <c r="I59" s="32"/>
+      <c r="J59" s="33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="3:10">
+      <c r="C60" s="8"/>
+      <c r="D60" s="8"/>
+      <c r="E60" s="10"/>
+      <c r="F60" s="48"/>
+      <c r="G60" s="48"/>
+      <c r="H60" s="23"/>
+      <c r="I60" s="23"/>
+      <c r="J60" s="8"/>
+    </row>
+    <row r="61" spans="3:10" ht="15">
+      <c r="C61" s="8"/>
+      <c r="D61" s="97" t="s">
         <v>110</v>
       </c>
-      <c r="E59" s="85"/>
-      <c r="F59" s="85"/>
-      <c r="G59" s="85"/>
-      <c r="H59" s="57"/>
-      <c r="I59" s="11"/>
-      <c r="J59" s="8"/>
-    </row>
-    <row r="60" spans="3:10" ht="15">
-      <c r="C60" s="8">
-        <v>1</v>
-      </c>
-      <c r="D60" s="30" t="s">
-        <v>111</v>
-      </c>
-      <c r="E60" s="3">
-        <v>1</v>
-      </c>
-      <c r="F60" s="29">
-        <v>2000000</v>
-      </c>
-      <c r="G60" s="59">
-        <f>F60*E60</f>
-        <v>2000000</v>
-      </c>
-      <c r="H60" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="I60" s="14"/>
-      <c r="J60" s="34"/>
-    </row>
-    <row r="61" spans="3:10" ht="15">
-      <c r="C61" s="8">
-        <v>2</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E61" s="3">
-        <v>1</v>
-      </c>
-      <c r="F61" s="39">
-        <v>250000</v>
-      </c>
-      <c r="G61" s="59">
-        <f t="shared" ref="G61:G65" si="2">F61*E61</f>
-        <v>250000</v>
-      </c>
-      <c r="H61" s="65" t="s">
-        <v>116</v>
-      </c>
-      <c r="I61" s="14"/>
-      <c r="J61" s="22"/>
+      <c r="E61" s="97"/>
+      <c r="F61" s="97"/>
+      <c r="G61" s="97"/>
+      <c r="H61" s="57"/>
+      <c r="I61" s="11"/>
+      <c r="J61" s="8"/>
     </row>
     <row r="62" spans="3:10" ht="15">
       <c r="C62" s="8">
+        <v>1</v>
+      </c>
+      <c r="D62" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="E62" s="3">
+        <v>1</v>
+      </c>
+      <c r="F62" s="29">
+        <v>2000000</v>
+      </c>
+      <c r="G62" s="59">
+        <f>F62*E62</f>
+        <v>2000000</v>
+      </c>
+      <c r="H62" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="I62" s="14"/>
+      <c r="J62" s="34"/>
+    </row>
+    <row r="63" spans="3:10" ht="15">
+      <c r="C63" s="8">
+        <v>2</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E63" s="3">
+        <v>1</v>
+      </c>
+      <c r="F63" s="39">
+        <v>250000</v>
+      </c>
+      <c r="G63" s="59">
+        <f t="shared" ref="G63:G67" si="2">F63*E63</f>
+        <v>250000</v>
+      </c>
+      <c r="H63" s="65" t="s">
+        <v>116</v>
+      </c>
+      <c r="I63" s="14"/>
+      <c r="J63" s="22"/>
+    </row>
+    <row r="64" spans="3:10" ht="15">
+      <c r="C64" s="8">
         <v>3</v>
       </c>
-      <c r="D62" s="1" t="s">
+      <c r="D64" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="E62" s="30">
-        <v>1</v>
-      </c>
-      <c r="F62" s="39">
+      <c r="E64" s="30">
+        <v>1</v>
+      </c>
+      <c r="F64" s="39">
         <v>1000000</v>
       </c>
-      <c r="G62" s="59">
+      <c r="G64" s="59">
         <f t="shared" si="2"/>
         <v>1000000</v>
       </c>
-      <c r="H62" s="65" t="s">
-        <v>116</v>
-      </c>
-      <c r="I62" s="11"/>
-      <c r="J62" s="22"/>
-    </row>
-    <row r="63" spans="3:10" ht="15">
-      <c r="C63" s="8"/>
-      <c r="D63" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E63" s="30">
-        <v>1</v>
-      </c>
-      <c r="F63" s="39">
-        <v>1880000</v>
-      </c>
-      <c r="G63" s="59">
-        <f t="shared" si="2"/>
-        <v>1880000</v>
-      </c>
-      <c r="H63" s="65" t="s">
-        <v>116</v>
-      </c>
-      <c r="I63" s="14"/>
-      <c r="J63" s="22"/>
-    </row>
-    <row r="64" spans="3:10" ht="15">
-      <c r="C64" s="8"/>
-      <c r="D64" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E64" s="30">
-        <v>1</v>
-      </c>
-      <c r="F64" s="39">
-        <v>1200000</v>
-      </c>
-      <c r="G64" s="59">
-        <f t="shared" si="2"/>
-        <v>1200000</v>
-      </c>
       <c r="H64" s="65" t="s">
         <v>116</v>
       </c>
-      <c r="I64" s="14"/>
+      <c r="I64" s="11"/>
       <c r="J64" s="22"/>
     </row>
     <row r="65" spans="3:10" ht="15">
       <c r="C65" s="8"/>
       <c r="D65" s="1" t="s">
-        <v>171</v>
+        <v>114</v>
       </c>
       <c r="E65" s="30">
         <v>1</v>
       </c>
       <c r="F65" s="39">
-        <v>326700</v>
+        <v>1880000</v>
       </c>
       <c r="G65" s="59">
         <f t="shared" si="2"/>
-        <v>326700</v>
-      </c>
-      <c r="H65" s="14" t="s">
+        <v>1880000</v>
+      </c>
+      <c r="H65" s="65" t="s">
         <v>116</v>
       </c>
       <c r="I65" s="14"/>
@@ -6376,703 +7194,183 @@
     </row>
     <row r="66" spans="3:10" ht="15">
       <c r="C66" s="8"/>
-      <c r="D66" s="1"/>
-      <c r="E66" s="30"/>
-      <c r="F66" s="39"/>
-      <c r="G66" s="59"/>
-      <c r="H66" s="14"/>
+      <c r="D66" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E66" s="30">
+        <v>1</v>
+      </c>
+      <c r="F66" s="39">
+        <v>1200000</v>
+      </c>
+      <c r="G66" s="59">
+        <f t="shared" si="2"/>
+        <v>1200000</v>
+      </c>
+      <c r="H66" s="65" t="s">
+        <v>116</v>
+      </c>
       <c r="I66" s="14"/>
       <c r="J66" s="22"/>
     </row>
     <row r="67" spans="3:10" ht="15">
       <c r="C67" s="8"/>
-      <c r="D67" s="36"/>
-      <c r="E67" s="37"/>
-      <c r="F67" s="53"/>
-      <c r="G67" s="51">
-        <f>SUM(G60:G65)</f>
-        <v>6656700</v>
-      </c>
-      <c r="H67" s="32"/>
-      <c r="I67" s="32"/>
-      <c r="J67" s="33" t="s">
-        <v>7</v>
-      </c>
+      <c r="D67" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E67" s="30">
+        <v>1</v>
+      </c>
+      <c r="F67" s="39">
+        <v>326700</v>
+      </c>
+      <c r="G67" s="59">
+        <f t="shared" si="2"/>
+        <v>326700</v>
+      </c>
+      <c r="H67" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="I67" s="14"/>
+      <c r="J67" s="22"/>
     </row>
     <row r="68" spans="3:10" ht="15">
       <c r="C68" s="8"/>
-      <c r="D68" s="36"/>
-      <c r="E68" s="37"/>
-      <c r="F68" s="53"/>
-      <c r="G68" s="66"/>
-      <c r="H68" s="67"/>
-      <c r="I68" s="67"/>
-      <c r="J68" s="68"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="30"/>
+      <c r="F68" s="39"/>
+      <c r="G68" s="59"/>
+      <c r="H68" s="14"/>
+      <c r="I68" s="14"/>
+      <c r="J68" s="22"/>
     </row>
     <row r="69" spans="3:10" ht="15">
       <c r="C69" s="8"/>
-      <c r="D69" s="85" t="s">
-        <v>117</v>
-      </c>
-      <c r="E69" s="85"/>
-      <c r="F69" s="85"/>
-      <c r="G69" s="85"/>
-      <c r="H69" s="57"/>
-      <c r="I69" s="11"/>
-      <c r="J69" s="8"/>
+      <c r="D69" s="36"/>
+      <c r="E69" s="37"/>
+      <c r="F69" s="53"/>
+      <c r="G69" s="51">
+        <f>SUM(G62:G67)</f>
+        <v>6656700</v>
+      </c>
+      <c r="H69" s="32"/>
+      <c r="I69" s="32"/>
+      <c r="J69" s="33" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="70" spans="3:10" ht="15">
       <c r="C70" s="8"/>
-      <c r="D70" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="E70" s="3">
-        <v>1</v>
-      </c>
-      <c r="F70" s="29">
-        <v>7174000</v>
-      </c>
-      <c r="G70" s="59">
-        <f>F70*E70</f>
-        <v>7174000</v>
-      </c>
-      <c r="H70" s="64" t="s">
-        <v>22</v>
-      </c>
-      <c r="I70" s="14"/>
-      <c r="J70" s="34"/>
+      <c r="D70" s="36"/>
+      <c r="E70" s="37"/>
+      <c r="F70" s="53"/>
+      <c r="G70" s="66"/>
+      <c r="H70" s="67"/>
+      <c r="I70" s="67"/>
+      <c r="J70" s="68"/>
     </row>
     <row r="71" spans="3:10" ht="15">
       <c r="C71" s="8"/>
-      <c r="D71" s="2"/>
-      <c r="E71" s="3"/>
-      <c r="F71" s="39"/>
-      <c r="G71" s="59"/>
-      <c r="H71" s="65"/>
-      <c r="I71" s="14"/>
-      <c r="J71" s="22"/>
+      <c r="D71" s="97" t="s">
+        <v>117</v>
+      </c>
+      <c r="E71" s="97"/>
+      <c r="F71" s="97"/>
+      <c r="G71" s="97"/>
+      <c r="H71" s="57"/>
+      <c r="I71" s="11"/>
+      <c r="J71" s="8"/>
     </row>
     <row r="72" spans="3:10" ht="15">
       <c r="C72" s="8"/>
-      <c r="D72" s="1"/>
-      <c r="E72" s="30"/>
-      <c r="F72" s="39"/>
-      <c r="G72" s="59"/>
-      <c r="H72" s="14"/>
+      <c r="D72" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="E72" s="3">
+        <v>1</v>
+      </c>
+      <c r="F72" s="29">
+        <v>7174000</v>
+      </c>
+      <c r="G72" s="59">
+        <f>F72*E72</f>
+        <v>7174000</v>
+      </c>
+      <c r="H72" s="64" t="s">
+        <v>22</v>
+      </c>
       <c r="I72" s="14"/>
-      <c r="J72" s="22"/>
+      <c r="J72" s="34"/>
     </row>
     <row r="73" spans="3:10" ht="15">
       <c r="C73" s="8"/>
-      <c r="D73" s="36"/>
-      <c r="E73" s="37"/>
-      <c r="F73" s="53"/>
-      <c r="G73" s="51">
-        <f>SUM(G70:G71)</f>
-        <v>7174000</v>
-      </c>
-      <c r="H73" s="32"/>
-      <c r="I73" s="32"/>
-      <c r="J73" s="33" t="s">
-        <v>7</v>
-      </c>
+      <c r="D73" s="2"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="39"/>
+      <c r="G73" s="59"/>
+      <c r="H73" s="65"/>
+      <c r="I73" s="14"/>
+      <c r="J73" s="22"/>
     </row>
     <row r="74" spans="3:10" ht="15">
       <c r="C74" s="8"/>
-      <c r="D74" s="21"/>
-      <c r="E74" s="10"/>
-      <c r="F74" s="48"/>
-      <c r="G74" s="58"/>
-      <c r="H74" s="8"/>
-      <c r="I74" s="8"/>
-      <c r="J74" s="8"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="30"/>
+      <c r="F74" s="39"/>
+      <c r="G74" s="59"/>
+      <c r="H74" s="14"/>
+      <c r="I74" s="14"/>
+      <c r="J74" s="22"/>
     </row>
     <row r="75" spans="3:10" ht="15">
       <c r="C75" s="8"/>
-      <c r="D75" s="21"/>
-      <c r="E75" s="10"/>
-      <c r="F75" s="48"/>
-      <c r="G75" s="49">
-        <f>G8-G19-G50-G57-G67-G73</f>
-        <v>-31728700</v>
-      </c>
-      <c r="H75" s="12"/>
-      <c r="I75" s="20"/>
-      <c r="J75" s="31" t="s">
+      <c r="D75" s="36"/>
+      <c r="E75" s="37"/>
+      <c r="F75" s="53"/>
+      <c r="G75" s="51">
+        <f>SUM(G72:G73)</f>
+        <v>7174000</v>
+      </c>
+      <c r="H75" s="32"/>
+      <c r="I75" s="32"/>
+      <c r="J75" s="33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76" spans="3:10" ht="15">
+      <c r="C76" s="8"/>
+      <c r="D76" s="21"/>
+      <c r="E76" s="10"/>
+      <c r="F76" s="48"/>
+      <c r="G76" s="58"/>
+      <c r="H76" s="8"/>
+      <c r="I76" s="8"/>
+      <c r="J76" s="8"/>
+    </row>
+    <row r="77" spans="3:10" ht="15">
+      <c r="C77" s="8"/>
+      <c r="D77" s="21"/>
+      <c r="E77" s="10"/>
+      <c r="F77" s="48"/>
+      <c r="G77" s="49">
+        <f>G8-G19-G52-G59-G69-G75</f>
+        <v>-32058700</v>
+      </c>
+      <c r="H77" s="12"/>
+      <c r="I77" s="20"/>
+      <c r="J77" s="31" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="D59:G59"/>
-    <mergeCell ref="D69:G69"/>
+    <mergeCell ref="D61:G61"/>
+    <mergeCell ref="D71:G71"/>
     <mergeCell ref="C2:J2"/>
     <mergeCell ref="D4:G4"/>
     <mergeCell ref="D9:G9"/>
     <mergeCell ref="D20:G20"/>
-    <mergeCell ref="D51:G51"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A00FBF6-6528-4077-97A8-E7F8FA86DD30}">
-  <dimension ref="C2:J42"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <cols>
-    <col min="1" max="2" width="9.140625" style="5"/>
-    <col min="3" max="3" width="8.42578125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="37.85546875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="24" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" style="52" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.42578125" style="52" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="25" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" style="25" customWidth="1"/>
-    <col min="10" max="10" width="33.5703125" style="5" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="5"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="3:10" ht="20.25">
-      <c r="C2" s="81" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-    </row>
-    <row r="3" spans="3:10" ht="15.75">
-      <c r="C3" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="47" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="47" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="3:10" ht="15.75" customHeight="1">
-      <c r="C4" s="7"/>
-      <c r="D4" s="85" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="85"/>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-    </row>
-    <row r="5" spans="3:10" ht="20.25">
-      <c r="C5" s="7"/>
-      <c r="D5" s="85" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="80"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-    </row>
-    <row r="6" spans="3:10">
-      <c r="C6" s="8">
-        <v>1</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="10">
-        <v>1</v>
-      </c>
-      <c r="F6" s="48">
-        <v>29294650.400000002</v>
-      </c>
-      <c r="G6" s="48">
-        <f>F6*E6</f>
-        <v>29294650.400000002</v>
-      </c>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="8"/>
-    </row>
-    <row r="7" spans="3:10">
-      <c r="C7" s="8">
-        <v>2</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="E7" s="10">
-        <v>1</v>
-      </c>
-      <c r="F7" s="48"/>
-      <c r="G7" s="48">
-        <f>F7*E7</f>
-        <v>0</v>
-      </c>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="9"/>
-    </row>
-    <row r="8" spans="3:10">
-      <c r="C8" s="8">
-        <v>3</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="E8" s="10">
-        <v>1</v>
-      </c>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48">
-        <f>F8*E8</f>
-        <v>0</v>
-      </c>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="9"/>
-    </row>
-    <row r="9" spans="3:10" ht="15">
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="49">
-        <f>SUM(G6:G8)</f>
-        <v>29294650.400000002</v>
-      </c>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="3:10" ht="15">
-      <c r="C10" s="8"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="9"/>
-    </row>
-    <row r="11" spans="3:10" ht="15">
-      <c r="C11" s="8"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="9"/>
-    </row>
-    <row r="12" spans="3:10" ht="15">
-      <c r="C12" s="8"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="55">
-        <f>SUM(G10:G10)</f>
-        <v>0</v>
-      </c>
-      <c r="H12" s="56"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="33" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="3:10" ht="15">
-      <c r="C13" s="8"/>
-      <c r="D13" s="85" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="85"/>
-      <c r="F13" s="85"/>
-      <c r="G13" s="85"/>
-      <c r="H13" s="74"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="9"/>
-    </row>
-    <row r="14" spans="3:10" ht="15">
-      <c r="C14" s="8"/>
-      <c r="D14" s="30" t="s">
-        <v>138</v>
-      </c>
-      <c r="E14" s="38">
-        <v>1</v>
-      </c>
-      <c r="F14" s="29">
-        <v>9064000</v>
-      </c>
-      <c r="G14" s="29">
-        <f>F14*E14</f>
-        <v>9064000</v>
-      </c>
-      <c r="H14" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="I14" s="11"/>
-      <c r="J14" s="9"/>
-    </row>
-    <row r="15" spans="3:10" ht="15">
-      <c r="C15" s="8"/>
-      <c r="D15" s="30" t="s">
-        <v>147</v>
-      </c>
-      <c r="E15" s="38">
-        <v>1</v>
-      </c>
-      <c r="F15" s="29">
-        <v>200000</v>
-      </c>
-      <c r="G15" s="29">
-        <f>F15*E15</f>
-        <v>200000</v>
-      </c>
-      <c r="H15" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="I15" s="11"/>
-      <c r="J15" s="9"/>
-    </row>
-    <row r="16" spans="3:10" ht="15">
-      <c r="C16" s="8"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="9"/>
-    </row>
-    <row r="17" spans="3:10" ht="15">
-      <c r="C17" s="8"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="9"/>
-    </row>
-    <row r="18" spans="3:10" ht="15">
-      <c r="C18" s="8"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="9"/>
-    </row>
-    <row r="19" spans="3:10" ht="15">
-      <c r="C19" s="8"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="30"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="9"/>
-    </row>
-    <row r="20" spans="3:10" s="46" customFormat="1" ht="15">
-      <c r="C20" s="8"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="44"/>
-      <c r="G20" s="44"/>
-      <c r="H20" s="45"/>
-      <c r="I20" s="41"/>
-      <c r="J20" s="41"/>
-    </row>
-    <row r="21" spans="3:10" ht="15">
-      <c r="C21" s="8"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="38"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="30"/>
-      <c r="J21" s="15"/>
-    </row>
-    <row r="22" spans="3:10" ht="15">
-      <c r="C22" s="8"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="29"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="9"/>
-    </row>
-    <row r="23" spans="3:10" ht="15">
-      <c r="C23" s="8"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="38"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="29"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="9"/>
-    </row>
-    <row r="24" spans="3:10" ht="15">
-      <c r="C24" s="8"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="29"/>
-      <c r="G24" s="29"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="9"/>
-    </row>
-    <row r="25" spans="3:10" ht="15">
-      <c r="C25" s="8"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="30"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="9"/>
-    </row>
-    <row r="26" spans="3:10" ht="15">
-      <c r="C26" s="8"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="38"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="29"/>
-      <c r="H26" s="30"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="9"/>
-    </row>
-    <row r="27" spans="3:10" ht="15">
-      <c r="C27" s="8"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="30"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="9"/>
-    </row>
-    <row r="28" spans="3:10" ht="15">
-      <c r="C28" s="8"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="30"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="9"/>
-    </row>
-    <row r="29" spans="3:10" ht="15">
-      <c r="C29" s="8"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="9"/>
-    </row>
-    <row r="30" spans="3:10" ht="15">
-      <c r="C30" s="8"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="29"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="9"/>
-    </row>
-    <row r="31" spans="3:10" ht="15">
-      <c r="C31" s="8"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="38"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="29"/>
-      <c r="H31" s="30"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="75"/>
-    </row>
-    <row r="32" spans="3:10" ht="15">
-      <c r="C32" s="8"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="38"/>
-      <c r="F32" s="29"/>
-      <c r="G32" s="55">
-        <f>SUM(G14:G31)</f>
-        <v>9264000</v>
-      </c>
-      <c r="H32" s="56"/>
-      <c r="I32" s="35"/>
-      <c r="J32" s="33" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="3:10" ht="15">
-      <c r="C33" s="8"/>
-      <c r="D33" s="85" t="s">
-        <v>27</v>
-      </c>
-      <c r="E33" s="85"/>
-      <c r="F33" s="85"/>
-      <c r="G33" s="85"/>
-      <c r="H33" s="57"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="8"/>
-    </row>
-    <row r="34" spans="3:10" ht="15">
-      <c r="C34" s="8">
-        <v>1</v>
-      </c>
-      <c r="D34" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="E34" s="10"/>
-      <c r="F34" s="48"/>
-      <c r="G34" s="50"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="14"/>
-      <c r="J34" s="34"/>
-    </row>
-    <row r="35" spans="3:10" ht="15">
-      <c r="C35" s="8">
-        <v>2</v>
-      </c>
-      <c r="D35" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="E35" s="10"/>
-      <c r="F35" s="48"/>
-      <c r="G35" s="50"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
-      <c r="J35" s="22"/>
-    </row>
-    <row r="36" spans="3:10" ht="15">
-      <c r="C36" s="8">
-        <v>3</v>
-      </c>
-      <c r="D36" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="E36" s="10"/>
-      <c r="F36" s="48"/>
-      <c r="G36" s="50"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="22"/>
-    </row>
-    <row r="37" spans="3:10" ht="15">
-      <c r="C37" s="8">
-        <v>4</v>
-      </c>
-      <c r="D37" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="E37" s="10"/>
-      <c r="F37" s="48"/>
-      <c r="G37" s="50"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="22"/>
-    </row>
-    <row r="38" spans="3:10" ht="15">
-      <c r="C38" s="8"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="48"/>
-      <c r="G38" s="50"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="22"/>
-    </row>
-    <row r="39" spans="3:10" ht="15">
-      <c r="C39" s="8"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="37"/>
-      <c r="F39" s="53"/>
-      <c r="G39" s="51">
-        <f>SUM(G34:G38)</f>
-        <v>0</v>
-      </c>
-      <c r="H39" s="32"/>
-      <c r="I39" s="32"/>
-      <c r="J39" s="33" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="3:10">
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="48"/>
-      <c r="G40" s="48"/>
-      <c r="H40" s="23"/>
-      <c r="I40" s="23"/>
-      <c r="J40" s="8"/>
-    </row>
-    <row r="41" spans="3:10" ht="15">
-      <c r="C41" s="8"/>
-      <c r="D41" s="21"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="48"/>
-      <c r="G41" s="58"/>
-      <c r="H41" s="8"/>
-      <c r="I41" s="8"/>
-      <c r="J41" s="8"/>
-    </row>
-    <row r="42" spans="3:10" ht="15">
-      <c r="C42" s="8"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="48"/>
-      <c r="G42" s="49">
-        <f>G8-G12-G32</f>
-        <v>-9264000</v>
-      </c>
-      <c r="H42" s="12"/>
-      <c r="I42" s="20"/>
-      <c r="J42" s="31" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="D33:G33"/>
-    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="D53:G53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update ngày 27/06 mua linh kiện test mạch zeus
</commit_message>
<xml_diff>
--- a/Project/TongHopQuy2.xlsx
+++ b/Project/TongHopQuy2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ViTechSolution_LTD\04.Team_Log\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VitechSolutions\Team_Log\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC96687-77A3-4B3B-AF5D-90C825FCEA2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8356763D-34CB-434A-BDF2-19B3F6BA5324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tổng hợp quỹ công ty" sheetId="6" r:id="rId1"/>
@@ -29,7 +29,7 @@
   </externalReferences>
   <definedNames>
     <definedName name="chi_phi_cong_ty">'Chi Phí Công ty'!$G$80</definedName>
-    <definedName name="Pega">PEGA!$G$46</definedName>
+    <definedName name="Pega">PEGA!$G$48</definedName>
     <definedName name="RowTitleRegion1..C7" localSheetId="4">#REF!</definedName>
     <definedName name="RowTitleRegion1..C7" localSheetId="5">#REF!</definedName>
     <definedName name="RowTitleRegion1..C7" localSheetId="8">#REF!</definedName>
@@ -56,12 +56,12 @@
     <definedName name="RowTitleRegion3..G26">[1]Effort_08062020!#REF!</definedName>
     <definedName name="smarthome" localSheetId="8">'Chi Phí Công ty'!$G$80</definedName>
     <definedName name="smarthome">SMARTHOME!$G$32</definedName>
-    <definedName name="sport1_p1.5" localSheetId="4">'160_Zeus'!$G$43</definedName>
+    <definedName name="sport1_p1.5" localSheetId="4">'160_Zeus'!$G$47</definedName>
     <definedName name="sport1_p1.5" localSheetId="5">'270_Hecquyn'!$G$42</definedName>
     <definedName name="sport1_p1.5">SPORT1_P1.5!$G$59</definedName>
     <definedName name="sport1_p2">SPORT1_P2!$G$32</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="200">
   <si>
     <t>STT</t>
   </si>
@@ -648,13 +648,31 @@
     <t>Cọc 50% sản xuất</t>
   </si>
   <si>
-    <t>module giải mã I2S</t>
-  </si>
-  <si>
-    <t>Đặt DFPlayer mini</t>
-  </si>
-  <si>
     <t>Ăn trưa ngày 19/06</t>
+  </si>
+  <si>
+    <t>Ăn trưa ngày 26/06</t>
+  </si>
+  <si>
+    <t>mạch tiền khuếch đại NE5532</t>
+  </si>
+  <si>
+    <t>Mạch khuếch đại TDA2030</t>
+  </si>
+  <si>
+    <t>Mạch khuếch đại TPA3118</t>
+  </si>
+  <si>
+    <t>IC 3118</t>
+  </si>
+  <si>
+    <t>Tổng hợp chi phí dự án SPORT1_P1.5 160Zeus</t>
+  </si>
+  <si>
+    <t>Mua cáp màn hình + Header</t>
+  </si>
+  <si>
+    <t>Linh kiện hàn mạch NE5532 test</t>
   </si>
 </sst>
 </file>
@@ -1501,7 +1519,7 @@
       </c>
       <c r="J4" s="11">
         <f>chi_phi_cong_ty</f>
-        <v>-32138700</v>
+        <v>-32238700</v>
       </c>
       <c r="K4" s="8"/>
     </row>
@@ -1512,7 +1530,7 @@
       </c>
       <c r="J5" s="11">
         <f>Pega</f>
-        <v>-25505086</v>
+        <v>-25605086</v>
       </c>
       <c r="K5" s="9"/>
     </row>
@@ -1572,7 +1590,7 @@
       <c r="I12" s="9"/>
       <c r="J12" s="12">
         <f>SUM(J4:J11)</f>
-        <v>-71578766.400000006</v>
+        <v>-71778766.400000006</v>
       </c>
       <c r="K12" s="13" t="s">
         <v>7</v>
@@ -1710,10 +1728,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8032BD6C-08F6-46C4-8E07-045BAFBCF7A7}">
-  <dimension ref="C2:J46"/>
+  <dimension ref="C2:J48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2199,7 +2217,7 @@
         <v>2685000</v>
       </c>
       <c r="G25" s="11">
-        <f t="shared" ref="G25:G30" si="3">E25*F25</f>
+        <f t="shared" ref="G25:G31" si="3">E25*F25</f>
         <v>2685000</v>
       </c>
       <c r="H25" s="70" t="s">
@@ -2314,142 +2332,140 @@
       <c r="J30" s="9"/>
     </row>
     <row r="31" spans="3:10">
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
+      <c r="D31" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="E31" s="5">
+        <v>1</v>
+      </c>
+      <c r="F31" s="5">
+        <v>100000</v>
+      </c>
+      <c r="G31" s="78">
+        <f t="shared" si="3"/>
+        <v>100000</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="I31" s="11"/>
       <c r="J31" s="9"/>
     </row>
-    <row r="32" spans="3:10" ht="15">
-      <c r="C32" s="8"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="73"/>
-      <c r="G32" s="32">
-        <f>SUM(G10:G30)</f>
-        <v>39505086</v>
-      </c>
-      <c r="H32" s="32"/>
-      <c r="I32" s="35"/>
-      <c r="J32" s="33" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="3:10" ht="15">
-      <c r="C33" s="8"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="73"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
+    <row r="32" spans="3:10">
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="78"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="9"/>
+    </row>
+    <row r="33" spans="3:10">
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="78"/>
+      <c r="H33" s="5"/>
       <c r="I33" s="11"/>
       <c r="J33" s="9"/>
     </row>
     <row r="34" spans="3:10" ht="15">
       <c r="C34" s="8"/>
-      <c r="D34" s="94" t="s">
-        <v>12</v>
-      </c>
-      <c r="E34" s="95"/>
-      <c r="F34" s="95"/>
-      <c r="G34" s="96"/>
-      <c r="H34" s="26"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="9"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="73"/>
+      <c r="G34" s="32">
+        <f>SUM(G10:G31)</f>
+        <v>39605086</v>
+      </c>
+      <c r="H34" s="32"/>
+      <c r="I34" s="35"/>
+      <c r="J34" s="33" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="35" spans="3:10" ht="15">
-      <c r="C35" s="8">
-        <v>1</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E35" s="10"/>
-      <c r="F35" s="48"/>
-      <c r="G35" s="32">
-        <v>25000000</v>
-      </c>
-      <c r="H35" s="32"/>
-      <c r="I35" s="35"/>
-      <c r="J35" s="33" t="s">
-        <v>7</v>
-      </c>
+      <c r="C35" s="8"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="73"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="9"/>
     </row>
     <row r="36" spans="3:10" ht="15">
       <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="48"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="15"/>
+      <c r="D36" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="95"/>
+      <c r="F36" s="95"/>
+      <c r="G36" s="96"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="9"/>
     </row>
     <row r="37" spans="3:10" ht="15">
-      <c r="C37" s="8"/>
-      <c r="D37" s="94" t="s">
-        <v>27</v>
-      </c>
-      <c r="E37" s="95"/>
-      <c r="F37" s="95"/>
-      <c r="G37" s="96"/>
-      <c r="H37" s="27"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="8"/>
+      <c r="C37" s="8">
+        <v>1</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E37" s="10"/>
+      <c r="F37" s="48"/>
+      <c r="G37" s="32">
+        <v>25000000</v>
+      </c>
+      <c r="H37" s="32"/>
+      <c r="I37" s="35"/>
+      <c r="J37" s="33" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="38" spans="3:10" ht="15">
-      <c r="C38" s="8">
-        <v>1</v>
-      </c>
-      <c r="D38" s="21" t="s">
-        <v>11</v>
-      </c>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
       <c r="E38" s="10"/>
       <c r="F38" s="48"/>
-      <c r="G38" s="14">
-        <v>5000000</v>
-      </c>
+      <c r="G38" s="14"/>
       <c r="H38" s="14"/>
       <c r="I38" s="14"/>
-      <c r="J38" s="34"/>
+      <c r="J38" s="15"/>
     </row>
     <row r="39" spans="3:10" ht="15">
-      <c r="C39" s="8">
-        <v>2</v>
-      </c>
-      <c r="D39" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="10"/>
-      <c r="F39" s="48"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="14"/>
-      <c r="J39" s="22"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="94" t="s">
+        <v>27</v>
+      </c>
+      <c r="E39" s="95"/>
+      <c r="F39" s="95"/>
+      <c r="G39" s="96"/>
+      <c r="H39" s="27"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="8"/>
     </row>
     <row r="40" spans="3:10" ht="15">
       <c r="C40" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D40" s="21" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E40" s="10"/>
       <c r="F40" s="48"/>
       <c r="G40" s="14">
-        <v>25000000</v>
+        <v>5000000</v>
       </c>
       <c r="H40" s="14"/>
-      <c r="I40" s="11"/>
-      <c r="J40" s="22"/>
+      <c r="I40" s="14"/>
+      <c r="J40" s="34"/>
     </row>
     <row r="41" spans="3:10" ht="15">
       <c r="C41" s="8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D41" s="21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E41" s="10"/>
       <c r="F41" s="48"/>
@@ -2460,56 +2476,86 @@
     </row>
     <row r="42" spans="3:10" ht="15">
       <c r="C42" s="8">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D42" s="21" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="E42" s="10"/>
       <c r="F42" s="48"/>
       <c r="G42" s="14">
+        <v>25000000</v>
+      </c>
+      <c r="H42" s="14"/>
+      <c r="I42" s="11"/>
+      <c r="J42" s="22"/>
+    </row>
+    <row r="43" spans="3:10" ht="15">
+      <c r="C43" s="8">
+        <v>4</v>
+      </c>
+      <c r="D43" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43" s="10"/>
+      <c r="F43" s="48"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="22"/>
+    </row>
+    <row r="44" spans="3:10" ht="15">
+      <c r="C44" s="8">
+        <v>5</v>
+      </c>
+      <c r="D44" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E44" s="10"/>
+      <c r="F44" s="48"/>
+      <c r="G44" s="14">
         <v>10000000</v>
       </c>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="22"/>
-    </row>
-    <row r="43" spans="3:10" ht="15">
-      <c r="C43" s="8"/>
-      <c r="D43" s="36"/>
-      <c r="E43" s="37"/>
-      <c r="F43" s="53"/>
-      <c r="G43" s="32">
-        <f>SUM(G38:G42)</f>
-        <v>40000000</v>
-      </c>
-      <c r="H43" s="32"/>
-      <c r="I43" s="32"/>
-      <c r="J43" s="33" t="s">
-        <v>7</v>
-      </c>
+      <c r="H44" s="14"/>
+      <c r="I44" s="14"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="3:10" ht="15">
       <c r="C45" s="8"/>
-      <c r="D45" s="21"/>
-      <c r="E45" s="10"/>
-      <c r="F45" s="48"/>
-      <c r="G45" s="5"/>
-      <c r="H45" s="5"/>
-      <c r="I45" s="5"/>
-    </row>
-    <row r="46" spans="3:10" ht="15">
-      <c r="C46" s="8"/>
-      <c r="D46" s="21"/>
-      <c r="E46" s="10"/>
-      <c r="F46" s="48"/>
-      <c r="G46" s="12">
-        <f>G8-G32-G35-G43</f>
-        <v>-25505086</v>
-      </c>
-      <c r="H46" s="12"/>
-      <c r="I46" s="20"/>
-      <c r="J46" s="31" t="s">
+      <c r="D45" s="36"/>
+      <c r="E45" s="37"/>
+      <c r="F45" s="53"/>
+      <c r="G45" s="32">
+        <f>SUM(G40:G44)</f>
+        <v>40000000</v>
+      </c>
+      <c r="H45" s="32"/>
+      <c r="I45" s="32"/>
+      <c r="J45" s="33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="3:10" ht="15">
+      <c r="C47" s="8"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="48"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
+    </row>
+    <row r="48" spans="3:10" ht="15">
+      <c r="C48" s="8"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="48"/>
+      <c r="G48" s="12">
+        <f>G8-G34-G37-G45</f>
+        <v>-25605086</v>
+      </c>
+      <c r="H48" s="12"/>
+      <c r="I48" s="20"/>
+      <c r="J48" s="31" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2518,8 +2564,8 @@
     <mergeCell ref="C2:J2"/>
     <mergeCell ref="D4:G4"/>
     <mergeCell ref="D9:G9"/>
-    <mergeCell ref="D34:G34"/>
-    <mergeCell ref="D37:G37"/>
+    <mergeCell ref="D36:G36"/>
+    <mergeCell ref="D39:G39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3749,10 +3795,689 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C59F4560-1B60-4B5E-991D-A390F0A6ECED}">
-  <dimension ref="C2:J43"/>
+  <dimension ref="C2:J47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="5"/>
+    <col min="3" max="3" width="8.42578125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="37.85546875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="24" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="52" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.42578125" style="52" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="25" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" style="25" customWidth="1"/>
+    <col min="10" max="10" width="33.5703125" style="5" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:10" ht="20.25">
+      <c r="C2" s="93" t="s">
+        <v>197</v>
+      </c>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="93"/>
+    </row>
+    <row r="3" spans="3:10" ht="15.75">
+      <c r="C3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="3:10" ht="15.75" customHeight="1">
+      <c r="C4" s="7"/>
+      <c r="D4" s="97" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="97"/>
+      <c r="F4" s="97"/>
+      <c r="G4" s="97"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+    </row>
+    <row r="5" spans="3:10" ht="15">
+      <c r="C5" s="8">
+        <v>1</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E5" s="10">
+        <v>1</v>
+      </c>
+      <c r="F5" s="29">
+        <v>38328910</v>
+      </c>
+      <c r="G5" s="48">
+        <f>F5*E5</f>
+        <v>38328910</v>
+      </c>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="8"/>
+    </row>
+    <row r="6" spans="3:10">
+      <c r="C6" s="8">
+        <v>2</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="E6" s="10">
+        <v>1</v>
+      </c>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48">
+        <f>F6*E6</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="9"/>
+    </row>
+    <row r="7" spans="3:10">
+      <c r="C7" s="8">
+        <v>3</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="E7" s="10">
+        <v>1</v>
+      </c>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48">
+        <f>F7*E7</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="9"/>
+    </row>
+    <row r="8" spans="3:10" ht="15">
+      <c r="C8" s="8"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="49">
+        <f>SUM(G5:G7)</f>
+        <v>38328910</v>
+      </c>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="13" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10" ht="15">
+      <c r="C9" s="8"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="49">
+        <f>G8-G37</f>
+        <v>30528910</v>
+      </c>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="13" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" ht="15">
+      <c r="C10" s="8"/>
+      <c r="D10" s="97" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="97"/>
+      <c r="F10" s="97"/>
+      <c r="G10" s="97"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="15"/>
+    </row>
+    <row r="11" spans="3:10" ht="15">
+      <c r="C11" s="8"/>
+      <c r="D11" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="E11" s="38">
+        <v>3</v>
+      </c>
+      <c r="F11" s="29">
+        <v>116000</v>
+      </c>
+      <c r="G11" s="29">
+        <f>E11*F11</f>
+        <v>348000</v>
+      </c>
+      <c r="H11" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="11"/>
+      <c r="J11" s="9"/>
+    </row>
+    <row r="12" spans="3:10" ht="15">
+      <c r="C12" s="8"/>
+      <c r="D12" s="30" t="s">
+        <v>194</v>
+      </c>
+      <c r="E12" s="38">
+        <v>2</v>
+      </c>
+      <c r="F12" s="29">
+        <v>20000</v>
+      </c>
+      <c r="G12" s="29">
+        <f>E12*F12</f>
+        <v>40000</v>
+      </c>
+      <c r="H12" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12" s="11"/>
+      <c r="J12" s="9"/>
+    </row>
+    <row r="13" spans="3:10" ht="15">
+      <c r="C13" s="8"/>
+      <c r="D13" s="30" t="s">
+        <v>195</v>
+      </c>
+      <c r="E13" s="38">
+        <v>1</v>
+      </c>
+      <c r="F13" s="29">
+        <v>80000</v>
+      </c>
+      <c r="G13" s="29">
+        <f t="shared" ref="G13:G15" si="0">E13*F13</f>
+        <v>80000</v>
+      </c>
+      <c r="H13" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" s="11"/>
+      <c r="J13" s="9"/>
+    </row>
+    <row r="14" spans="3:10" ht="15">
+      <c r="C14" s="8"/>
+      <c r="D14" s="30" t="s">
+        <v>196</v>
+      </c>
+      <c r="E14" s="38">
+        <v>2</v>
+      </c>
+      <c r="F14" s="29">
+        <v>40000</v>
+      </c>
+      <c r="G14" s="29">
+        <f t="shared" si="0"/>
+        <v>80000</v>
+      </c>
+      <c r="H14" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="I14" s="11"/>
+      <c r="J14" s="9"/>
+    </row>
+    <row r="15" spans="3:10" ht="15">
+      <c r="C15" s="8"/>
+      <c r="D15" s="30" t="s">
+        <v>199</v>
+      </c>
+      <c r="E15" s="38">
+        <v>1</v>
+      </c>
+      <c r="F15" s="29">
+        <v>110000</v>
+      </c>
+      <c r="G15" s="29">
+        <f t="shared" si="0"/>
+        <v>110000</v>
+      </c>
+      <c r="H15" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="I15" s="11"/>
+      <c r="J15" s="9"/>
+    </row>
+    <row r="16" spans="3:10" ht="15">
+      <c r="C16" s="8"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="9"/>
+    </row>
+    <row r="17" spans="3:10" ht="15">
+      <c r="C17" s="8"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="55">
+        <f>SUM(G11:G15)</f>
+        <v>658000</v>
+      </c>
+      <c r="H17" s="56"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="3:10" ht="15">
+      <c r="C18" s="8"/>
+      <c r="D18" s="97" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="97"/>
+      <c r="F18" s="97"/>
+      <c r="G18" s="97"/>
+      <c r="H18" s="76"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="9"/>
+    </row>
+    <row r="19" spans="3:10" ht="15">
+      <c r="C19" s="8"/>
+      <c r="D19" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="E19" s="38">
+        <v>1</v>
+      </c>
+      <c r="F19" s="29">
+        <v>4800000</v>
+      </c>
+      <c r="G19" s="29">
+        <f>F19*E19</f>
+        <v>4800000</v>
+      </c>
+      <c r="H19" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="I19" s="11"/>
+      <c r="J19" s="9"/>
+    </row>
+    <row r="20" spans="3:10" ht="15">
+      <c r="C20" s="8"/>
+      <c r="D20" s="30" t="s">
+        <v>190</v>
+      </c>
+      <c r="E20" s="38">
+        <v>1</v>
+      </c>
+      <c r="F20" s="29">
+        <v>3000000</v>
+      </c>
+      <c r="G20" s="29">
+        <f t="shared" ref="G20:G22" si="1">F20*E20</f>
+        <v>3000000</v>
+      </c>
+      <c r="H20" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="I20" s="11"/>
+      <c r="J20" s="9"/>
+    </row>
+    <row r="21" spans="3:10" ht="15">
+      <c r="C21" s="8"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H21" s="30"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="9"/>
+    </row>
+    <row r="22" spans="3:10" ht="15">
+      <c r="C22" s="8"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H22" s="30"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="9"/>
+    </row>
+    <row r="23" spans="3:10" ht="15">
+      <c r="C23" s="8"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="9"/>
+    </row>
+    <row r="24" spans="3:10" ht="15">
+      <c r="C24" s="8"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="9"/>
+    </row>
+    <row r="25" spans="3:10" s="46" customFormat="1" ht="15">
+      <c r="C25" s="8"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="45"/>
+      <c r="I25" s="41"/>
+      <c r="J25" s="41"/>
+    </row>
+    <row r="26" spans="3:10" ht="15">
+      <c r="C26" s="8"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="15"/>
+    </row>
+    <row r="27" spans="3:10" ht="15">
+      <c r="C27" s="8"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="9"/>
+    </row>
+    <row r="28" spans="3:10" ht="15">
+      <c r="C28" s="8"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="9"/>
+    </row>
+    <row r="29" spans="3:10" ht="15">
+      <c r="C29" s="8"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="9"/>
+    </row>
+    <row r="30" spans="3:10" ht="15">
+      <c r="C30" s="8"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="9"/>
+    </row>
+    <row r="31" spans="3:10" ht="15">
+      <c r="C31" s="8"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="9"/>
+    </row>
+    <row r="32" spans="3:10" ht="15">
+      <c r="C32" s="8"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="38"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="30"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="9"/>
+    </row>
+    <row r="33" spans="3:10" ht="15">
+      <c r="C33" s="8"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="39"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="9"/>
+    </row>
+    <row r="34" spans="3:10" ht="15">
+      <c r="C34" s="8"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="39"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="30"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="9"/>
+    </row>
+    <row r="35" spans="3:10" ht="15">
+      <c r="C35" s="8"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="30"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="9"/>
+    </row>
+    <row r="36" spans="3:10" ht="15">
+      <c r="C36" s="8"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="29"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="30"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="75"/>
+    </row>
+    <row r="37" spans="3:10" ht="15">
+      <c r="C37" s="8"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="29"/>
+      <c r="G37" s="55">
+        <f>SUM(G19:G36)</f>
+        <v>7800000</v>
+      </c>
+      <c r="H37" s="56"/>
+      <c r="I37" s="35"/>
+      <c r="J37" s="33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="3:10" ht="15">
+      <c r="C38" s="8"/>
+      <c r="D38" s="97" t="s">
+        <v>27</v>
+      </c>
+      <c r="E38" s="97"/>
+      <c r="F38" s="97"/>
+      <c r="G38" s="97"/>
+      <c r="H38" s="57"/>
+      <c r="I38" s="11"/>
+      <c r="J38" s="8"/>
+    </row>
+    <row r="39" spans="3:10" ht="15">
+      <c r="C39" s="8">
+        <v>1</v>
+      </c>
+      <c r="D39" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" s="10"/>
+      <c r="F39" s="48"/>
+      <c r="G39" s="50"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="14"/>
+      <c r="J39" s="34"/>
+    </row>
+    <row r="40" spans="3:10" ht="15">
+      <c r="C40" s="8">
+        <v>2</v>
+      </c>
+      <c r="D40" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="10"/>
+      <c r="F40" s="48"/>
+      <c r="G40" s="50"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="14"/>
+      <c r="J40" s="22"/>
+    </row>
+    <row r="41" spans="3:10" ht="15">
+      <c r="C41" s="8">
+        <v>3</v>
+      </c>
+      <c r="D41" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E41" s="10"/>
+      <c r="F41" s="48"/>
+      <c r="G41" s="50"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="11"/>
+      <c r="J41" s="22"/>
+    </row>
+    <row r="42" spans="3:10" ht="15">
+      <c r="C42" s="8">
+        <v>4</v>
+      </c>
+      <c r="D42" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" s="10"/>
+      <c r="F42" s="48"/>
+      <c r="G42" s="50"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="22"/>
+    </row>
+    <row r="43" spans="3:10" ht="15">
+      <c r="C43" s="8"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="48"/>
+      <c r="G43" s="50"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="22"/>
+    </row>
+    <row r="44" spans="3:10" ht="15">
+      <c r="C44" s="8"/>
+      <c r="D44" s="36"/>
+      <c r="E44" s="37"/>
+      <c r="F44" s="53"/>
+      <c r="G44" s="51">
+        <f>SUM(G39:G43)</f>
+        <v>0</v>
+      </c>
+      <c r="H44" s="32"/>
+      <c r="I44" s="32"/>
+      <c r="J44" s="33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="3:10">
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="48"/>
+      <c r="G45" s="48"/>
+      <c r="H45" s="23"/>
+      <c r="I45" s="23"/>
+      <c r="J45" s="8"/>
+    </row>
+    <row r="46" spans="3:10" ht="15">
+      <c r="C46" s="8"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="48"/>
+      <c r="G46" s="58"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="8"/>
+      <c r="J46" s="8"/>
+    </row>
+    <row r="47" spans="3:10" ht="15">
+      <c r="C47" s="8"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="48"/>
+      <c r="G47" s="49">
+        <f>G8-G17-G37</f>
+        <v>29870910</v>
+      </c>
+      <c r="H47" s="12"/>
+      <c r="I47" s="20"/>
+      <c r="J47" s="31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="D38:G38"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A00FBF6-6528-4077-97A8-E7F8FA86DD30}">
+  <dimension ref="C2:J42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3801,7 +4526,7 @@
         <v>17</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>170</v>
+        <v>4</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>5</v>
@@ -3815,56 +4540,49 @@
       <c r="E4" s="97"/>
       <c r="F4" s="97"/>
       <c r="G4" s="97"/>
-      <c r="H4" s="80"/>
+      <c r="H4" s="74"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
     </row>
-    <row r="5" spans="3:10" ht="15">
-      <c r="C5" s="8">
-        <v>1</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="E5" s="10">
-        <v>1</v>
-      </c>
-      <c r="F5" s="29">
-        <v>38328910</v>
-      </c>
-      <c r="G5" s="48">
-        <f>F5*E5</f>
-        <v>38328910</v>
-      </c>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="8"/>
+    <row r="5" spans="3:10" ht="20.25">
+      <c r="C5" s="7"/>
+      <c r="D5" s="97" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="97"/>
+      <c r="F5" s="97"/>
+      <c r="G5" s="97"/>
+      <c r="H5" s="80"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
     </row>
     <row r="6" spans="3:10">
       <c r="C6" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>154</v>
+        <v>31</v>
       </c>
       <c r="E6" s="10">
         <v>1</v>
       </c>
-      <c r="F6" s="48"/>
+      <c r="F6" s="48">
+        <v>29294650.400000002</v>
+      </c>
       <c r="G6" s="48">
         <f>F6*E6</f>
-        <v>0</v>
+        <v>29294650.400000002</v>
       </c>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
-      <c r="J6" s="9"/>
+      <c r="J6" s="8"/>
     </row>
     <row r="7" spans="3:10">
       <c r="C7" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="E7" s="10">
         <v>1</v>
@@ -3878,20 +4596,24 @@
       <c r="I7" s="11"/>
       <c r="J7" s="9"/>
     </row>
-    <row r="8" spans="3:10" ht="15">
-      <c r="C8" s="8"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="10"/>
+    <row r="8" spans="3:10">
+      <c r="C8" s="8">
+        <v>3</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="E8" s="10">
+        <v>1</v>
+      </c>
       <c r="F8" s="48"/>
-      <c r="G8" s="49">
-        <f>SUM(G5:G7)</f>
-        <v>38328910</v>
-      </c>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="13" t="s">
-        <v>168</v>
-      </c>
+      <c r="G8" s="48">
+        <f>F8*E8</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="9"/>
     </row>
     <row r="9" spans="3:10" ht="15">
       <c r="C9" s="8"/>
@@ -3899,45 +4621,31 @@
       <c r="E9" s="10"/>
       <c r="F9" s="48"/>
       <c r="G9" s="49">
-        <f>G8-G33</f>
-        <v>30528910</v>
+        <f>SUM(G6:G8)</f>
+        <v>29294650.400000002</v>
       </c>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
       <c r="J9" s="13" t="s">
-        <v>169</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="3:10" ht="15">
       <c r="C10" s="8"/>
-      <c r="D10" s="97" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="97"/>
-      <c r="F10" s="97"/>
-      <c r="G10" s="97"/>
-      <c r="H10" s="76"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="15"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="9"/>
     </row>
     <row r="11" spans="3:10" ht="15">
       <c r="C11" s="8"/>
-      <c r="D11" s="30" t="s">
-        <v>191</v>
-      </c>
-      <c r="E11" s="38">
-        <v>1</v>
-      </c>
-      <c r="F11" s="29">
-        <v>195000</v>
-      </c>
-      <c r="G11" s="29">
-        <f>E11*F11</f>
-        <v>195000</v>
-      </c>
-      <c r="H11" s="30" t="s">
-        <v>9</v>
-      </c>
+      <c r="D11" s="30"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="30"/>
       <c r="I11" s="11"/>
       <c r="J11" s="9"/>
     </row>
@@ -3946,73 +4654,84 @@
       <c r="D12" s="30"/>
       <c r="E12" s="38"/>
       <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="9"/>
+      <c r="G12" s="55">
+        <f>SUM(G10:G10)</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="56"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="33" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="13" spans="3:10" ht="15">
       <c r="C13" s="8"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="55">
-        <f>SUM(G11:G11)</f>
-        <v>195000</v>
-      </c>
-      <c r="H13" s="56"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="33" t="s">
-        <v>7</v>
-      </c>
+      <c r="D13" s="97" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="97"/>
+      <c r="F13" s="97"/>
+      <c r="G13" s="97"/>
+      <c r="H13" s="74"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="9"/>
     </row>
     <row r="14" spans="3:10" ht="15">
       <c r="C14" s="8"/>
-      <c r="D14" s="97" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" s="97"/>
-      <c r="F14" s="97"/>
-      <c r="G14" s="97"/>
-      <c r="H14" s="76"/>
+      <c r="D14" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="E14" s="38">
+        <v>1</v>
+      </c>
+      <c r="F14" s="29">
+        <v>9064000</v>
+      </c>
+      <c r="G14" s="29">
+        <f>F14*E14</f>
+        <v>9064000</v>
+      </c>
+      <c r="H14" s="30" t="s">
+        <v>22</v>
+      </c>
       <c r="I14" s="11"/>
       <c r="J14" s="9"/>
     </row>
     <row r="15" spans="3:10" ht="15">
       <c r="C15" s="8"/>
       <c r="D15" s="30" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="E15" s="38">
         <v>1</v>
       </c>
       <c r="F15" s="29">
-        <v>4800000</v>
+        <v>200000</v>
       </c>
       <c r="G15" s="29">
         <f>F15*E15</f>
-        <v>4800000</v>
+        <v>200000</v>
       </c>
       <c r="H15" s="30" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="I15" s="11"/>
       <c r="J15" s="9"/>
     </row>
     <row r="16" spans="3:10" ht="15">
       <c r="C16" s="8"/>
-      <c r="D16" s="30" t="s">
-        <v>190</v>
-      </c>
-      <c r="E16" s="38">
-        <v>1</v>
-      </c>
-      <c r="F16" s="29">
-        <v>3000000</v>
+      <c r="D16" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E16" s="3">
+        <v>1</v>
+      </c>
+      <c r="F16" s="39">
+        <v>21000000</v>
       </c>
       <c r="G16" s="29">
-        <f t="shared" ref="G16:G18" si="0">F16*E16</f>
-        <v>3000000</v>
+        <f t="shared" ref="G16:G23" si="0">F16*E16</f>
+        <v>21000000</v>
       </c>
       <c r="H16" s="30" t="s">
         <v>51</v>
@@ -4025,10 +4744,7 @@
       <c r="D17" s="1"/>
       <c r="E17" s="3"/>
       <c r="F17" s="39"/>
-      <c r="G17" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G17" s="29"/>
       <c r="H17" s="30"/>
       <c r="I17" s="11"/>
       <c r="J17" s="9"/>
@@ -4038,17 +4754,14 @@
       <c r="D18" s="1"/>
       <c r="E18" s="3"/>
       <c r="F18" s="39"/>
-      <c r="G18" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G18" s="29"/>
       <c r="H18" s="30"/>
       <c r="I18" s="11"/>
       <c r="J18" s="9"/>
     </row>
     <row r="19" spans="3:10" ht="15">
       <c r="C19" s="8"/>
-      <c r="D19" s="1"/>
+      <c r="D19" s="2"/>
       <c r="E19" s="3"/>
       <c r="F19" s="39"/>
       <c r="G19" s="29"/>
@@ -4056,35 +4769,35 @@
       <c r="I19" s="11"/>
       <c r="J19" s="9"/>
     </row>
-    <row r="20" spans="3:10" ht="15">
+    <row r="20" spans="3:10" s="46" customFormat="1" ht="15">
       <c r="C20" s="8"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="39"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="44"/>
       <c r="G20" s="29"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="9"/>
-    </row>
-    <row r="21" spans="3:10" s="46" customFormat="1" ht="15">
+      <c r="H20" s="45"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="41"/>
+    </row>
+    <row r="21" spans="3:10" ht="15">
       <c r="C21" s="8"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="44"/>
-      <c r="G21" s="44"/>
-      <c r="H21" s="45"/>
-      <c r="I21" s="41"/>
-      <c r="J21" s="41"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="15"/>
     </row>
     <row r="22" spans="3:10" ht="15">
       <c r="C22" s="8"/>
-      <c r="D22" s="28"/>
+      <c r="D22" s="30"/>
       <c r="E22" s="38"/>
       <c r="F22" s="29"/>
       <c r="G22" s="29"/>
       <c r="H22" s="30"/>
-      <c r="I22" s="30"/>
-      <c r="J22" s="15"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="9"/>
     </row>
     <row r="23" spans="3:10" ht="15">
       <c r="C23" s="8"/>
@@ -4138,9 +4851,9 @@
     </row>
     <row r="28" spans="3:10" ht="15">
       <c r="C28" s="8"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="29"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="39"/>
       <c r="G28" s="29"/>
       <c r="H28" s="30"/>
       <c r="I28" s="11"/>
@@ -4168,618 +4881,6 @@
     </row>
     <row r="31" spans="3:10" ht="15">
       <c r="C31" s="8"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="39"/>
-      <c r="G31" s="29"/>
-      <c r="H31" s="30"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="9"/>
-    </row>
-    <row r="32" spans="3:10" ht="15">
-      <c r="C32" s="8"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="38"/>
-      <c r="F32" s="29"/>
-      <c r="G32" s="29"/>
-      <c r="H32" s="30"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="75"/>
-    </row>
-    <row r="33" spans="3:10" ht="15">
-      <c r="C33" s="8"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="55">
-        <f>SUM(G15:G32)</f>
-        <v>7800000</v>
-      </c>
-      <c r="H33" s="56"/>
-      <c r="I33" s="35"/>
-      <c r="J33" s="33" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="3:10" ht="15">
-      <c r="C34" s="8"/>
-      <c r="D34" s="97" t="s">
-        <v>27</v>
-      </c>
-      <c r="E34" s="97"/>
-      <c r="F34" s="97"/>
-      <c r="G34" s="97"/>
-      <c r="H34" s="57"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="8"/>
-    </row>
-    <row r="35" spans="3:10" ht="15">
-      <c r="C35" s="8">
-        <v>1</v>
-      </c>
-      <c r="D35" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35" s="10"/>
-      <c r="F35" s="48"/>
-      <c r="G35" s="50"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
-      <c r="J35" s="34"/>
-    </row>
-    <row r="36" spans="3:10" ht="15">
-      <c r="C36" s="8">
-        <v>2</v>
-      </c>
-      <c r="D36" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="E36" s="10"/>
-      <c r="F36" s="48"/>
-      <c r="G36" s="50"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="22"/>
-    </row>
-    <row r="37" spans="3:10" ht="15">
-      <c r="C37" s="8">
-        <v>3</v>
-      </c>
-      <c r="D37" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="E37" s="10"/>
-      <c r="F37" s="48"/>
-      <c r="G37" s="50"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="22"/>
-    </row>
-    <row r="38" spans="3:10" ht="15">
-      <c r="C38" s="8">
-        <v>4</v>
-      </c>
-      <c r="D38" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="E38" s="10"/>
-      <c r="F38" s="48"/>
-      <c r="G38" s="50"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="22"/>
-    </row>
-    <row r="39" spans="3:10" ht="15">
-      <c r="C39" s="8"/>
-      <c r="D39" s="21"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="48"/>
-      <c r="G39" s="50"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="14"/>
-      <c r="J39" s="22"/>
-    </row>
-    <row r="40" spans="3:10" ht="15">
-      <c r="C40" s="8"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="37"/>
-      <c r="F40" s="53"/>
-      <c r="G40" s="51">
-        <f>SUM(G35:G39)</f>
-        <v>0</v>
-      </c>
-      <c r="H40" s="32"/>
-      <c r="I40" s="32"/>
-      <c r="J40" s="33" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="3:10">
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="48"/>
-      <c r="G41" s="48"/>
-      <c r="H41" s="23"/>
-      <c r="I41" s="23"/>
-      <c r="J41" s="8"/>
-    </row>
-    <row r="42" spans="3:10" ht="15">
-      <c r="C42" s="8"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="48"/>
-      <c r="G42" s="58"/>
-      <c r="H42" s="8"/>
-      <c r="I42" s="8"/>
-      <c r="J42" s="8"/>
-    </row>
-    <row r="43" spans="3:10" ht="15">
-      <c r="C43" s="8"/>
-      <c r="D43" s="21"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="48"/>
-      <c r="G43" s="49">
-        <f>G8-G13-G33</f>
-        <v>30333910</v>
-      </c>
-      <c r="H43" s="12"/>
-      <c r="I43" s="20"/>
-      <c r="J43" s="31" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="D14:G14"/>
-    <mergeCell ref="D34:G34"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A00FBF6-6528-4077-97A8-E7F8FA86DD30}">
-  <dimension ref="C2:J42"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <cols>
-    <col min="1" max="2" width="9.140625" style="5"/>
-    <col min="3" max="3" width="8.42578125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="37.85546875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="24" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" style="52" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.42578125" style="52" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="25" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" style="25" customWidth="1"/>
-    <col min="10" max="10" width="33.5703125" style="5" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="5"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="3:10" ht="20.25">
-      <c r="C2" s="93" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
-      <c r="H2" s="93"/>
-      <c r="I2" s="93"/>
-      <c r="J2" s="93"/>
-    </row>
-    <row r="3" spans="3:10" ht="15.75">
-      <c r="C3" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="47" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="47" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="3:10" ht="15.75" customHeight="1">
-      <c r="C4" s="7"/>
-      <c r="D4" s="97" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="97"/>
-      <c r="F4" s="97"/>
-      <c r="G4" s="97"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-    </row>
-    <row r="5" spans="3:10" ht="20.25">
-      <c r="C5" s="7"/>
-      <c r="D5" s="97" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="97"/>
-      <c r="F5" s="97"/>
-      <c r="G5" s="97"/>
-      <c r="H5" s="80"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-    </row>
-    <row r="6" spans="3:10">
-      <c r="C6" s="8">
-        <v>1</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="10">
-        <v>1</v>
-      </c>
-      <c r="F6" s="48">
-        <v>29294650.400000002</v>
-      </c>
-      <c r="G6" s="48">
-        <f>F6*E6</f>
-        <v>29294650.400000002</v>
-      </c>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="8"/>
-    </row>
-    <row r="7" spans="3:10">
-      <c r="C7" s="8">
-        <v>2</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="E7" s="10">
-        <v>1</v>
-      </c>
-      <c r="F7" s="48"/>
-      <c r="G7" s="48">
-        <f>F7*E7</f>
-        <v>0</v>
-      </c>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="9"/>
-    </row>
-    <row r="8" spans="3:10">
-      <c r="C8" s="8">
-        <v>3</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="E8" s="10">
-        <v>1</v>
-      </c>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48">
-        <f>F8*E8</f>
-        <v>0</v>
-      </c>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="9"/>
-    </row>
-    <row r="9" spans="3:10" ht="15">
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="49">
-        <f>SUM(G6:G8)</f>
-        <v>29294650.400000002</v>
-      </c>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="3:10" ht="15">
-      <c r="C10" s="8"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="9"/>
-    </row>
-    <row r="11" spans="3:10" ht="15">
-      <c r="C11" s="8"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="9"/>
-    </row>
-    <row r="12" spans="3:10" ht="15">
-      <c r="C12" s="8"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="55">
-        <f>SUM(G10:G10)</f>
-        <v>0</v>
-      </c>
-      <c r="H12" s="56"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="33" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="3:10" ht="15">
-      <c r="C13" s="8"/>
-      <c r="D13" s="97" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="97"/>
-      <c r="F13" s="97"/>
-      <c r="G13" s="97"/>
-      <c r="H13" s="74"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="9"/>
-    </row>
-    <row r="14" spans="3:10" ht="15">
-      <c r="C14" s="8"/>
-      <c r="D14" s="30" t="s">
-        <v>138</v>
-      </c>
-      <c r="E14" s="38">
-        <v>1</v>
-      </c>
-      <c r="F14" s="29">
-        <v>9064000</v>
-      </c>
-      <c r="G14" s="29">
-        <f>F14*E14</f>
-        <v>9064000</v>
-      </c>
-      <c r="H14" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="I14" s="11"/>
-      <c r="J14" s="9"/>
-    </row>
-    <row r="15" spans="3:10" ht="15">
-      <c r="C15" s="8"/>
-      <c r="D15" s="30" t="s">
-        <v>147</v>
-      </c>
-      <c r="E15" s="38">
-        <v>1</v>
-      </c>
-      <c r="F15" s="29">
-        <v>200000</v>
-      </c>
-      <c r="G15" s="29">
-        <f>F15*E15</f>
-        <v>200000</v>
-      </c>
-      <c r="H15" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="I15" s="11"/>
-      <c r="J15" s="9"/>
-    </row>
-    <row r="16" spans="3:10" ht="15">
-      <c r="C16" s="8"/>
-      <c r="D16" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="E16" s="3">
-        <v>1</v>
-      </c>
-      <c r="F16" s="39">
-        <v>21000000</v>
-      </c>
-      <c r="G16" s="29">
-        <f t="shared" ref="G16:G23" si="0">F16*E16</f>
-        <v>21000000</v>
-      </c>
-      <c r="H16" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="I16" s="11"/>
-      <c r="J16" s="9"/>
-    </row>
-    <row r="17" spans="3:10" ht="15">
-      <c r="C17" s="8"/>
-      <c r="D17" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="E17" s="3">
-        <v>1</v>
-      </c>
-      <c r="F17" s="39">
-        <v>4200000</v>
-      </c>
-      <c r="G17" s="29">
-        <f t="shared" si="0"/>
-        <v>4200000</v>
-      </c>
-      <c r="H17" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="I17" s="11"/>
-      <c r="J17" s="9"/>
-    </row>
-    <row r="18" spans="3:10" ht="15">
-      <c r="C18" s="8"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H18" s="30"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="9"/>
-    </row>
-    <row r="19" spans="3:10" ht="15">
-      <c r="C19" s="8"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H19" s="30"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="9"/>
-    </row>
-    <row r="20" spans="3:10" s="46" customFormat="1" ht="15">
-      <c r="C20" s="8"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="44"/>
-      <c r="G20" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H20" s="45"/>
-      <c r="I20" s="41"/>
-      <c r="J20" s="41"/>
-    </row>
-    <row r="21" spans="3:10" ht="15">
-      <c r="C21" s="8"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="38"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H21" s="30"/>
-      <c r="I21" s="30"/>
-      <c r="J21" s="15"/>
-    </row>
-    <row r="22" spans="3:10" ht="15">
-      <c r="C22" s="8"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H22" s="30"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="9"/>
-    </row>
-    <row r="23" spans="3:10" ht="15">
-      <c r="C23" s="8"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="38"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H23" s="30"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="9"/>
-    </row>
-    <row r="24" spans="3:10" ht="15">
-      <c r="C24" s="8"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="29"/>
-      <c r="G24" s="29"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="9"/>
-    </row>
-    <row r="25" spans="3:10" ht="15">
-      <c r="C25" s="8"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="30"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="9"/>
-    </row>
-    <row r="26" spans="3:10" ht="15">
-      <c r="C26" s="8"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="38"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="29"/>
-      <c r="H26" s="30"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="9"/>
-    </row>
-    <row r="27" spans="3:10" ht="15">
-      <c r="C27" s="8"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="30"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="9"/>
-    </row>
-    <row r="28" spans="3:10" ht="15">
-      <c r="C28" s="8"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="30"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="9"/>
-    </row>
-    <row r="29" spans="3:10" ht="15">
-      <c r="C29" s="8"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="9"/>
-    </row>
-    <row r="30" spans="3:10" ht="15">
-      <c r="C30" s="8"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="29"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="9"/>
-    </row>
-    <row r="31" spans="3:10" ht="15">
-      <c r="C31" s="8"/>
       <c r="D31" s="30"/>
       <c r="E31" s="38"/>
       <c r="F31" s="29"/>
@@ -4795,7 +4896,7 @@
       <c r="F32" s="29"/>
       <c r="G32" s="55">
         <f>SUM(G14:G31)</f>
-        <v>34464000</v>
+        <v>30264000</v>
       </c>
       <c r="H32" s="56"/>
       <c r="I32" s="35"/>
@@ -4923,7 +5024,7 @@
       <c r="F42" s="48"/>
       <c r="G42" s="49">
         <f>G8-G12-G32</f>
-        <v>-34464000</v>
+        <v>-30264000</v>
       </c>
       <c r="H42" s="12"/>
       <c r="I42" s="20"/>
@@ -4948,7 +5049,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F413B64-656B-492A-8F7D-8434699F234E}">
   <dimension ref="C2:J32"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B4" workbookViewId="0">
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
@@ -5948,8 +6049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73990C79-75DF-434D-B272-2581D279AD79}">
   <dimension ref="C2:J80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -6322,7 +6423,7 @@
         <v>120000</v>
       </c>
       <c r="G22" s="29">
-        <f t="shared" ref="G22:G51" si="1">E22*F22</f>
+        <f t="shared" ref="G22:G52" si="1">E22*F22</f>
         <v>120000</v>
       </c>
       <c r="H22" s="30" t="s">
@@ -6962,7 +7063,7 @@
     <row r="51" spans="3:10" ht="15">
       <c r="C51" s="8"/>
       <c r="D51" s="30" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E51" s="3">
         <v>1</v>
@@ -6982,11 +7083,22 @@
     </row>
     <row r="52" spans="3:10" ht="15">
       <c r="C52" s="8"/>
-      <c r="D52" s="30"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="29"/>
-      <c r="G52" s="29"/>
-      <c r="H52" s="9"/>
+      <c r="D52" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="E52" s="3">
+        <v>1</v>
+      </c>
+      <c r="F52" s="29">
+        <v>100000</v>
+      </c>
+      <c r="G52" s="29">
+        <f t="shared" si="1"/>
+        <v>100000</v>
+      </c>
+      <c r="H52" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="I52" s="8"/>
       <c r="J52" s="8"/>
     </row>
@@ -7016,8 +7128,8 @@
       <c r="E55" s="38"/>
       <c r="F55" s="29"/>
       <c r="G55" s="55">
-        <f>SUM(G21:G51)</f>
-        <v>4508000</v>
+        <f>SUM(G21:G52)</f>
+        <v>4608000</v>
       </c>
       <c r="H55" s="56"/>
       <c r="I55" s="35"/>
@@ -7426,7 +7538,7 @@
       <c r="F80" s="48"/>
       <c r="G80" s="49">
         <f>G8-G19-G55-G62-G72-G78</f>
-        <v>-32138700</v>
+        <v>-32238700</v>
       </c>
       <c r="H80" s="12"/>
       <c r="I80" s="20"/>

</xml_diff>

<commit_message>
Update theo dõi luồng tiền tại các tài khoản
</commit_message>
<xml_diff>
--- a/Project/TongHopQuy2.xlsx
+++ b/Project/TongHopQuy2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VitechSolutions\Team_Log\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ViTechSolution_LTD\04.Team_Log\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8356763D-34CB-434A-BDF2-19B3F6BA5324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A63C4E-DD6A-4B7D-80B2-B5FC2A4343C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tổng hợp quỹ công ty" sheetId="6" r:id="rId1"/>
@@ -23,17 +23,20 @@
     <sheet name="SMARTHOME" sheetId="5" r:id="rId8"/>
     <sheet name="Chi Phí Công ty" sheetId="8" r:id="rId9"/>
     <sheet name="Quản lý tài khoản CT" sheetId="14" r:id="rId10"/>
+    <sheet name="Quản lý tiền vào ra tài khoản" sheetId="16" r:id="rId11"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId11"/>
+    <externalReference r:id="rId12"/>
   </externalReferences>
   <definedNames>
     <definedName name="chi_phi_cong_ty">'Chi Phí Công ty'!$G$80</definedName>
+    <definedName name="Pega" localSheetId="10">PEGA!$G$46</definedName>
     <definedName name="Pega">PEGA!$G$48</definedName>
     <definedName name="RowTitleRegion1..C7" localSheetId="4">#REF!</definedName>
     <definedName name="RowTitleRegion1..C7" localSheetId="5">#REF!</definedName>
     <definedName name="RowTitleRegion1..C7" localSheetId="8">#REF!</definedName>
     <definedName name="RowTitleRegion1..C7" localSheetId="1">#REF!</definedName>
+    <definedName name="RowTitleRegion1..C7" localSheetId="10">#REF!</definedName>
     <definedName name="RowTitleRegion1..C7" localSheetId="7">#REF!</definedName>
     <definedName name="RowTitleRegion1..C7" localSheetId="2">#REF!</definedName>
     <definedName name="RowTitleRegion1..C7" localSheetId="6">#REF!</definedName>
@@ -42,6 +45,7 @@
     <definedName name="RowTitleRegion2..G5" localSheetId="5">#REF!</definedName>
     <definedName name="RowTitleRegion2..G5" localSheetId="8">#REF!</definedName>
     <definedName name="RowTitleRegion2..G5" localSheetId="1">#REF!</definedName>
+    <definedName name="RowTitleRegion2..G5" localSheetId="10">#REF!</definedName>
     <definedName name="RowTitleRegion2..G5" localSheetId="7">#REF!</definedName>
     <definedName name="RowTitleRegion2..G5" localSheetId="2">#REF!</definedName>
     <definedName name="RowTitleRegion2..G5" localSheetId="6">#REF!</definedName>
@@ -71,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="226">
   <si>
     <t>STT</t>
   </si>
@@ -673,6 +677,84 @@
   </si>
   <si>
     <t>Linh kiện hàn mạch NE5532 test</t>
+  </si>
+  <si>
+    <t>ăn trưa ngày 10/07</t>
+  </si>
+  <si>
+    <t>Tk Công ty</t>
+  </si>
+  <si>
+    <t>TK cá nhân VPB</t>
+  </si>
+  <si>
+    <t>TK cá nhân ACB</t>
+  </si>
+  <si>
+    <t>TK cá nhân TPB</t>
+  </si>
+  <si>
+    <t>Tiền dự án Pega</t>
+  </si>
+  <si>
+    <t>Ứng tiền du lịch</t>
+  </si>
+  <si>
+    <t>Ứng tiền a Khơ</t>
+  </si>
+  <si>
+    <t>Ứng tiền a Lực</t>
+  </si>
+  <si>
+    <t>Ck vẽ mạch anh Hưng</t>
+  </si>
+  <si>
+    <t>40PCs B1026</t>
+  </si>
+  <si>
+    <t>Nhận thêm 14tr tiền dự án</t>
+  </si>
+  <si>
+    <t>Cọc linh kiện digikey mạch màn hình 5in</t>
+  </si>
+  <si>
+    <t>Tiền màn hình 5 in x5</t>
+  </si>
+  <si>
+    <t>Tiền đặt mạch màn hình 5in</t>
+  </si>
+  <si>
+    <t>EC 20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chuyển nốt tiền linh kiện digikey </t>
+  </si>
+  <si>
+    <t>Ship linh kiện</t>
+  </si>
+  <si>
+    <t>Vận chuyển + thuế 40 BT1026</t>
+  </si>
+  <si>
+    <t>Cọc EC21</t>
+  </si>
+  <si>
+    <t>Anh Khơ rút Chuyển vào tk cá nhân TPBank Tuấn</t>
+  </si>
+  <si>
+    <t>Cọc đặt mạch zeus</t>
+  </si>
+  <si>
+    <t>Cọc đặt mạch hecquyn</t>
+  </si>
+  <si>
+    <t>Nhận tiền dự án từ tk cty</t>
+  </si>
+  <si>
+    <t>ứng tiền anh thịnh vẽ mạch</t>
+  </si>
+  <si>
+    <t>Tuấn ứng tiền dự án</t>
   </si>
 </sst>
 </file>
@@ -773,7 +855,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -819,6 +901,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -903,7 +991,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1162,6 +1250,10 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="10" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1519,7 +1611,7 @@
       </c>
       <c r="J4" s="11">
         <f>chi_phi_cong_ty</f>
-        <v>-32238700</v>
+        <v>-32298700</v>
       </c>
       <c r="K4" s="8"/>
     </row>
@@ -1590,7 +1682,7 @@
       <c r="I12" s="9"/>
       <c r="J12" s="12">
         <f>SUM(J4:J11)</f>
-        <v>-71778766.400000006</v>
+        <v>-71838766.400000006</v>
       </c>
       <c r="K12" s="13" t="s">
         <v>7</v>
@@ -1726,12 +1818,334 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F9372CB-71CC-4641-8BE0-54E7DBA302DF}">
+  <dimension ref="A1:E28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="44.5703125" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" style="81" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" style="81" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="81" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" style="81" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="98" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="99" t="s">
+        <v>201</v>
+      </c>
+      <c r="C1" s="99" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1" s="99" t="s">
+        <v>203</v>
+      </c>
+      <c r="E1" s="99" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="30" t="s">
+        <v>205</v>
+      </c>
+      <c r="B2" s="50">
+        <v>79000000</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="30"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="30" t="s">
+        <v>206</v>
+      </c>
+      <c r="B4" s="29"/>
+      <c r="C4" s="32">
+        <v>-25000000</v>
+      </c>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="21" t="s">
+        <v>207</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="14">
+        <v>-5000000</v>
+      </c>
+      <c r="E5" s="14"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="14">
+        <v>-25000000</v>
+      </c>
+      <c r="E6" s="14"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29">
+        <v>-10000000</v>
+      </c>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="30" t="s">
+        <v>210</v>
+      </c>
+      <c r="B8" s="29"/>
+      <c r="C8" s="100">
+        <v>-8606000</v>
+      </c>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="30" t="s">
+        <v>211</v>
+      </c>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29">
+        <v>14000000</v>
+      </c>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+    </row>
+    <row r="10" spans="1:5" ht="15.75">
+      <c r="A10" s="30" t="s">
+        <v>212</v>
+      </c>
+      <c r="B10" s="29"/>
+      <c r="C10" s="101">
+        <v>-2500000</v>
+      </c>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="30" t="s">
+        <v>213</v>
+      </c>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29">
+        <v>-5894900</v>
+      </c>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="30" t="s">
+        <v>214</v>
+      </c>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29">
+        <v>-2950000</v>
+      </c>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="30" t="s">
+        <v>215</v>
+      </c>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29">
+        <v>-733000</v>
+      </c>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="30" t="s">
+        <v>216</v>
+      </c>
+      <c r="B14" s="29"/>
+      <c r="C14" s="29">
+        <v>-2547152</v>
+      </c>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="30"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29">
+        <v>-2272000</v>
+      </c>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+    </row>
+    <row r="16" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A16" s="30" t="s">
+        <v>217</v>
+      </c>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29">
+        <v>-24000</v>
+      </c>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="30" t="s">
+        <v>218</v>
+      </c>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29">
+        <v>-2014000</v>
+      </c>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="30" t="s">
+        <v>219</v>
+      </c>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29">
+        <v>-210000</v>
+      </c>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>220</v>
+      </c>
+      <c r="B19"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29">
+        <v>25000000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="30" t="s">
+        <v>221</v>
+      </c>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29">
+        <v>-3000000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="30" t="s">
+        <v>222</v>
+      </c>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29">
+        <v>-21000000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="30" t="s">
+        <v>223</v>
+      </c>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29">
+        <v>19600000</v>
+      </c>
+      <c r="E22" s="29"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="30" t="s">
+        <v>224</v>
+      </c>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29">
+        <v>-5000000</v>
+      </c>
+      <c r="E23" s="29"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="30" t="s">
+        <v>225</v>
+      </c>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29">
+        <v>-14000000</v>
+      </c>
+      <c r="E24" s="29"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="30"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="30"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="30"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="30"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29">
+        <f>SUM(C4:C18)</f>
+        <v>-78751052</v>
+      </c>
+      <c r="D28" s="29">
+        <f>SUM(D22:D26)</f>
+        <v>600000</v>
+      </c>
+      <c r="E28" s="29">
+        <f>SUM(E19:E27)</f>
+        <v>1000000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8032BD6C-08F6-46C4-8E07-045BAFBCF7A7}">
   <dimension ref="C2:J48"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3797,8 +4211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C59F4560-1B60-4B5E-991D-A390F0A6ECED}">
   <dimension ref="C2:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4730,7 +5144,7 @@
         <v>21000000</v>
       </c>
       <c r="G16" s="29">
-        <f t="shared" ref="G16:G23" si="0">F16*E16</f>
+        <f t="shared" ref="G16" si="0">F16*E16</f>
         <v>21000000</v>
       </c>
       <c r="H16" s="30" t="s">
@@ -6049,8 +6463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73990C79-75DF-434D-B272-2581D279AD79}">
   <dimension ref="C2:J80"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I52" sqref="I52"/>
+    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -6423,7 +6837,7 @@
         <v>120000</v>
       </c>
       <c r="G22" s="29">
-        <f t="shared" ref="G22:G52" si="1">E22*F22</f>
+        <f t="shared" ref="G22:G53" si="1">E22*F22</f>
         <v>120000</v>
       </c>
       <c r="H22" s="30" t="s">
@@ -7104,11 +7518,22 @@
     </row>
     <row r="53" spans="3:10" ht="15">
       <c r="C53" s="8"/>
-      <c r="D53" s="30"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="29"/>
-      <c r="G53" s="29"/>
-      <c r="H53" s="9"/>
+      <c r="D53" s="30" t="s">
+        <v>200</v>
+      </c>
+      <c r="E53" s="3">
+        <v>1</v>
+      </c>
+      <c r="F53" s="29">
+        <v>60000</v>
+      </c>
+      <c r="G53" s="29">
+        <f t="shared" si="1"/>
+        <v>60000</v>
+      </c>
+      <c r="H53" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="I53" s="8"/>
       <c r="J53" s="8"/>
     </row>
@@ -7128,8 +7553,8 @@
       <c r="E55" s="38"/>
       <c r="F55" s="29"/>
       <c r="G55" s="55">
-        <f>SUM(G21:G52)</f>
-        <v>4608000</v>
+        <f>SUM(G21:G53)</f>
+        <v>4668000</v>
       </c>
       <c r="H55" s="56"/>
       <c r="I55" s="35"/>
@@ -7538,7 +7963,7 @@
       <c r="F80" s="48"/>
       <c r="G80" s="49">
         <f>G8-G19-G55-G62-G72-G78</f>
-        <v>-32238700</v>
+        <v>-32298700</v>
       </c>
       <c r="H80" s="12"/>
       <c r="I80" s="20"/>

</xml_diff>

<commit_message>
Update sau khi nhan 170 BT-1026
</commit_message>
<xml_diff>
--- a/Project/TongHopQuy2.xlsx
+++ b/Project/TongHopQuy2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ViTechSolution_LTD\04.Team_Log\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF51C5A-8721-43A1-B079-C48BA8B5A719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67195B82-5C7D-40B8-AC87-33ABF867161F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tổng hợp quỹ công ty" sheetId="6" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="238">
   <si>
     <t>STT</t>
   </si>
@@ -779,6 +779,18 @@
   </si>
   <si>
     <t>Tuấn thanh lý Pi compute -&gt; ứng</t>
+  </si>
+  <si>
+    <t>Tuấn ứng cho anh Khơ</t>
+  </si>
+  <si>
+    <t>Thuế nhập khẩu</t>
+  </si>
+  <si>
+    <t>Phí làm tờ khai hải quan</t>
+  </si>
+  <si>
+    <t>Làm luật HQ</t>
   </si>
 </sst>
 </file>
@@ -1862,10 +1874,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F9372CB-71CC-4641-8BE0-54E7DBA302DF}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2162,27 +2174,52 @@
         <v>2200000</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="28"/>
+    <row r="27" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A27" s="28" t="s">
+        <v>234</v>
+      </c>
       <c r="B27" s="27"/>
       <c r="C27" s="27"/>
       <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="E27" s="27">
+        <v>-2000000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="14.25" customHeight="1">
       <c r="A28" s="28"/>
       <c r="B28" s="27"/>
-      <c r="C28" s="27">
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+    </row>
+    <row r="29" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A29" s="28"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+    </row>
+    <row r="30" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A30" s="28"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="28"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27">
         <f>SUM(C4:C18)</f>
         <v>-78751052</v>
       </c>
-      <c r="D28" s="27">
+      <c r="D31" s="27">
         <f>SUM(D22:D26)</f>
         <v>600000</v>
       </c>
-      <c r="E28" s="27">
+      <c r="E31" s="27">
         <f>SUM(E19:E27)</f>
-        <v>11200000</v>
+        <v>9200000</v>
       </c>
     </row>
   </sheetData>
@@ -4287,8 +4324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C59F4560-1B60-4B5E-991D-A390F0A6ECED}">
   <dimension ref="C2:J47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4436,7 +4473,7 @@
       <c r="F9" s="46"/>
       <c r="G9" s="47">
         <f>G8-G37</f>
-        <v>24528910</v>
+        <v>18988910</v>
       </c>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
@@ -4631,7 +4668,7 @@
         <v>3000000</v>
       </c>
       <c r="G20" s="27">
-        <f t="shared" ref="G20:G22" si="1">F20*E20</f>
+        <f t="shared" ref="G20:G29" si="1">F20*E20</f>
         <v>3000000</v>
       </c>
       <c r="H20" s="28" t="s">
@@ -4663,34 +4700,64 @@
     </row>
     <row r="22" spans="3:10" ht="15">
       <c r="C22" s="8"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="37"/>
+      <c r="D22" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E22" s="3">
+        <v>1</v>
+      </c>
+      <c r="F22" s="37">
+        <v>3040000</v>
+      </c>
       <c r="G22" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H22" s="28"/>
+        <v>3040000</v>
+      </c>
+      <c r="H22" s="28" t="s">
+        <v>9</v>
+      </c>
       <c r="I22" s="11"/>
       <c r="J22" s="9"/>
     </row>
     <row r="23" spans="3:10" ht="15">
       <c r="C23" s="8"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="28"/>
+      <c r="D23" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="E23" s="3">
+        <v>1</v>
+      </c>
+      <c r="F23" s="37">
+        <v>1500000</v>
+      </c>
+      <c r="G23" s="27">
+        <f t="shared" si="1"/>
+        <v>1500000</v>
+      </c>
+      <c r="H23" s="28" t="s">
+        <v>9</v>
+      </c>
       <c r="I23" s="11"/>
       <c r="J23" s="9"/>
     </row>
     <row r="24" spans="3:10" ht="15">
       <c r="C24" s="8"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="28"/>
+      <c r="D24" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="E24" s="3">
+        <v>1</v>
+      </c>
+      <c r="F24" s="37">
+        <v>1000000</v>
+      </c>
+      <c r="G24" s="27">
+        <f t="shared" si="1"/>
+        <v>1000000</v>
+      </c>
+      <c r="H24" s="28" t="s">
+        <v>9</v>
+      </c>
       <c r="I24" s="11"/>
       <c r="J24" s="9"/>
     </row>
@@ -4699,7 +4766,10 @@
       <c r="D25" s="40"/>
       <c r="E25" s="41"/>
       <c r="F25" s="42"/>
-      <c r="G25" s="42"/>
+      <c r="G25" s="27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="H25" s="43"/>
       <c r="I25" s="39"/>
       <c r="J25" s="39"/>
@@ -4709,7 +4779,10 @@
       <c r="D26" s="26"/>
       <c r="E26" s="36"/>
       <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
+      <c r="G26" s="27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="H26" s="28"/>
       <c r="I26" s="28"/>
       <c r="J26" s="15"/>
@@ -4719,7 +4792,10 @@
       <c r="D27" s="28"/>
       <c r="E27" s="36"/>
       <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
+      <c r="G27" s="27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="H27" s="28"/>
       <c r="I27" s="11"/>
       <c r="J27" s="9"/>
@@ -4729,7 +4805,10 @@
       <c r="D28" s="28"/>
       <c r="E28" s="36"/>
       <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
+      <c r="G28" s="27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="H28" s="28"/>
       <c r="I28" s="11"/>
       <c r="J28" s="9"/>
@@ -4739,7 +4818,10 @@
       <c r="D29" s="28"/>
       <c r="E29" s="36"/>
       <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
+      <c r="G29" s="27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="H29" s="28"/>
       <c r="I29" s="11"/>
       <c r="J29" s="9"/>
@@ -4821,7 +4903,7 @@
       <c r="F37" s="27"/>
       <c r="G37" s="53">
         <f>SUM(G19:G36)</f>
-        <v>13800000</v>
+        <v>19340000</v>
       </c>
       <c r="H37" s="54"/>
       <c r="I37" s="33"/>
@@ -4949,7 +5031,7 @@
       <c r="F47" s="46"/>
       <c r="G47" s="47">
         <f>G8-G17-G37</f>
-        <v>23870910</v>
+        <v>18330910</v>
       </c>
       <c r="H47" s="12"/>
       <c r="I47" s="20"/>

</xml_diff>

<commit_message>
Update finish 270 Hecquyn + 160 zeus
</commit_message>
<xml_diff>
--- a/Project/TongHopQuy2.xlsx
+++ b/Project/TongHopQuy2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ViTechSolution_LTD\04.Team_Log\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981AB656-104B-430E-86AD-B914CADE298B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6943354F-121E-4685-AC3F-81E12C7DAF1A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
     <externalReference r:id="rId13"/>
   </externalReferences>
   <definedNames>
-    <definedName name="chi_phi_cong_ty">'Chi Phí Công ty'!$G$87</definedName>
+    <definedName name="chi_phi_cong_ty">'Chi Phí Công ty'!$G$88</definedName>
     <definedName name="Pega" localSheetId="10">PEGA!$G$47</definedName>
     <definedName name="Pega">PEGA!$G$49</definedName>
     <definedName name="RowTitleRegion1..C7" localSheetId="4">#REF!</definedName>
@@ -62,12 +62,12 @@
     <definedName name="RowTitleRegion3..G26" localSheetId="2">[1]Effort_08062020!#REF!</definedName>
     <definedName name="RowTitleRegion3..G26" localSheetId="6">[1]Effort_08062020!#REF!</definedName>
     <definedName name="RowTitleRegion3..G26">[1]Effort_08062020!#REF!</definedName>
-    <definedName name="smarthome" localSheetId="8">'Chi Phí Công ty'!$G$87</definedName>
+    <definedName name="smarthome" localSheetId="8">'Chi Phí Công ty'!$G$88</definedName>
     <definedName name="smarthome">SMARTHOME!$G$32</definedName>
-    <definedName name="sport1_p1.5" localSheetId="4">'160_Zeus'!$G$48</definedName>
-    <definedName name="sport1_p1.5" localSheetId="5">'270_Hecquyn'!$G$44</definedName>
+    <definedName name="sport1_p1.5" localSheetId="4">'160_Zeus'!$G$40</definedName>
+    <definedName name="sport1_p1.5" localSheetId="5">'270_Hecquyn'!$G$26</definedName>
     <definedName name="sport1_p1.5" localSheetId="11">SoM_Dev!$G$47</definedName>
-    <definedName name="sport1_p1.5">SPORT1_P1.5!$G$59</definedName>
+    <definedName name="sport1_p1.5">SPORT1_P1.5!$G$57</definedName>
     <definedName name="sport1_p2">SPORT1_P2!$G$32</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="270">
   <si>
     <t>STT</t>
   </si>
@@ -735,9 +735,6 @@
     <t>Cọc đặt mạch hecquyn</t>
   </si>
   <si>
-    <t>Nhận tiền dự án từ tk cty</t>
-  </si>
-  <si>
     <t>ứng tiền anh thịnh vẽ mạch</t>
   </si>
   <si>
@@ -850,6 +847,51 @@
   </si>
   <si>
     <t>Tiền phí lưu kho iMX + vận chuyển</t>
+  </si>
+  <si>
+    <t>A kho</t>
+  </si>
+  <si>
+    <t>Tổng Vitech</t>
+  </si>
+  <si>
+    <t>Tổng chi</t>
+  </si>
+  <si>
+    <t>Tổng thu</t>
+  </si>
+  <si>
+    <t>10% bảo hành</t>
+  </si>
+  <si>
+    <t>Đặt Cách ly 5-5 bảo hành</t>
+  </si>
+  <si>
+    <t>Tiền 270 hecquyn + 160 zeus</t>
+  </si>
+  <si>
+    <t>Chuyển vào tk cá nhân ACB</t>
+  </si>
+  <si>
+    <t>Chuyển từ tk cty sang tk cá nhân</t>
+  </si>
+  <si>
+    <t>Nhận tiền dự án 270 hecquyn+ 160zeus từ tk cty</t>
+  </si>
+  <si>
+    <t>A Khơ ứng trước</t>
+  </si>
+  <si>
+    <t>Ăn trưa 7/11</t>
+  </si>
+  <si>
+    <t>Tuấn ứng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Còn nợ </t>
+  </si>
+  <si>
+    <t>Ngày 7/11, tài khoản cá nhân ACB Tuấn</t>
   </si>
 </sst>
 </file>
@@ -1863,7 +1905,7 @@
       </c>
       <c r="J6" s="11">
         <f>sport1_p1.5</f>
-        <v>-558000.40000000596</v>
+        <v>345299.59999999404</v>
       </c>
       <c r="K6" s="9"/>
     </row>
@@ -1912,7 +1954,7 @@
       <c r="I12" s="9"/>
       <c r="J12" s="12">
         <f>SUM(J4:J11)</f>
-        <v>-74900266.400000006</v>
+        <v>-73996966.400000006</v>
       </c>
       <c r="K12" s="13" t="s">
         <v>7</v>
@@ -1928,10 +1970,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36E1739C-0CA9-4D70-99CB-9453E6E8DAF2}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2042,6 +2084,20 @@
       </c>
       <c r="H14" s="61"/>
     </row>
+    <row r="17" spans="3:6">
+      <c r="C17" t="s">
+        <v>261</v>
+      </c>
+      <c r="D17" s="61">
+        <v>90000000</v>
+      </c>
+      <c r="E17" t="s">
+        <v>175</v>
+      </c>
+      <c r="F17" t="s">
+        <v>262</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2053,7 +2109,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2094,9 +2150,13 @@
       <c r="E2" s="23"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="24"/>
+      <c r="A3" s="24" t="s">
+        <v>263</v>
+      </c>
       <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
+      <c r="C3" s="44">
+        <v>79000000</v>
+      </c>
       <c r="D3" s="23"/>
       <c r="E3" s="23"/>
     </row>
@@ -2296,7 +2356,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="24" t="s">
-        <v>217</v>
+        <v>264</v>
       </c>
       <c r="B22" s="23"/>
       <c r="C22" s="23"/>
@@ -2307,7 +2367,7 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="24" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B23" s="23"/>
       <c r="C23" s="23"/>
@@ -2318,7 +2378,7 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="24" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B24" s="23"/>
       <c r="C24" s="23"/>
@@ -2331,7 +2391,7 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="24" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B25" s="23"/>
       <c r="C25" s="23"/>
@@ -2341,7 +2401,7 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="24" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B26" s="23"/>
       <c r="C26" s="23"/>
@@ -2352,7 +2412,7 @@
     </row>
     <row r="27" spans="1:5" ht="14.25" customHeight="1">
       <c r="A27" s="24" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B27" s="23"/>
       <c r="C27" s="23"/>
@@ -2386,8 +2446,8 @@
       <c r="A31" s="24"/>
       <c r="B31" s="23"/>
       <c r="C31" s="23">
-        <f>SUM(C4:C18)</f>
-        <v>-78751052</v>
+        <f>SUM(C3:C18)</f>
+        <v>248948</v>
       </c>
       <c r="D31" s="23">
         <f>SUM(D22:D26)</f>
@@ -2541,7 +2601,7 @@
     <row r="11" spans="3:10" ht="15">
       <c r="C11" s="8"/>
       <c r="D11" s="24" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E11" s="32">
         <v>1</v>
@@ -2562,7 +2622,7 @@
     <row r="12" spans="3:10" ht="15">
       <c r="C12" s="8"/>
       <c r="D12" s="24" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E12" s="32">
         <v>1</v>
@@ -2583,7 +2643,7 @@
     <row r="13" spans="3:10" ht="15">
       <c r="C13" s="8"/>
       <c r="D13" s="24" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E13" s="32">
         <v>1</v>
@@ -3005,7 +3065,7 @@
   <dimension ref="C2:J49"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3115,7 +3175,7 @@
       </c>
       <c r="I6" s="103"/>
       <c r="J6" s="99" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="3:10">
@@ -3179,7 +3239,7 @@
       </c>
       <c r="I10" s="103"/>
       <c r="J10" s="99" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11" spans="3:10">
@@ -3233,7 +3293,7 @@
         <v>4</v>
       </c>
       <c r="D13" s="106" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E13" s="105">
         <v>1</v>
@@ -3256,7 +3316,7 @@
         <v>5</v>
       </c>
       <c r="D14" s="157" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E14" s="159">
         <v>1</v>
@@ -3279,7 +3339,7 @@
         <v>6</v>
       </c>
       <c r="D15" s="106" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E15" s="105">
         <v>1</v>
@@ -3302,7 +3362,7 @@
         <v>7</v>
       </c>
       <c r="D16" s="106" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E16" s="105">
         <v>1</v>
@@ -3325,7 +3385,7 @@
         <v>8</v>
       </c>
       <c r="D17" s="106" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E17" s="105">
         <v>1</v>
@@ -3647,7 +3707,7 @@
         <v>23</v>
       </c>
       <c r="D31" s="99" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E31" s="105">
         <v>1</v>
@@ -3670,7 +3730,7 @@
         <v>24</v>
       </c>
       <c r="D32" s="99" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E32" s="105">
         <v>1</v>
@@ -3693,7 +3753,7 @@
         <v>25</v>
       </c>
       <c r="D33" s="99" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E33" s="105">
         <v>1</v>
@@ -3927,10 +3987,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06BE7A19-D435-4A51-A018-E212475E8992}">
-  <dimension ref="C2:M59"/>
+  <dimension ref="C2:M57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="M45" sqref="M45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4534,8 +4594,8 @@
         <v>152</v>
       </c>
       <c r="M31" s="146">
-        <f>SUM(G33:G37)+G44</f>
-        <v>4145000</v>
+        <f>SUM(G33:G35)+G42+SUM(G16:G22)+G24+G25</f>
+        <v>7264000</v>
       </c>
     </row>
     <row r="32" spans="3:13">
@@ -4564,25 +4624,25 @@
         <v>9</v>
       </c>
       <c r="M32" s="146">
-        <f>G31+G32+G39+G40+G41</f>
-        <v>1677000</v>
+        <f>G31+G32+G37+G38+G39+SUM(G10:G15)+G23</f>
+        <v>3088000</v>
       </c>
     </row>
     <row r="33" spans="3:10">
       <c r="C33" s="99">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D33" s="108" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E33" s="143">
         <v>1</v>
       </c>
       <c r="F33" s="129">
-        <v>928000</v>
+        <v>1750000</v>
       </c>
       <c r="G33" s="142">
-        <v>928000</v>
+        <v>1750000</v>
       </c>
       <c r="H33" s="140" t="s">
         <v>21</v>
@@ -4592,19 +4652,19 @@
     </row>
     <row r="34" spans="3:10">
       <c r="C34" s="99">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D34" s="108" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E34" s="143">
         <v>1</v>
       </c>
       <c r="F34" s="129">
-        <v>222000</v>
+        <v>155000</v>
       </c>
       <c r="G34" s="142">
-        <v>222000</v>
+        <v>155000</v>
       </c>
       <c r="H34" s="140" t="s">
         <v>21</v>
@@ -4612,112 +4672,114 @@
       <c r="I34" s="103"/>
       <c r="J34" s="99"/>
     </row>
-    <row r="35" spans="3:10">
+    <row r="35" spans="3:10" s="152" customFormat="1">
       <c r="C35" s="99">
-        <v>7</v>
-      </c>
-      <c r="D35" s="108" t="s">
-        <v>46</v>
-      </c>
-      <c r="E35" s="143">
-        <v>1</v>
-      </c>
-      <c r="F35" s="129">
-        <v>1750000</v>
-      </c>
-      <c r="G35" s="142">
-        <v>1750000</v>
-      </c>
-      <c r="H35" s="140" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35" s="147" t="s">
+        <v>48</v>
+      </c>
+      <c r="E35" s="148">
+        <v>1</v>
+      </c>
+      <c r="F35" s="149">
+        <v>830000</v>
+      </c>
+      <c r="G35" s="149">
+        <v>830000</v>
+      </c>
+      <c r="H35" s="150" t="s">
         <v>21</v>
       </c>
-      <c r="I35" s="103"/>
-      <c r="J35" s="99"/>
-    </row>
-    <row r="36" spans="3:10">
+      <c r="I35" s="151"/>
+      <c r="J35" s="151"/>
+    </row>
+    <row r="36" spans="3:10" ht="15">
       <c r="C36" s="99">
-        <v>8</v>
-      </c>
-      <c r="D36" s="108" t="s">
-        <v>47</v>
-      </c>
-      <c r="E36" s="143">
-        <v>1</v>
-      </c>
-      <c r="F36" s="129">
-        <v>155000</v>
+        <v>10</v>
+      </c>
+      <c r="D36" s="106" t="s">
+        <v>49</v>
+      </c>
+      <c r="E36" s="141">
+        <v>1</v>
+      </c>
+      <c r="F36" s="142">
+        <v>8606000</v>
       </c>
       <c r="G36" s="142">
-        <v>155000</v>
+        <v>8606000</v>
       </c>
       <c r="H36" s="140" t="s">
-        <v>21</v>
-      </c>
-      <c r="I36" s="103"/>
-      <c r="J36" s="99"/>
-    </row>
-    <row r="37" spans="3:10" s="152" customFormat="1">
+        <v>50</v>
+      </c>
+      <c r="I36" s="140" t="s">
+        <v>50</v>
+      </c>
+      <c r="J36" s="15"/>
+    </row>
+    <row r="37" spans="3:10">
       <c r="C37" s="99">
-        <v>9</v>
-      </c>
-      <c r="D37" s="147" t="s">
-        <v>48</v>
-      </c>
-      <c r="E37" s="148">
-        <v>1</v>
-      </c>
-      <c r="F37" s="149">
-        <v>830000</v>
-      </c>
-      <c r="G37" s="149">
-        <v>830000</v>
-      </c>
-      <c r="H37" s="150" t="s">
-        <v>21</v>
-      </c>
-      <c r="I37" s="151"/>
-      <c r="J37" s="151"/>
-    </row>
-    <row r="38" spans="3:10" ht="15">
+        <v>11</v>
+      </c>
+      <c r="D37" s="140" t="s">
+        <v>72</v>
+      </c>
+      <c r="E37" s="141">
+        <v>1</v>
+      </c>
+      <c r="F37" s="142">
+        <v>50000</v>
+      </c>
+      <c r="G37" s="142">
+        <f t="shared" ref="G37:G41" si="2">E37*F37</f>
+        <v>50000</v>
+      </c>
+      <c r="H37" s="140" t="s">
+        <v>9</v>
+      </c>
+      <c r="I37" s="103"/>
+      <c r="J37" s="99"/>
+    </row>
+    <row r="38" spans="3:10">
       <c r="C38" s="99">
-        <v>10</v>
-      </c>
-      <c r="D38" s="106" t="s">
-        <v>49</v>
+        <v>12</v>
+      </c>
+      <c r="D38" s="140" t="s">
+        <v>123</v>
       </c>
       <c r="E38" s="141">
         <v>1</v>
       </c>
       <c r="F38" s="142">
-        <v>8606000</v>
+        <v>201000</v>
       </c>
       <c r="G38" s="142">
-        <v>8606000</v>
+        <f t="shared" si="2"/>
+        <v>201000</v>
       </c>
       <c r="H38" s="140" t="s">
-        <v>50</v>
-      </c>
-      <c r="I38" s="140" t="s">
-        <v>50</v>
-      </c>
-      <c r="J38" s="15"/>
+        <v>9</v>
+      </c>
+      <c r="I38" s="103"/>
+      <c r="J38" s="99"/>
     </row>
     <row r="39" spans="3:10">
       <c r="C39" s="99">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D39" s="140" t="s">
-        <v>72</v>
+        <v>126</v>
       </c>
       <c r="E39" s="141">
         <v>1</v>
       </c>
       <c r="F39" s="142">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="G39" s="142">
-        <f t="shared" ref="G39:G43" si="2">E39*F39</f>
-        <v>50000</v>
+        <f t="shared" si="2"/>
+        <v>40000</v>
       </c>
       <c r="H39" s="140" t="s">
         <v>9</v>
@@ -4727,208 +4789,201 @@
     </row>
     <row r="40" spans="3:10">
       <c r="C40" s="99">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D40" s="140" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="E40" s="141">
         <v>1</v>
       </c>
       <c r="F40" s="142">
-        <v>201000</v>
+        <v>2014000</v>
       </c>
       <c r="G40" s="142">
         <f t="shared" si="2"/>
-        <v>201000</v>
+        <v>2014000</v>
       </c>
       <c r="H40" s="140" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="I40" s="103"/>
       <c r="J40" s="99"/>
     </row>
     <row r="41" spans="3:10">
       <c r="C41" s="99">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D41" s="140" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="E41" s="141">
-        <v>1</v>
+        <v>72</v>
       </c>
       <c r="F41" s="142">
-        <v>40000</v>
+        <v>30500</v>
       </c>
       <c r="G41" s="142">
         <f t="shared" si="2"/>
-        <v>40000</v>
-      </c>
-      <c r="H41" s="140" t="s">
-        <v>9</v>
-      </c>
+        <v>2196000</v>
+      </c>
+      <c r="H41" s="140"/>
       <c r="I41" s="103"/>
       <c r="J41" s="99"/>
     </row>
     <row r="42" spans="3:10">
       <c r="C42" s="99">
-        <v>14</v>
-      </c>
-      <c r="D42" s="140" t="s">
-        <v>129</v>
-      </c>
-      <c r="E42" s="141">
-        <v>1</v>
-      </c>
-      <c r="F42" s="142">
-        <v>2014000</v>
+        <v>17</v>
+      </c>
+      <c r="D42" s="108" t="s">
+        <v>53</v>
+      </c>
+      <c r="E42" s="143">
+        <v>1</v>
+      </c>
+      <c r="F42" s="129">
+        <v>260000</v>
       </c>
       <c r="G42" s="142">
-        <f t="shared" si="2"/>
-        <v>2014000</v>
+        <v>260000</v>
       </c>
       <c r="H42" s="140" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="I42" s="103"/>
       <c r="J42" s="99"/>
     </row>
     <row r="43" spans="3:10">
-      <c r="C43" s="99">
-        <v>16</v>
-      </c>
-      <c r="D43" s="140" t="s">
-        <v>130</v>
-      </c>
-      <c r="E43" s="141">
-        <v>72</v>
-      </c>
-      <c r="F43" s="142">
-        <v>30500</v>
+      <c r="C43" s="99"/>
+      <c r="D43" s="108" t="s">
+        <v>260</v>
+      </c>
+      <c r="E43" s="143">
+        <v>1</v>
+      </c>
+      <c r="F43" s="129">
+        <v>246700</v>
       </c>
       <c r="G43" s="142">
-        <f t="shared" si="2"/>
-        <v>2196000</v>
-      </c>
-      <c r="H43" s="140"/>
+        <f>F43*E43</f>
+        <v>246700</v>
+      </c>
+      <c r="H43" s="140" t="s">
+        <v>9</v>
+      </c>
       <c r="I43" s="103"/>
       <c r="J43" s="99"/>
     </row>
     <row r="44" spans="3:10">
-      <c r="C44" s="99">
-        <v>17</v>
-      </c>
-      <c r="D44" s="108" t="s">
-        <v>53</v>
-      </c>
-      <c r="E44" s="143">
-        <v>1</v>
-      </c>
-      <c r="F44" s="129">
-        <v>260000</v>
-      </c>
-      <c r="G44" s="142">
-        <v>260000</v>
-      </c>
-      <c r="H44" s="140" t="s">
-        <v>21</v>
-      </c>
+      <c r="C44" s="99"/>
+      <c r="D44" s="108"/>
+      <c r="E44" s="143"/>
+      <c r="F44" s="129"/>
+      <c r="G44" s="142"/>
+      <c r="H44" s="140"/>
       <c r="I44" s="103"/>
       <c r="J44" s="99"/>
     </row>
     <row r="45" spans="3:10">
       <c r="C45" s="99"/>
-      <c r="D45" s="108"/>
-      <c r="E45" s="143"/>
-      <c r="F45" s="129"/>
+      <c r="D45" s="140"/>
+      <c r="E45" s="141"/>
+      <c r="F45" s="142"/>
       <c r="G45" s="142"/>
       <c r="H45" s="140"/>
       <c r="I45" s="103"/>
-      <c r="J45" s="99"/>
-    </row>
-    <row r="46" spans="3:10">
+      <c r="J45" s="135"/>
+    </row>
+    <row r="46" spans="3:10" ht="15">
       <c r="C46" s="99"/>
-      <c r="D46" s="108"/>
-      <c r="E46" s="143"/>
-      <c r="F46" s="129"/>
-      <c r="G46" s="142"/>
-      <c r="H46" s="140"/>
-      <c r="I46" s="103"/>
-      <c r="J46" s="99"/>
-    </row>
-    <row r="47" spans="3:10">
+      <c r="D46" s="140"/>
+      <c r="E46" s="141"/>
+      <c r="F46" s="142"/>
+      <c r="G46" s="144">
+        <f>SUM(G31:G45)</f>
+        <v>17734700</v>
+      </c>
+      <c r="H46" s="145"/>
+      <c r="I46" s="124"/>
+      <c r="J46" s="27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="3:10" ht="15">
       <c r="C47" s="99"/>
       <c r="D47" s="140"/>
       <c r="E47" s="141"/>
       <c r="F47" s="142"/>
-      <c r="G47" s="142"/>
-      <c r="H47" s="140"/>
-      <c r="I47" s="103"/>
-      <c r="J47" s="135"/>
+      <c r="G47" s="153">
+        <f>G8-G46</f>
+        <v>6025299.599999994</v>
+      </c>
+      <c r="H47" s="154"/>
+      <c r="I47" s="155"/>
+      <c r="J47" s="136" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="48" spans="3:10" ht="15">
       <c r="C48" s="99"/>
-      <c r="D48" s="140"/>
-      <c r="E48" s="141"/>
-      <c r="F48" s="142"/>
-      <c r="G48" s="144">
-        <f>SUM(G31:G47)</f>
-        <v>18638000</v>
-      </c>
-      <c r="H48" s="145"/>
-      <c r="I48" s="124"/>
-      <c r="J48" s="27" t="s">
-        <v>7</v>
-      </c>
+      <c r="D48" s="165" t="s">
+        <v>26</v>
+      </c>
+      <c r="E48" s="165"/>
+      <c r="F48" s="165"/>
+      <c r="G48" s="165"/>
+      <c r="H48" s="127"/>
+      <c r="I48" s="103"/>
+      <c r="J48" s="99"/>
     </row>
     <row r="49" spans="3:10" ht="15">
-      <c r="C49" s="99"/>
-      <c r="D49" s="140"/>
-      <c r="E49" s="141"/>
-      <c r="F49" s="142"/>
-      <c r="G49" s="153">
-        <f>G8-G48</f>
-        <v>5121999.599999994</v>
-      </c>
-      <c r="H49" s="154"/>
-      <c r="I49" s="155"/>
-      <c r="J49" s="136" t="s">
-        <v>160</v>
-      </c>
+      <c r="C49" s="99">
+        <v>1</v>
+      </c>
+      <c r="D49" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" s="98"/>
+      <c r="F49" s="101"/>
+      <c r="G49" s="44"/>
+      <c r="H49" s="14"/>
+      <c r="I49" s="14"/>
+      <c r="J49" s="130"/>
     </row>
     <row r="50" spans="3:10" ht="15">
-      <c r="C50" s="99"/>
-      <c r="D50" s="165" t="s">
-        <v>26</v>
-      </c>
-      <c r="E50" s="165"/>
-      <c r="F50" s="165"/>
-      <c r="G50" s="165"/>
-      <c r="H50" s="127"/>
-      <c r="I50" s="103"/>
-      <c r="J50" s="99"/>
+      <c r="C50" s="99">
+        <v>2</v>
+      </c>
+      <c r="D50" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E50" s="98"/>
+      <c r="F50" s="101"/>
+      <c r="G50" s="44"/>
+      <c r="H50" s="14"/>
+      <c r="I50" s="14"/>
+      <c r="J50" s="130"/>
     </row>
     <row r="51" spans="3:10" ht="15">
       <c r="C51" s="99">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D51" s="15" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E51" s="98"/>
       <c r="F51" s="101"/>
       <c r="G51" s="44"/>
       <c r="H51" s="14"/>
-      <c r="I51" s="14"/>
+      <c r="I51" s="103"/>
       <c r="J51" s="130"/>
     </row>
     <row r="52" spans="3:10" ht="15">
       <c r="C52" s="99">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D52" s="15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E52" s="98"/>
       <c r="F52" s="101"/>
@@ -4938,90 +4993,62 @@
       <c r="J52" s="130"/>
     </row>
     <row r="53" spans="3:10" ht="15">
-      <c r="C53" s="99">
-        <v>3</v>
-      </c>
-      <c r="D53" s="15" t="s">
-        <v>13</v>
-      </c>
+      <c r="C53" s="99"/>
+      <c r="D53" s="15"/>
       <c r="E53" s="98"/>
       <c r="F53" s="101"/>
       <c r="G53" s="44"/>
       <c r="H53" s="14"/>
-      <c r="I53" s="103"/>
+      <c r="I53" s="14"/>
       <c r="J53" s="130"/>
     </row>
     <row r="54" spans="3:10" ht="15">
-      <c r="C54" s="99">
-        <v>4</v>
-      </c>
-      <c r="D54" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E54" s="98"/>
-      <c r="F54" s="101"/>
-      <c r="G54" s="44"/>
-      <c r="H54" s="14"/>
-      <c r="I54" s="14"/>
-      <c r="J54" s="130"/>
-    </row>
-    <row r="55" spans="3:10" ht="15">
+      <c r="C54" s="99"/>
+      <c r="D54" s="131"/>
+      <c r="E54" s="132"/>
+      <c r="F54" s="54"/>
+      <c r="G54" s="45">
+        <f>SUM(G49:G53)</f>
+        <v>0</v>
+      </c>
+      <c r="H54" s="26"/>
+      <c r="I54" s="26"/>
+      <c r="J54" s="27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="3:10">
       <c r="C55" s="99"/>
-      <c r="D55" s="15"/>
+      <c r="D55" s="99"/>
       <c r="E55" s="98"/>
       <c r="F55" s="101"/>
-      <c r="G55" s="44"/>
-      <c r="H55" s="14"/>
-      <c r="I55" s="14"/>
-      <c r="J55" s="130"/>
+      <c r="G55" s="101"/>
+      <c r="H55" s="105"/>
+      <c r="I55" s="105"/>
+      <c r="J55" s="99"/>
     </row>
     <row r="56" spans="3:10" ht="15">
       <c r="C56" s="99"/>
-      <c r="D56" s="131"/>
-      <c r="E56" s="132"/>
-      <c r="F56" s="54"/>
-      <c r="G56" s="45">
-        <f>SUM(G51:G55)</f>
-        <v>0</v>
-      </c>
-      <c r="H56" s="26"/>
-      <c r="I56" s="26"/>
-      <c r="J56" s="27" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="57" spans="3:10">
+      <c r="D56" s="15"/>
+      <c r="E56" s="98"/>
+      <c r="F56" s="101"/>
+      <c r="G56" s="135"/>
+      <c r="H56" s="99"/>
+      <c r="I56" s="99"/>
+      <c r="J56" s="99"/>
+    </row>
+    <row r="57" spans="3:10" ht="15">
       <c r="C57" s="99"/>
-      <c r="D57" s="99"/>
+      <c r="D57" s="15"/>
       <c r="E57" s="98"/>
       <c r="F57" s="101"/>
-      <c r="G57" s="101"/>
-      <c r="H57" s="105"/>
-      <c r="I57" s="105"/>
-      <c r="J57" s="99"/>
-    </row>
-    <row r="58" spans="3:10" ht="15">
-      <c r="C58" s="99"/>
-      <c r="D58" s="15"/>
-      <c r="E58" s="98"/>
-      <c r="F58" s="101"/>
-      <c r="G58" s="135"/>
-      <c r="H58" s="99"/>
-      <c r="I58" s="99"/>
-      <c r="J58" s="99"/>
-    </row>
-    <row r="59" spans="3:10" ht="15">
-      <c r="C59" s="99"/>
-      <c r="D59" s="15"/>
-      <c r="E59" s="98"/>
-      <c r="F59" s="101"/>
-      <c r="G59" s="43">
-        <f>G8-G29-G48</f>
-        <v>-558000.40000000596</v>
-      </c>
-      <c r="H59" s="12"/>
-      <c r="I59" s="12"/>
-      <c r="J59" s="136" t="s">
+      <c r="G57" s="43">
+        <f>G8-G29-G46</f>
+        <v>345299.59999999404</v>
+      </c>
+      <c r="H57" s="12"/>
+      <c r="I57" s="12"/>
+      <c r="J57" s="136" t="s">
         <v>25</v>
       </c>
     </row>
@@ -5031,7 +5058,7 @@
     <mergeCell ref="D4:G4"/>
     <mergeCell ref="D9:G9"/>
     <mergeCell ref="D30:G30"/>
-    <mergeCell ref="D50:G50"/>
+    <mergeCell ref="D48:G48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5148,10 +5175,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C59F4560-1B60-4B5E-991D-A390F0A6ECED}">
-  <dimension ref="C2:K48"/>
+  <dimension ref="C2:P40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -5165,11 +5192,12 @@
     <col min="8" max="8" width="12.85546875" style="21" customWidth="1"/>
     <col min="9" max="9" width="16.28515625" style="21" customWidth="1"/>
     <col min="10" max="10" width="33.5703125" style="5" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="5"/>
+    <col min="11" max="12" width="19.140625" style="5" customWidth="1"/>
+    <col min="13" max="16" width="11.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:11" ht="20.25">
+    <row r="2" spans="3:12" ht="20.25">
       <c r="C2" s="163" t="s">
         <v>191</v>
       </c>
@@ -5181,7 +5209,7 @@
       <c r="I2" s="163"/>
       <c r="J2" s="163"/>
     </row>
-    <row r="3" spans="3:11" ht="15.75">
+    <row r="3" spans="3:12" ht="15.75">
       <c r="C3" s="6" t="s">
         <v>0</v>
       </c>
@@ -5207,7 +5235,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="3:11" ht="15.75" customHeight="1">
+    <row r="4" spans="3:12" ht="15.75" customHeight="1">
       <c r="C4" s="7"/>
       <c r="D4" s="166" t="s">
         <v>6</v>
@@ -5219,7 +5247,7 @@
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
     </row>
-    <row r="5" spans="3:11" ht="15">
+    <row r="5" spans="3:12" ht="15">
       <c r="C5" s="8">
         <v>1</v>
       </c>
@@ -5244,7 +5272,7 @@
         <v>95822275</v>
       </c>
     </row>
-    <row r="6" spans="3:11">
+    <row r="6" spans="3:12">
       <c r="C6" s="8">
         <v>2</v>
       </c>
@@ -5254,20 +5282,24 @@
       <c r="E6" s="10">
         <v>1</v>
       </c>
-      <c r="F6" s="42"/>
+      <c r="F6" s="42">
+        <f>N20*0.5</f>
+        <v>47911120</v>
+      </c>
       <c r="G6" s="42">
         <f>F6*E6</f>
-        <v>0</v>
+        <v>47911120</v>
       </c>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
       <c r="J6" s="9"/>
       <c r="K6" s="156">
-        <f>K5-G38-G17</f>
-        <v>32452337</v>
-      </c>
-    </row>
-    <row r="7" spans="3:11">
+        <f>K5-G30-G17</f>
+        <v>36739931</v>
+      </c>
+      <c r="L6" s="156"/>
+    </row>
+    <row r="7" spans="3:12">
       <c r="C7" s="8">
         <v>3</v>
       </c>
@@ -5286,14 +5318,14 @@
       <c r="I7" s="11"/>
       <c r="J7" s="9"/>
     </row>
-    <row r="8" spans="3:11" ht="15">
+    <row r="8" spans="3:12" ht="15">
       <c r="C8" s="8"/>
       <c r="D8" s="9"/>
       <c r="E8" s="10"/>
       <c r="F8" s="42"/>
       <c r="G8" s="43">
         <f>SUM(G5:G7)</f>
-        <v>38328910</v>
+        <v>86240030</v>
       </c>
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
@@ -5301,14 +5333,14 @@
         <v>162</v>
       </c>
     </row>
-    <row r="9" spans="3:11" ht="15">
+    <row r="9" spans="3:12" ht="15">
       <c r="C9" s="8"/>
       <c r="D9" s="9"/>
       <c r="E9" s="10"/>
       <c r="F9" s="42"/>
       <c r="G9" s="43">
-        <f>G8-G38-G17</f>
-        <v>-25041028</v>
+        <f>G8-G30-G17</f>
+        <v>27157686</v>
       </c>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
@@ -5316,7 +5348,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="10" spans="3:11" ht="15">
+    <row r="10" spans="3:12" ht="15">
       <c r="C10" s="8"/>
       <c r="D10" s="166" t="s">
         <v>28</v>
@@ -5328,7 +5360,7 @@
       <c r="I10" s="14"/>
       <c r="J10" s="15"/>
     </row>
-    <row r="11" spans="3:11" ht="15">
+    <row r="11" spans="3:12" ht="15">
       <c r="C11" s="8"/>
       <c r="D11" s="24" t="s">
         <v>187</v>
@@ -5349,7 +5381,7 @@
       <c r="I11" s="11"/>
       <c r="J11" s="9"/>
     </row>
-    <row r="12" spans="3:11" ht="15">
+    <row r="12" spans="3:12" ht="15">
       <c r="C12" s="8"/>
       <c r="D12" s="24" t="s">
         <v>188</v>
@@ -5370,7 +5402,7 @@
       <c r="I12" s="11"/>
       <c r="J12" s="9"/>
     </row>
-    <row r="13" spans="3:11" ht="15">
+    <row r="13" spans="3:12" ht="15">
       <c r="C13" s="8"/>
       <c r="D13" s="24" t="s">
         <v>189</v>
@@ -5391,7 +5423,7 @@
       <c r="I13" s="11"/>
       <c r="J13" s="9"/>
     </row>
-    <row r="14" spans="3:11" ht="15">
+    <row r="14" spans="3:12" ht="15">
       <c r="C14" s="8"/>
       <c r="D14" s="24" t="s">
         <v>190</v>
@@ -5412,7 +5444,7 @@
       <c r="I14" s="11"/>
       <c r="J14" s="9"/>
     </row>
-    <row r="15" spans="3:11" ht="15">
+    <row r="15" spans="3:12" ht="15">
       <c r="C15" s="8"/>
       <c r="D15" s="24" t="s">
         <v>193</v>
@@ -5433,7 +5465,7 @@
       <c r="I15" s="11"/>
       <c r="J15" s="9"/>
     </row>
-    <row r="16" spans="3:11" ht="15">
+    <row r="16" spans="3:12" ht="15">
       <c r="C16" s="8"/>
       <c r="D16" s="24"/>
       <c r="E16" s="32"/>
@@ -5443,7 +5475,7 @@
       <c r="I16" s="11"/>
       <c r="J16" s="9"/>
     </row>
-    <row r="17" spans="3:10" ht="15">
+    <row r="17" spans="3:16" ht="15">
       <c r="C17" s="8"/>
       <c r="D17" s="24"/>
       <c r="E17" s="32"/>
@@ -5458,7 +5490,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="3:10" ht="15">
+    <row r="18" spans="3:16" ht="15">
       <c r="C18" s="8"/>
       <c r="D18" s="166" t="s">
         <v>29</v>
@@ -5470,7 +5502,7 @@
       <c r="I18" s="11"/>
       <c r="J18" s="9"/>
     </row>
-    <row r="19" spans="3:10" ht="15">
+    <row r="19" spans="3:16" ht="15">
       <c r="C19" s="8"/>
       <c r="D19" s="24" t="s">
         <v>136</v>
@@ -5490,8 +5522,26 @@
       </c>
       <c r="I19" s="11"/>
       <c r="J19" s="9"/>
-    </row>
-    <row r="20" spans="3:10" ht="15">
+      <c r="K19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="L19" s="62" t="s">
+        <v>21</v>
+      </c>
+      <c r="M19" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="N19" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="O19" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="P19" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="20" spans="3:16" ht="15">
       <c r="C20" s="8"/>
       <c r="D20" s="24" t="s">
         <v>184</v>
@@ -5503,7 +5553,7 @@
         <v>3000000</v>
       </c>
       <c r="G20" s="23">
-        <f t="shared" ref="G20:G30" si="1">F20*E20</f>
+        <f t="shared" ref="G20:G27" si="1">F20*E20</f>
         <v>3000000</v>
       </c>
       <c r="H20" s="24" t="s">
@@ -5511,11 +5561,34 @@
       </c>
       <c r="I20" s="11"/>
       <c r="J20" s="9"/>
-    </row>
-    <row r="21" spans="3:10" ht="15">
+      <c r="K20" s="156">
+        <f>SUM(G11:G15)+(G19+SUM(G22:G24)+G27)</f>
+        <v>17879344</v>
+      </c>
+      <c r="L20" s="156">
+        <f>G25+G28+G29</f>
+        <v>2403000</v>
+      </c>
+      <c r="M20" s="156">
+        <f>G20+G21+G26</f>
+        <v>38800000</v>
+      </c>
+      <c r="N20" s="156">
+        <v>95822240</v>
+      </c>
+      <c r="O20" s="156">
+        <f>M20+L20+K20</f>
+        <v>59082344</v>
+      </c>
+      <c r="P20" s="156">
+        <f>N20-O20</f>
+        <v>36739896</v>
+      </c>
+    </row>
+    <row r="21" spans="3:16" ht="15">
       <c r="C21" s="8"/>
       <c r="D21" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E21" s="3">
         <v>1</v>
@@ -5532,11 +5605,12 @@
       </c>
       <c r="I21" s="11"/>
       <c r="J21" s="9"/>
-    </row>
-    <row r="22" spans="3:10" ht="15">
+      <c r="N21" s="156"/>
+    </row>
+    <row r="22" spans="3:16" ht="28.5">
       <c r="C22" s="8"/>
       <c r="D22" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E22" s="3">
         <v>1</v>
@@ -5553,13 +5627,24 @@
       </c>
       <c r="I22" s="11"/>
       <c r="J22" s="35" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="23" spans="3:10" ht="15">
+        <v>240</v>
+      </c>
+      <c r="M22" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="N22" s="156">
+        <f>N20*0.1</f>
+        <v>9582224</v>
+      </c>
+      <c r="P22" s="156">
+        <f>P20-N22</f>
+        <v>27157672</v>
+      </c>
+    </row>
+    <row r="23" spans="3:16" ht="15">
       <c r="C23" s="8"/>
       <c r="D23" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E23" s="3">
         <v>1</v>
@@ -5577,10 +5662,10 @@
       <c r="I23" s="11"/>
       <c r="J23" s="9"/>
     </row>
-    <row r="24" spans="3:10" ht="15">
+    <row r="24" spans="3:16" ht="15">
       <c r="C24" s="8"/>
       <c r="D24" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E24" s="3">
         <v>1</v>
@@ -5597,11 +5682,12 @@
       </c>
       <c r="I24" s="11"/>
       <c r="J24" s="9"/>
-    </row>
-    <row r="25" spans="3:10" s="40" customFormat="1" ht="15">
+      <c r="P24" s="156"/>
+    </row>
+    <row r="25" spans="3:16" s="40" customFormat="1" ht="15">
       <c r="C25" s="8"/>
       <c r="D25" s="36" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E25" s="37">
         <v>1</v>
@@ -5618,13 +5704,13 @@
       </c>
       <c r="I25" s="35"/>
       <c r="J25" s="35" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="26" spans="3:10" ht="15">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="26" spans="3:16" ht="15">
       <c r="C26" s="8"/>
       <c r="D26" s="22" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E26" s="32">
         <v>1</v>
@@ -5642,10 +5728,10 @@
       <c r="I26" s="24"/>
       <c r="J26" s="15"/>
     </row>
-    <row r="27" spans="3:10" ht="30">
+    <row r="27" spans="3:16" ht="30">
       <c r="C27" s="8"/>
       <c r="D27" s="22" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E27" s="32">
         <v>1</v>
@@ -5662,257 +5748,225 @@
       </c>
       <c r="I27" s="24"/>
       <c r="J27" s="15" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="28" spans="3:10" ht="15">
-      <c r="C28" s="8"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23">
-        <v>5437594</v>
-      </c>
-      <c r="H28" s="24"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="28" spans="3:16">
+      <c r="C28" s="99">
+        <v>5</v>
+      </c>
+      <c r="D28" s="108" t="s">
+        <v>44</v>
+      </c>
+      <c r="E28" s="143">
+        <v>1</v>
+      </c>
+      <c r="F28" s="129">
+        <v>928000</v>
+      </c>
+      <c r="G28" s="142">
+        <v>928000</v>
+      </c>
+      <c r="H28" s="140" t="s">
+        <v>21</v>
+      </c>
       <c r="I28" s="11"/>
       <c r="J28" s="9"/>
     </row>
-    <row r="29" spans="3:10" ht="15">
-      <c r="C29" s="8"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H29" s="24"/>
+    <row r="29" spans="3:16">
+      <c r="C29" s="99">
+        <v>6</v>
+      </c>
+      <c r="D29" s="108" t="s">
+        <v>45</v>
+      </c>
+      <c r="E29" s="143">
+        <v>1</v>
+      </c>
+      <c r="F29" s="129">
+        <v>222000</v>
+      </c>
+      <c r="G29" s="142">
+        <v>222000</v>
+      </c>
+      <c r="H29" s="140" t="s">
+        <v>21</v>
+      </c>
       <c r="I29" s="11"/>
-      <c r="J29" s="9"/>
-    </row>
-    <row r="30" spans="3:10" ht="15">
+      <c r="J29" s="58"/>
+    </row>
+    <row r="30" spans="3:16" ht="15">
       <c r="C30" s="8"/>
       <c r="D30" s="24"/>
       <c r="E30" s="32"/>
       <c r="F30" s="23"/>
-      <c r="G30" s="23">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H30" s="24"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="9"/>
-    </row>
-    <row r="31" spans="3:10" ht="15">
+      <c r="G30" s="49">
+        <f>SUM(G19:G29)</f>
+        <v>58424344</v>
+      </c>
+      <c r="H30" s="50"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="3:16" ht="15">
       <c r="C31" s="8"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="24"/>
+      <c r="D31" s="166" t="s">
+        <v>26</v>
+      </c>
+      <c r="E31" s="166"/>
+      <c r="F31" s="166"/>
+      <c r="G31" s="166"/>
+      <c r="H31" s="51"/>
       <c r="I31" s="11"/>
-      <c r="J31" s="9"/>
-    </row>
-    <row r="32" spans="3:10" ht="15">
-      <c r="C32" s="8"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="24"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="9"/>
+      <c r="J31" s="8"/>
+    </row>
+    <row r="32" spans="3:16" ht="15">
+      <c r="C32" s="8">
+        <v>1</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="10">
+        <v>1</v>
+      </c>
+      <c r="F32" s="42">
+        <f>(P22/10)*2.5</f>
+        <v>6789418</v>
+      </c>
+      <c r="G32" s="44">
+        <f>F32</f>
+        <v>6789418</v>
+      </c>
+      <c r="H32" s="14"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="28"/>
     </row>
     <row r="33" spans="3:10" ht="15">
-      <c r="C33" s="8"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="23"/>
-      <c r="G33" s="23"/>
-      <c r="H33" s="24"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="9"/>
+      <c r="C33" s="8">
+        <v>2</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="10">
+        <v>1</v>
+      </c>
+      <c r="F33" s="42">
+        <f>(P22/10)*2.5</f>
+        <v>6789418</v>
+      </c>
+      <c r="G33" s="44">
+        <f t="shared" ref="G33:G35" si="2">F33</f>
+        <v>6789418</v>
+      </c>
+      <c r="H33" s="14"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="18"/>
     </row>
     <row r="34" spans="3:10" ht="15">
-      <c r="C34" s="8"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="33"/>
-      <c r="G34" s="23"/>
-      <c r="H34" s="24"/>
+      <c r="C34" s="8">
+        <v>3</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" s="10">
+        <v>1</v>
+      </c>
+      <c r="F34" s="42">
+        <f>(P22/10)*3</f>
+        <v>8147301.6000000006</v>
+      </c>
+      <c r="G34" s="44">
+        <f t="shared" si="2"/>
+        <v>8147301.6000000006</v>
+      </c>
+      <c r="H34" s="14"/>
       <c r="I34" s="11"/>
-      <c r="J34" s="9"/>
+      <c r="J34" s="18"/>
     </row>
     <row r="35" spans="3:10" ht="15">
-      <c r="C35" s="8"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="33"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="24"/>
-      <c r="I35" s="11"/>
-      <c r="J35" s="9"/>
+      <c r="C35" s="8">
+        <v>4</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="10">
+        <v>1</v>
+      </c>
+      <c r="F35" s="42">
+        <f>(P22/10)*2</f>
+        <v>5431534.4000000004</v>
+      </c>
+      <c r="G35" s="44">
+        <f t="shared" si="2"/>
+        <v>5431534.4000000004</v>
+      </c>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="18"/>
     </row>
     <row r="36" spans="3:10" ht="15">
       <c r="C36" s="8"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="33"/>
-      <c r="G36" s="23"/>
-      <c r="H36" s="24"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="9"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="42"/>
+      <c r="G36" s="44"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="18"/>
     </row>
     <row r="37" spans="3:10" ht="15">
       <c r="C37" s="8"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="32"/>
-      <c r="F37" s="23"/>
-      <c r="G37" s="23"/>
-      <c r="H37" s="24"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="58"/>
-    </row>
-    <row r="38" spans="3:10" ht="15">
+      <c r="D37" s="30"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="47"/>
+      <c r="G37" s="45">
+        <f>SUM(G32:G36)</f>
+        <v>27157672</v>
+      </c>
+      <c r="H37" s="26"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="3:10">
       <c r="C38" s="8"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="32"/>
-      <c r="F38" s="23"/>
-      <c r="G38" s="49">
-        <f>SUM(G19:G37)</f>
-        <v>62711938</v>
-      </c>
-      <c r="H38" s="50"/>
-      <c r="I38" s="29"/>
-      <c r="J38" s="27" t="s">
-        <v>7</v>
-      </c>
+      <c r="D38" s="8"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="42"/>
+      <c r="G38" s="42"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="8"/>
     </row>
     <row r="39" spans="3:10" ht="15">
       <c r="C39" s="8"/>
-      <c r="D39" s="166" t="s">
-        <v>26</v>
-      </c>
-      <c r="E39" s="166"/>
-      <c r="F39" s="166"/>
-      <c r="G39" s="166"/>
-      <c r="H39" s="51"/>
-      <c r="I39" s="11"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="42"/>
+      <c r="G39" s="52"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
       <c r="J39" s="8"/>
     </row>
     <row r="40" spans="3:10" ht="15">
-      <c r="C40" s="8">
-        <v>1</v>
-      </c>
-      <c r="D40" s="17" t="s">
-        <v>11</v>
-      </c>
+      <c r="C40" s="8"/>
+      <c r="D40" s="17"/>
       <c r="E40" s="10"/>
       <c r="F40" s="42"/>
-      <c r="G40" s="44"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
-      <c r="J40" s="28"/>
-    </row>
-    <row r="41" spans="3:10" ht="15">
-      <c r="C41" s="8">
-        <v>2</v>
-      </c>
-      <c r="D41" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" s="10"/>
-      <c r="F41" s="42"/>
-      <c r="G41" s="44"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="14"/>
-      <c r="J41" s="18"/>
-    </row>
-    <row r="42" spans="3:10" ht="15">
-      <c r="C42" s="8">
-        <v>3</v>
-      </c>
-      <c r="D42" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="E42" s="10"/>
-      <c r="F42" s="42"/>
-      <c r="G42" s="44"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="11"/>
-      <c r="J42" s="18"/>
-    </row>
-    <row r="43" spans="3:10" ht="15">
-      <c r="C43" s="8">
-        <v>4</v>
-      </c>
-      <c r="D43" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="E43" s="10"/>
-      <c r="F43" s="42"/>
-      <c r="G43" s="44"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="18"/>
-    </row>
-    <row r="44" spans="3:10" ht="15">
-      <c r="C44" s="8"/>
-      <c r="D44" s="17"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="42"/>
-      <c r="G44" s="44"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
-      <c r="J44" s="18"/>
-    </row>
-    <row r="45" spans="3:10" ht="15">
-      <c r="C45" s="8"/>
-      <c r="D45" s="30"/>
-      <c r="E45" s="31"/>
-      <c r="F45" s="47"/>
-      <c r="G45" s="45">
-        <f>SUM(G40:G44)</f>
-        <v>0</v>
-      </c>
-      <c r="H45" s="26"/>
-      <c r="I45" s="26"/>
-      <c r="J45" s="27" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="46" spans="3:10">
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="10"/>
-      <c r="F46" s="42"/>
-      <c r="G46" s="42"/>
-      <c r="H46" s="19"/>
-      <c r="I46" s="19"/>
-      <c r="J46" s="8"/>
-    </row>
-    <row r="47" spans="3:10" ht="15">
-      <c r="C47" s="8"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="10"/>
-      <c r="F47" s="42"/>
-      <c r="G47" s="52"/>
-      <c r="H47" s="8"/>
-      <c r="I47" s="8"/>
-      <c r="J47" s="8"/>
-    </row>
-    <row r="48" spans="3:10" ht="15">
-      <c r="C48" s="8"/>
-      <c r="D48" s="17"/>
-      <c r="E48" s="10"/>
-      <c r="F48" s="42"/>
-      <c r="G48" s="43">
-        <f>G8-G17-G38</f>
-        <v>-25041028</v>
-      </c>
-      <c r="H48" s="12"/>
-      <c r="I48" s="16"/>
-      <c r="J48" s="25" t="s">
+      <c r="G40" s="43">
+        <f>G8-G17-G30</f>
+        <v>27157686</v>
+      </c>
+      <c r="H40" s="12"/>
+      <c r="I40" s="16"/>
+      <c r="J40" s="25" t="s">
         <v>25</v>
       </c>
     </row>
@@ -5922,7 +5976,7 @@
     <mergeCell ref="D4:G4"/>
     <mergeCell ref="D10:G10"/>
     <mergeCell ref="D18:G18"/>
-    <mergeCell ref="D39:G39"/>
+    <mergeCell ref="D31:G31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5931,10 +5985,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A00FBF6-6528-4077-97A8-E7F8FA86DD30}">
-  <dimension ref="C2:K44"/>
+  <dimension ref="C2:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -5948,11 +6002,14 @@
     <col min="8" max="8" width="12.85546875" style="21" customWidth="1"/>
     <col min="9" max="9" width="16.28515625" style="21" customWidth="1"/>
     <col min="10" max="10" width="33.5703125" style="5" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="5"/>
+    <col min="11" max="12" width="14.7109375" style="5" customWidth="1"/>
+    <col min="13" max="13" width="19" style="5" customWidth="1"/>
+    <col min="14" max="15" width="12.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:11" ht="20.25">
+    <row r="2" spans="3:16" ht="20.25">
       <c r="C2" s="163" t="s">
         <v>27</v>
       </c>
@@ -5964,7 +6021,7 @@
       <c r="I2" s="163"/>
       <c r="J2" s="163"/>
     </row>
-    <row r="3" spans="3:11" ht="15.75">
+    <row r="3" spans="3:16" ht="15.75">
       <c r="C3" s="6" t="s">
         <v>0</v>
       </c>
@@ -5990,7 +6047,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="3:11" ht="15.75" customHeight="1">
+    <row r="4" spans="3:16" ht="15.75" customHeight="1">
       <c r="C4" s="7"/>
       <c r="D4" s="166" t="s">
         <v>6</v>
@@ -6002,7 +6059,7 @@
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
     </row>
-    <row r="5" spans="3:11" ht="20.25">
+    <row r="5" spans="3:16" ht="20.25">
       <c r="C5" s="7"/>
       <c r="D5" s="166" t="s">
         <v>6</v>
@@ -6014,12 +6071,12 @@
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
     </row>
-    <row r="6" spans="3:11">
+    <row r="6" spans="3:16">
       <c r="C6" s="8">
         <v>1</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E6" s="10">
         <v>1</v>
@@ -6039,7 +6096,7 @@
         <v>73236626</v>
       </c>
     </row>
-    <row r="7" spans="3:11">
+    <row r="7" spans="3:16">
       <c r="C7" s="8">
         <v>2</v>
       </c>
@@ -6049,25 +6106,28 @@
       <c r="E7" s="10">
         <v>1</v>
       </c>
-      <c r="F7" s="42"/>
+      <c r="F7" s="42">
+        <f>O12*0.5</f>
+        <v>36618345</v>
+      </c>
       <c r="G7" s="42">
         <f>F7*E7</f>
-        <v>0</v>
+        <v>36618345</v>
       </c>
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
       <c r="J7" s="9"/>
       <c r="K7" s="156">
-        <f>K6-G34</f>
+        <f>K6-G17</f>
         <v>16001226</v>
       </c>
     </row>
-    <row r="8" spans="3:11">
+    <row r="8" spans="3:16">
       <c r="C8" s="8">
         <v>3</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>159</v>
+        <v>268</v>
       </c>
       <c r="E8" s="10">
         <v>1</v>
@@ -6081,451 +6141,373 @@
       <c r="I8" s="11"/>
       <c r="J8" s="9"/>
     </row>
-    <row r="9" spans="3:11" ht="15">
+    <row r="9" spans="3:16" ht="15">
       <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="43">
-        <f>SUM(G6:G8)</f>
-        <v>29294650.399999999</v>
-      </c>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="3:11" ht="15">
+      <c r="D9" s="24"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="9"/>
+    </row>
+    <row r="10" spans="3:16" ht="15">
       <c r="C10" s="8"/>
+      <c r="D10" s="24"/>
       <c r="E10" s="32"/>
       <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="9"/>
-    </row>
-    <row r="11" spans="3:11" ht="15">
+      <c r="G10" s="43">
+        <f>SUM(G6:G8)</f>
+        <v>65912995.399999999</v>
+      </c>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="3:16" ht="15">
       <c r="C11" s="8"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="24"/>
+      <c r="D11" s="166" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="166"/>
+      <c r="F11" s="166"/>
+      <c r="G11" s="166"/>
+      <c r="H11" s="57"/>
       <c r="I11" s="11"/>
       <c r="J11" s="9"/>
-    </row>
-    <row r="12" spans="3:11" ht="15">
+      <c r="K11" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="P11" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="12" spans="3:16" ht="15">
       <c r="C12" s="8"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="49">
-        <f>SUM(G10:G10)</f>
-        <v>0</v>
-      </c>
-      <c r="H12" s="50"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="27" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="3:11" ht="15">
+      <c r="D12" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="E12" s="32">
+        <v>1</v>
+      </c>
+      <c r="F12" s="23">
+        <v>9064000</v>
+      </c>
+      <c r="G12" s="23">
+        <f>F12*E12</f>
+        <v>9064000</v>
+      </c>
+      <c r="H12" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="11"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="156">
+        <f>G12+G13</f>
+        <v>9264000</v>
+      </c>
+      <c r="L12" s="156">
+        <f>G15</f>
+        <v>26971400</v>
+      </c>
+      <c r="M12" s="156">
+        <f>G14</f>
+        <v>21000000</v>
+      </c>
+      <c r="N12" s="156">
+        <f>SUM(K12:M12)</f>
+        <v>57235400</v>
+      </c>
+      <c r="O12" s="156">
+        <v>73236690</v>
+      </c>
+      <c r="P12" s="156">
+        <f>O12-N12</f>
+        <v>16001290</v>
+      </c>
+    </row>
+    <row r="13" spans="3:16" ht="15">
       <c r="C13" s="8"/>
-      <c r="D13" s="166" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="166"/>
-      <c r="F13" s="166"/>
-      <c r="G13" s="166"/>
-      <c r="H13" s="57"/>
+      <c r="D13" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="E13" s="32">
+        <v>1</v>
+      </c>
+      <c r="F13" s="23">
+        <v>200000</v>
+      </c>
+      <c r="G13" s="23">
+        <f>F13*E13</f>
+        <v>200000</v>
+      </c>
+      <c r="H13" s="24" t="s">
+        <v>21</v>
+      </c>
       <c r="I13" s="11"/>
       <c r="J13" s="9"/>
-    </row>
-    <row r="14" spans="3:11" ht="15">
+      <c r="K13" s="156">
+        <f>G21+K12</f>
+        <v>12156540.333333334</v>
+      </c>
+      <c r="L13" s="156">
+        <f>G20+L12</f>
+        <v>29863940.333333332</v>
+      </c>
+    </row>
+    <row r="14" spans="3:16" ht="28.5">
       <c r="C14" s="8"/>
-      <c r="D14" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="E14" s="32">
-        <v>1</v>
-      </c>
-      <c r="F14" s="23">
-        <v>9064000</v>
+      <c r="D14" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+      <c r="F14" s="33">
+        <v>21000000</v>
       </c>
       <c r="G14" s="23">
-        <f>F14*E14</f>
-        <v>9064000</v>
+        <f t="shared" ref="G14" si="0">F14*E14</f>
+        <v>21000000</v>
       </c>
       <c r="H14" s="24" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="I14" s="11"/>
       <c r="J14" s="9"/>
-    </row>
-    <row r="15" spans="3:11" ht="15">
+      <c r="K14" s="85" t="s">
+        <v>265</v>
+      </c>
+      <c r="L14" s="62" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="15" spans="3:16" ht="15">
       <c r="C15" s="8"/>
-      <c r="D15" s="24" t="s">
-        <v>141</v>
-      </c>
-      <c r="E15" s="32">
-        <v>1</v>
-      </c>
-      <c r="F15" s="23">
-        <v>200000</v>
+      <c r="D15" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1</v>
+      </c>
+      <c r="F15" s="33">
+        <v>26971400</v>
       </c>
       <c r="G15" s="23">
-        <f>F15*E15</f>
-        <v>200000</v>
+        <f>E15*F15</f>
+        <v>26971400</v>
       </c>
       <c r="H15" s="24" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="I15" s="11"/>
       <c r="J15" s="9"/>
-    </row>
-    <row r="16" spans="3:11" ht="15">
+      <c r="K15" s="5">
+        <v>2000000</v>
+      </c>
+      <c r="L15" s="5">
+        <v>20000000</v>
+      </c>
+      <c r="M15" s="62" t="s">
+        <v>259</v>
+      </c>
+      <c r="O15" s="156">
+        <f>O12*0.1</f>
+        <v>7323669</v>
+      </c>
+      <c r="P15" s="156">
+        <f>P12-O15</f>
+        <v>8677621</v>
+      </c>
+    </row>
+    <row r="16" spans="3:16" ht="15">
       <c r="C16" s="8"/>
-      <c r="D16" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="E16" s="3">
-        <v>1</v>
-      </c>
-      <c r="F16" s="33">
-        <v>21000000</v>
-      </c>
-      <c r="G16" s="23">
-        <f t="shared" ref="G16" si="0">F16*E16</f>
-        <v>21000000</v>
-      </c>
-      <c r="H16" s="24" t="s">
-        <v>50</v>
-      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="24"/>
       <c r="I16" s="11"/>
       <c r="J16" s="9"/>
+      <c r="K16" s="156">
+        <f>K13-K15</f>
+        <v>10156540.333333334</v>
+      </c>
+      <c r="L16" s="156">
+        <f>L13-L15</f>
+        <v>9863940.3333333321</v>
+      </c>
     </row>
     <row r="17" spans="3:10" ht="15">
       <c r="C17" s="8"/>
-      <c r="D17" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="E17" s="3">
-        <v>1</v>
-      </c>
-      <c r="F17" s="33">
-        <v>26971400</v>
-      </c>
-      <c r="G17" s="23">
-        <f>E17*F17</f>
-        <v>26971400</v>
-      </c>
-      <c r="H17" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="I17" s="11"/>
-      <c r="J17" s="9"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="49">
+        <f>SUM(G12:G16)</f>
+        <v>57235400</v>
+      </c>
+      <c r="H17" s="50"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="27" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="18" spans="3:10" ht="15">
       <c r="C18" s="8"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="24"/>
+      <c r="D18" s="166" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="166"/>
+      <c r="F18" s="166"/>
+      <c r="G18" s="166"/>
+      <c r="H18" s="51"/>
       <c r="I18" s="11"/>
-      <c r="J18" s="9"/>
-    </row>
-    <row r="19" spans="3:10" ht="15">
-      <c r="C19" s="8"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="9"/>
-    </row>
-    <row r="20" spans="3:10" ht="15">
-      <c r="C20" s="8"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="9"/>
-    </row>
-    <row r="21" spans="3:10" ht="15">
-      <c r="C21" s="8"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="24"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="9"/>
-    </row>
-    <row r="22" spans="3:10" s="40" customFormat="1" ht="15">
+      <c r="J18" s="8"/>
+    </row>
+    <row r="19" spans="3:10" ht="45">
+      <c r="C19" s="8">
+        <v>1</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="10">
+        <v>1</v>
+      </c>
+      <c r="F19" s="42">
+        <f>(P15/3)</f>
+        <v>2892540.3333333335</v>
+      </c>
+      <c r="G19" s="44">
+        <f>F19</f>
+        <v>2892540.3333333335</v>
+      </c>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="J19" s="28"/>
+    </row>
+    <row r="20" spans="3:10" ht="45">
+      <c r="C20" s="8">
+        <v>2</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="10">
+        <v>1</v>
+      </c>
+      <c r="F20" s="42">
+        <f>P15/3</f>
+        <v>2892540.3333333335</v>
+      </c>
+      <c r="G20" s="44">
+        <f t="shared" ref="G20:G21" si="1">F20</f>
+        <v>2892540.3333333335</v>
+      </c>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="J20" s="18"/>
+    </row>
+    <row r="21" spans="3:10" ht="45">
+      <c r="C21" s="8">
+        <v>4</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="10">
+        <v>1</v>
+      </c>
+      <c r="F21" s="42">
+        <f>P15/3</f>
+        <v>2892540.3333333335</v>
+      </c>
+      <c r="G21" s="44">
+        <f t="shared" si="1"/>
+        <v>2892540.3333333335</v>
+      </c>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="J21" s="18"/>
+    </row>
+    <row r="22" spans="3:10" ht="15">
       <c r="C22" s="8"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="35"/>
-      <c r="J22" s="35"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="18"/>
     </row>
     <row r="23" spans="3:10" ht="15">
       <c r="C23" s="8"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="24"/>
-      <c r="I23" s="24"/>
-      <c r="J23" s="15"/>
-    </row>
-    <row r="24" spans="3:10" ht="15">
+      <c r="D23" s="30"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="45">
+        <f>SUM(G19:G22)</f>
+        <v>8677621</v>
+      </c>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="3:10">
       <c r="C24" s="8"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="9"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="8"/>
     </row>
     <row r="25" spans="3:10" ht="15">
       <c r="C25" s="8"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="9"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="52"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
     </row>
     <row r="26" spans="3:10" ht="15">
       <c r="C26" s="8"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="9"/>
-    </row>
-    <row r="27" spans="3:10" ht="15">
-      <c r="C27" s="8"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="9"/>
-    </row>
-    <row r="28" spans="3:10" ht="15">
-      <c r="C28" s="8"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="9"/>
-    </row>
-    <row r="29" spans="3:10" ht="15">
-      <c r="C29" s="8"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="24"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="9"/>
-    </row>
-    <row r="30" spans="3:10" ht="15">
-      <c r="C30" s="8"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="9"/>
-    </row>
-    <row r="31" spans="3:10" ht="15">
-      <c r="C31" s="8"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="9"/>
-    </row>
-    <row r="32" spans="3:10" ht="15">
-      <c r="C32" s="8"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="33"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="24"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="9"/>
-    </row>
-    <row r="33" spans="3:10" ht="15">
-      <c r="C33" s="8"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="23"/>
-      <c r="G33" s="23"/>
-      <c r="H33" s="24"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="58"/>
-    </row>
-    <row r="34" spans="3:10" ht="15">
-      <c r="C34" s="8"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="32"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="49">
-        <f>SUM(G14:G33)</f>
-        <v>57235400</v>
-      </c>
-      <c r="H34" s="50"/>
-      <c r="I34" s="29"/>
-      <c r="J34" s="27" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="3:10" ht="15">
-      <c r="C35" s="8"/>
-      <c r="D35" s="166" t="s">
-        <v>26</v>
-      </c>
-      <c r="E35" s="166"/>
-      <c r="F35" s="166"/>
-      <c r="G35" s="166"/>
-      <c r="H35" s="51"/>
-      <c r="I35" s="11"/>
-      <c r="J35" s="8"/>
-    </row>
-    <row r="36" spans="3:10" ht="15">
-      <c r="C36" s="8">
-        <v>1</v>
-      </c>
-      <c r="D36" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="E36" s="10"/>
-      <c r="F36" s="42"/>
-      <c r="G36" s="44"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="28"/>
-    </row>
-    <row r="37" spans="3:10" ht="15">
-      <c r="C37" s="8">
-        <v>2</v>
-      </c>
-      <c r="D37" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="E37" s="10"/>
-      <c r="F37" s="42"/>
-      <c r="G37" s="44"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="18"/>
-    </row>
-    <row r="38" spans="3:10" ht="15">
-      <c r="C38" s="8">
-        <v>3</v>
-      </c>
-      <c r="D38" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="E38" s="10"/>
-      <c r="F38" s="42"/>
-      <c r="G38" s="44"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="11"/>
-      <c r="J38" s="18"/>
-    </row>
-    <row r="39" spans="3:10" ht="15">
-      <c r="C39" s="8">
-        <v>4</v>
-      </c>
-      <c r="D39" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="E39" s="10"/>
-      <c r="F39" s="42"/>
-      <c r="G39" s="44"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="14"/>
-      <c r="J39" s="18"/>
-    </row>
-    <row r="40" spans="3:10" ht="15">
-      <c r="C40" s="8"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="42"/>
-      <c r="G40" s="44"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
-      <c r="J40" s="18"/>
-    </row>
-    <row r="41" spans="3:10" ht="15">
-      <c r="C41" s="8"/>
-      <c r="D41" s="30"/>
-      <c r="E41" s="31"/>
-      <c r="F41" s="47"/>
-      <c r="G41" s="45">
-        <f>SUM(G36:G40)</f>
-        <v>0</v>
-      </c>
-      <c r="H41" s="26"/>
-      <c r="I41" s="26"/>
-      <c r="J41" s="27" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="3:10">
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="42"/>
-      <c r="G42" s="42"/>
-      <c r="H42" s="19"/>
-      <c r="I42" s="19"/>
-      <c r="J42" s="8"/>
-    </row>
-    <row r="43" spans="3:10" ht="15">
-      <c r="C43" s="8"/>
-      <c r="D43" s="17"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="42"/>
-      <c r="G43" s="52"/>
-      <c r="H43" s="8"/>
-      <c r="I43" s="8"/>
-      <c r="J43" s="8"/>
-    </row>
-    <row r="44" spans="3:10" ht="15">
-      <c r="C44" s="8"/>
-      <c r="D44" s="17"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="42"/>
-      <c r="G44" s="43">
-        <f>G8-G12-G34</f>
-        <v>-57235400</v>
-      </c>
-      <c r="H44" s="12"/>
-      <c r="I44" s="16"/>
-      <c r="J44" s="25" t="s">
+      <c r="D26" s="17"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="43">
+        <f>G10-G17-G23</f>
+        <v>-25.600000001490116</v>
+      </c>
+      <c r="H26" s="12"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="25" t="s">
         <v>25</v>
       </c>
     </row>
@@ -6533,8 +6515,8 @@
   <mergeCells count="5">
     <mergeCell ref="C2:J2"/>
     <mergeCell ref="D4:G4"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="D35:G35"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D18:G18"/>
     <mergeCell ref="D5:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6856,7 +6838,7 @@
     <row r="18" spans="3:10" ht="15">
       <c r="C18" s="8"/>
       <c r="D18" s="24" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E18" s="32">
         <v>1</v>
@@ -7080,7 +7062,7 @@
   <dimension ref="C2:J32"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -7555,10 +7537,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73990C79-75DF-434D-B272-2581D279AD79}">
-  <dimension ref="C2:J87"/>
+  <dimension ref="C2:M88"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H60" sqref="H60"/>
+    <sheetView topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H61" sqref="H61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -7572,7 +7554,9 @@
     <col min="8" max="8" width="12.85546875" style="139" customWidth="1"/>
     <col min="9" max="9" width="16.28515625" style="139" customWidth="1"/>
     <col min="10" max="10" width="33.5703125" style="111" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="111"/>
+    <col min="11" max="11" width="9.140625" style="111"/>
+    <col min="12" max="13" width="11.5703125" style="111" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="111"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:10" ht="20.25">
@@ -7850,7 +7834,7 @@
     <row r="17" spans="3:10" ht="15">
       <c r="C17" s="99"/>
       <c r="D17" s="116" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E17" s="117">
         <v>1</v>
@@ -7871,7 +7855,7 @@
     <row r="18" spans="3:10" ht="15">
       <c r="C18" s="99"/>
       <c r="D18" s="116" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E18" s="117">
         <v>1</v>
@@ -7892,7 +7876,7 @@
     <row r="19" spans="3:10" ht="15">
       <c r="C19" s="99"/>
       <c r="D19" s="116" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E19" s="117">
         <v>1</v>
@@ -7984,7 +7968,7 @@
         <v>120000</v>
       </c>
       <c r="G24" s="118">
-        <f t="shared" ref="G24:G59" si="1">E24*F24</f>
+        <f t="shared" ref="G24:G60" si="1">E24*F24</f>
         <v>120000</v>
       </c>
       <c r="H24" s="116" t="s">
@@ -8260,7 +8244,7 @@
         <v>120000</v>
       </c>
       <c r="G36" s="118">
-        <f t="shared" si="1"/>
+        <f>E36*F36</f>
         <v>120000</v>
       </c>
       <c r="H36" s="116" t="s">
@@ -8537,7 +8521,7 @@
       <c r="I48" s="99"/>
       <c r="J48" s="99"/>
     </row>
-    <row r="49" spans="3:10" ht="15">
+    <row r="49" spans="3:13" ht="15">
       <c r="C49" s="99"/>
       <c r="D49" s="116" t="s">
         <v>143</v>
@@ -8558,7 +8542,7 @@
       <c r="I49" s="99"/>
       <c r="J49" s="99"/>
     </row>
-    <row r="50" spans="3:10" ht="15">
+    <row r="50" spans="3:13" ht="15">
       <c r="C50" s="99"/>
       <c r="D50" s="116" t="s">
         <v>145</v>
@@ -8579,7 +8563,7 @@
       <c r="I50" s="99"/>
       <c r="J50" s="99"/>
     </row>
-    <row r="51" spans="3:10" ht="15">
+    <row r="51" spans="3:13" ht="15">
       <c r="C51" s="99"/>
       <c r="D51" s="116" t="s">
         <v>177</v>
@@ -8600,7 +8584,7 @@
       <c r="I51" s="99"/>
       <c r="J51" s="99"/>
     </row>
-    <row r="52" spans="3:10" ht="15">
+    <row r="52" spans="3:13" ht="15">
       <c r="C52" s="99"/>
       <c r="D52" s="116" t="s">
         <v>178</v>
@@ -8621,7 +8605,7 @@
       <c r="I52" s="99"/>
       <c r="J52" s="99"/>
     </row>
-    <row r="53" spans="3:10" ht="15">
+    <row r="53" spans="3:13" ht="15">
       <c r="C53" s="99"/>
       <c r="D53" s="116" t="s">
         <v>185</v>
@@ -8642,7 +8626,7 @@
       <c r="I53" s="99"/>
       <c r="J53" s="99"/>
     </row>
-    <row r="54" spans="3:10" ht="15">
+    <row r="54" spans="3:13" ht="15">
       <c r="C54" s="99"/>
       <c r="D54" s="116" t="s">
         <v>186</v>
@@ -8663,7 +8647,7 @@
       <c r="I54" s="99"/>
       <c r="J54" s="99"/>
     </row>
-    <row r="55" spans="3:10" ht="15">
+    <row r="55" spans="3:13" ht="15">
       <c r="C55" s="99"/>
       <c r="D55" s="116" t="s">
         <v>194</v>
@@ -8684,10 +8668,10 @@
       <c r="I55" s="99"/>
       <c r="J55" s="99"/>
     </row>
-    <row r="56" spans="3:10" ht="15">
+    <row r="56" spans="3:13" ht="15">
       <c r="C56" s="99"/>
       <c r="D56" s="116" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E56" s="119">
         <v>1</v>
@@ -8705,10 +8689,10 @@
       <c r="I56" s="99"/>
       <c r="J56" s="99"/>
     </row>
-    <row r="57" spans="3:10" ht="15">
+    <row r="57" spans="3:13" ht="15">
       <c r="C57" s="99"/>
       <c r="D57" s="116" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E57" s="119">
         <v>1</v>
@@ -8726,10 +8710,10 @@
       <c r="I57" s="99"/>
       <c r="J57" s="99"/>
     </row>
-    <row r="58" spans="3:10" ht="15">
+    <row r="58" spans="3:13" ht="15">
       <c r="C58" s="99"/>
       <c r="D58" s="116" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E58" s="119">
         <v>1</v>
@@ -8747,10 +8731,10 @@
       <c r="I58" s="99"/>
       <c r="J58" s="99"/>
     </row>
-    <row r="59" spans="3:10" ht="15">
+    <row r="59" spans="3:13" ht="15">
       <c r="C59" s="99"/>
       <c r="D59" s="116" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E59" s="119">
         <v>1</v>
@@ -8767,73 +8751,85 @@
       </c>
       <c r="I59" s="99"/>
       <c r="J59" s="99"/>
-    </row>
-    <row r="60" spans="3:10" ht="15">
+      <c r="L59" s="111" t="s">
+        <v>9</v>
+      </c>
+      <c r="M59" s="111" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="60" spans="3:13" ht="15">
       <c r="C60" s="99"/>
-      <c r="D60" s="116"/>
-      <c r="E60" s="117"/>
-      <c r="F60" s="118"/>
-      <c r="G60" s="122">
+      <c r="D60" s="116" t="s">
+        <v>266</v>
+      </c>
+      <c r="E60" s="119">
+        <v>1</v>
+      </c>
+      <c r="F60" s="118">
+        <v>77000</v>
+      </c>
+      <c r="G60" s="118">
+        <f t="shared" si="1"/>
+        <v>77000</v>
+      </c>
+      <c r="H60" s="99" t="s">
+        <v>21</v>
+      </c>
+      <c r="I60" s="99"/>
+      <c r="J60" s="99"/>
+    </row>
+    <row r="61" spans="3:13" ht="15">
+      <c r="C61" s="99"/>
+      <c r="D61" s="116"/>
+      <c r="E61" s="117"/>
+      <c r="F61" s="118"/>
+      <c r="G61" s="122">
         <f>SUM(G23:G56)</f>
         <v>4818000</v>
       </c>
-      <c r="H60" s="123"/>
-      <c r="I60" s="124"/>
-      <c r="J60" s="27" t="s">
+      <c r="H61" s="123"/>
+      <c r="I61" s="124"/>
+      <c r="J61" s="27" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="61" spans="3:10" ht="15">
-      <c r="C61" s="99"/>
-      <c r="D61" s="165" t="s">
+      <c r="L61" s="146">
+        <f>G21+SUM(G23:G38)+SUM(G43:G58)+G65+G71</f>
+        <v>17167000</v>
+      </c>
+      <c r="M61" s="146">
+        <f>SUM(G39:G42)+G59+G66+G63+G64+SUM(G72:G78)+G83</f>
+        <v>22283700</v>
+      </c>
+    </row>
+    <row r="62" spans="3:13" ht="15">
+      <c r="C62" s="99"/>
+      <c r="D62" s="165" t="s">
         <v>104</v>
       </c>
-      <c r="E61" s="165"/>
-      <c r="F61" s="165"/>
-      <c r="G61" s="165"/>
-      <c r="H61" s="127"/>
-      <c r="I61" s="103"/>
-      <c r="J61" s="99"/>
-    </row>
-    <row r="62" spans="3:10" ht="15">
-      <c r="C62" s="99">
-        <v>1</v>
-      </c>
-      <c r="D62" s="128" t="s">
+      <c r="E62" s="165"/>
+      <c r="F62" s="165"/>
+      <c r="G62" s="165"/>
+      <c r="H62" s="127"/>
+      <c r="I62" s="103"/>
+      <c r="J62" s="99"/>
+    </row>
+    <row r="63" spans="3:13" ht="15">
+      <c r="C63" s="99">
+        <v>1</v>
+      </c>
+      <c r="D63" s="128" t="s">
         <v>105</v>
       </c>
-      <c r="E62" s="119">
-        <v>1</v>
-      </c>
-      <c r="F62" s="120">
+      <c r="E63" s="119">
+        <v>1</v>
+      </c>
+      <c r="F63" s="120">
         <v>1800000</v>
-      </c>
-      <c r="G62" s="129">
-        <f>F62*E62</f>
-        <v>1800000</v>
-      </c>
-      <c r="H62" s="116" t="s">
-        <v>21</v>
-      </c>
-      <c r="I62" s="14"/>
-      <c r="J62" s="130"/>
-    </row>
-    <row r="63" spans="3:10" ht="15">
-      <c r="C63" s="99">
-        <v>2</v>
-      </c>
-      <c r="D63" s="128" t="s">
-        <v>106</v>
-      </c>
-      <c r="E63" s="119">
-        <v>1</v>
-      </c>
-      <c r="F63" s="120">
-        <v>5000000</v>
       </c>
       <c r="G63" s="129">
         <f>F63*E63</f>
-        <v>5000000</v>
+        <v>1800000</v>
       </c>
       <c r="H63" s="116" t="s">
         <v>21</v>
@@ -8841,201 +8837,203 @@
       <c r="I63" s="14"/>
       <c r="J63" s="130"/>
     </row>
-    <row r="64" spans="3:10" ht="15">
+    <row r="64" spans="3:13" ht="15">
       <c r="C64" s="99">
-        <v>3</v>
-      </c>
-      <c r="D64" s="116" t="s">
-        <v>107</v>
-      </c>
-      <c r="E64" s="116">
-        <v>1</v>
-      </c>
-      <c r="F64" s="118">
-        <v>2590000</v>
+        <v>2</v>
+      </c>
+      <c r="D64" s="128" t="s">
+        <v>106</v>
+      </c>
+      <c r="E64" s="119">
+        <v>1</v>
+      </c>
+      <c r="F64" s="120">
+        <v>5000000</v>
       </c>
       <c r="G64" s="129">
         <f>F64*E64</f>
+        <v>5000000</v>
+      </c>
+      <c r="H64" s="116" t="s">
+        <v>21</v>
+      </c>
+      <c r="I64" s="14"/>
+      <c r="J64" s="130"/>
+    </row>
+    <row r="65" spans="3:10" ht="15">
+      <c r="C65" s="99">
+        <v>3</v>
+      </c>
+      <c r="D65" s="116" t="s">
+        <v>107</v>
+      </c>
+      <c r="E65" s="116">
+        <v>1</v>
+      </c>
+      <c r="F65" s="118">
         <v>2590000</v>
-      </c>
-      <c r="H64" s="116" t="s">
-        <v>9</v>
-      </c>
-      <c r="I64" s="103"/>
-      <c r="J64" s="130"/>
-    </row>
-    <row r="65" spans="3:10" ht="15">
-      <c r="C65" s="99"/>
-      <c r="D65" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="E65" s="98">
-        <v>1</v>
-      </c>
-      <c r="F65" s="101">
-        <v>410000</v>
       </c>
       <c r="G65" s="129">
         <f>F65*E65</f>
-        <v>410000</v>
-      </c>
-      <c r="H65" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="I65" s="14"/>
+        <v>2590000</v>
+      </c>
+      <c r="H65" s="116" t="s">
+        <v>9</v>
+      </c>
+      <c r="I65" s="103"/>
       <c r="J65" s="130"/>
     </row>
     <row r="66" spans="3:10" ht="15">
       <c r="C66" s="99"/>
-      <c r="D66" s="15"/>
-      <c r="E66" s="98"/>
-      <c r="F66" s="101"/>
-      <c r="G66" s="44"/>
-      <c r="H66" s="14"/>
+      <c r="D66" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="E66" s="98">
+        <v>1</v>
+      </c>
+      <c r="F66" s="101">
+        <v>410000</v>
+      </c>
+      <c r="G66" s="129">
+        <f>F66*E66</f>
+        <v>410000</v>
+      </c>
+      <c r="H66" s="14" t="s">
+        <v>21</v>
+      </c>
       <c r="I66" s="14"/>
       <c r="J66" s="130"/>
     </row>
     <row r="67" spans="3:10" ht="15">
       <c r="C67" s="99"/>
-      <c r="D67" s="131"/>
-      <c r="E67" s="132"/>
-      <c r="F67" s="54"/>
-      <c r="G67" s="45">
-        <f>SUM(G62:G65)</f>
+      <c r="D67" s="15"/>
+      <c r="E67" s="98"/>
+      <c r="F67" s="101"/>
+      <c r="G67" s="44"/>
+      <c r="H67" s="14"/>
+      <c r="I67" s="14"/>
+      <c r="J67" s="130"/>
+    </row>
+    <row r="68" spans="3:10" ht="15">
+      <c r="C68" s="99"/>
+      <c r="D68" s="131"/>
+      <c r="E68" s="132"/>
+      <c r="F68" s="54"/>
+      <c r="G68" s="45">
+        <f>SUM(G63:G66)</f>
         <v>9800000</v>
       </c>
-      <c r="H67" s="26"/>
-      <c r="I67" s="26"/>
-      <c r="J67" s="27" t="s">
+      <c r="H68" s="26"/>
+      <c r="I68" s="26"/>
+      <c r="J68" s="27" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="3:10">
-      <c r="C68" s="99"/>
-      <c r="D68" s="99"/>
-      <c r="E68" s="98"/>
-      <c r="F68" s="101"/>
-      <c r="G68" s="101"/>
-      <c r="H68" s="105"/>
-      <c r="I68" s="105"/>
-      <c r="J68" s="99"/>
-    </row>
-    <row r="69" spans="3:10" ht="15">
+    <row r="69" spans="3:10">
       <c r="C69" s="99"/>
-      <c r="D69" s="165" t="s">
+      <c r="D69" s="99"/>
+      <c r="E69" s="98"/>
+      <c r="F69" s="101"/>
+      <c r="G69" s="101"/>
+      <c r="H69" s="105"/>
+      <c r="I69" s="105"/>
+      <c r="J69" s="99"/>
+    </row>
+    <row r="70" spans="3:10" ht="15">
+      <c r="C70" s="99"/>
+      <c r="D70" s="165" t="s">
         <v>108</v>
       </c>
-      <c r="E69" s="165"/>
-      <c r="F69" s="165"/>
-      <c r="G69" s="165"/>
-      <c r="H69" s="127"/>
-      <c r="I69" s="103"/>
-      <c r="J69" s="99"/>
-    </row>
-    <row r="70" spans="3:10" ht="15">
-      <c r="C70" s="99">
-        <v>1</v>
-      </c>
-      <c r="D70" s="116" t="s">
-        <v>109</v>
-      </c>
-      <c r="E70" s="119">
-        <v>1</v>
-      </c>
-      <c r="F70" s="118">
-        <v>2000000</v>
-      </c>
-      <c r="G70" s="129">
-        <f>F70*E70</f>
-        <v>2000000</v>
-      </c>
-      <c r="H70" s="133" t="s">
-        <v>9</v>
-      </c>
-      <c r="I70" s="14"/>
-      <c r="J70" s="130"/>
+      <c r="E70" s="165"/>
+      <c r="F70" s="165"/>
+      <c r="G70" s="165"/>
+      <c r="H70" s="127"/>
+      <c r="I70" s="103"/>
+      <c r="J70" s="99"/>
     </row>
     <row r="71" spans="3:10" ht="15">
       <c r="C71" s="99">
-        <v>2</v>
-      </c>
-      <c r="D71" s="108" t="s">
-        <v>110</v>
+        <v>1</v>
+      </c>
+      <c r="D71" s="116" t="s">
+        <v>109</v>
       </c>
       <c r="E71" s="119">
         <v>1</v>
       </c>
-      <c r="F71" s="120">
-        <v>250000</v>
+      <c r="F71" s="118">
+        <v>2000000</v>
       </c>
       <c r="G71" s="129">
-        <f t="shared" ref="G71:G77" si="2">F71*E71</f>
-        <v>250000</v>
-      </c>
-      <c r="H71" s="134" t="s">
-        <v>114</v>
+        <f>F71*E71</f>
+        <v>2000000</v>
+      </c>
+      <c r="H71" s="133" t="s">
+        <v>9</v>
       </c>
       <c r="I71" s="14"/>
       <c r="J71" s="130"/>
     </row>
     <row r="72" spans="3:10" ht="15">
       <c r="C72" s="99">
+        <v>2</v>
+      </c>
+      <c r="D72" s="108" t="s">
+        <v>110</v>
+      </c>
+      <c r="E72" s="119">
+        <v>1</v>
+      </c>
+      <c r="F72" s="120">
+        <v>250000</v>
+      </c>
+      <c r="G72" s="129">
+        <f t="shared" ref="G72:G78" si="2">F72*E72</f>
+        <v>250000</v>
+      </c>
+      <c r="H72" s="134" t="s">
+        <v>114</v>
+      </c>
+      <c r="I72" s="14"/>
+      <c r="J72" s="130"/>
+    </row>
+    <row r="73" spans="3:10" ht="15">
+      <c r="C73" s="99">
         <v>3</v>
       </c>
-      <c r="D72" s="128" t="s">
+      <c r="D73" s="128" t="s">
         <v>111</v>
       </c>
-      <c r="E72" s="116">
-        <v>1</v>
-      </c>
-      <c r="F72" s="120">
+      <c r="E73" s="116">
+        <v>1</v>
+      </c>
+      <c r="F73" s="120">
         <v>1000000</v>
       </c>
-      <c r="G72" s="129">
+      <c r="G73" s="129">
         <f t="shared" si="2"/>
         <v>1000000</v>
       </c>
-      <c r="H72" s="134" t="s">
-        <v>114</v>
-      </c>
-      <c r="I72" s="103"/>
-      <c r="J72" s="130"/>
-    </row>
-    <row r="73" spans="3:10" ht="15">
-      <c r="C73" s="99"/>
-      <c r="D73" s="128" t="s">
-        <v>112</v>
-      </c>
-      <c r="E73" s="116">
-        <v>1</v>
-      </c>
-      <c r="F73" s="120">
-        <v>1880000</v>
-      </c>
-      <c r="G73" s="129">
-        <f t="shared" si="2"/>
-        <v>1880000</v>
-      </c>
       <c r="H73" s="134" t="s">
         <v>114</v>
       </c>
-      <c r="I73" s="14"/>
+      <c r="I73" s="103"/>
       <c r="J73" s="130"/>
     </row>
     <row r="74" spans="3:10" ht="15">
       <c r="C74" s="99"/>
       <c r="D74" s="128" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E74" s="116">
         <v>1</v>
       </c>
       <c r="F74" s="120">
-        <v>1200000</v>
+        <v>1880000</v>
       </c>
       <c r="G74" s="129">
         <f t="shared" si="2"/>
-        <v>1200000</v>
+        <v>1880000</v>
       </c>
       <c r="H74" s="134" t="s">
         <v>114</v>
@@ -9046,209 +9044,230 @@
     <row r="75" spans="3:10" ht="15">
       <c r="C75" s="99"/>
       <c r="D75" s="128" t="s">
-        <v>165</v>
+        <v>113</v>
       </c>
       <c r="E75" s="116">
         <v>1</v>
       </c>
       <c r="F75" s="120">
-        <v>326700</v>
+        <v>1200000</v>
       </c>
       <c r="G75" s="129">
         <f t="shared" si="2"/>
-        <v>326700</v>
-      </c>
-      <c r="H75" s="14" t="s">
+        <v>1200000</v>
+      </c>
+      <c r="H75" s="134" t="s">
         <v>114</v>
       </c>
       <c r="I75" s="14"/>
-      <c r="J75" s="130" t="s">
-        <v>240</v>
-      </c>
+      <c r="J75" s="130"/>
     </row>
     <row r="76" spans="3:10" ht="15">
       <c r="C76" s="99"/>
       <c r="D76" s="128" t="s">
-        <v>238</v>
+        <v>165</v>
       </c>
       <c r="E76" s="116">
         <v>1</v>
       </c>
       <c r="F76" s="120">
-        <v>1452000</v>
+        <v>326700</v>
       </c>
       <c r="G76" s="129">
         <f t="shared" si="2"/>
-        <v>1452000</v>
+        <v>326700</v>
       </c>
       <c r="H76" s="14" t="s">
         <v>114</v>
       </c>
       <c r="I76" s="14"/>
       <c r="J76" s="130" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="77" spans="3:10" ht="15">
       <c r="C77" s="99"/>
       <c r="D77" s="128" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E77" s="116">
         <v>1</v>
       </c>
       <c r="F77" s="120">
-        <v>560000</v>
+        <v>1452000</v>
       </c>
       <c r="G77" s="129">
         <f t="shared" si="2"/>
-        <v>560000</v>
+        <v>1452000</v>
       </c>
       <c r="H77" s="14" t="s">
         <v>114</v>
       </c>
       <c r="I77" s="14"/>
       <c r="J77" s="130" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="78" spans="3:10" ht="15">
       <c r="C78" s="99"/>
-      <c r="D78" s="128"/>
-      <c r="E78" s="116"/>
-      <c r="F78" s="120"/>
-      <c r="G78" s="129"/>
-      <c r="H78" s="14"/>
+      <c r="D78" s="128" t="s">
+        <v>238</v>
+      </c>
+      <c r="E78" s="116">
+        <v>1</v>
+      </c>
+      <c r="F78" s="120">
+        <v>560000</v>
+      </c>
+      <c r="G78" s="129">
+        <f t="shared" si="2"/>
+        <v>560000</v>
+      </c>
+      <c r="H78" s="14" t="s">
+        <v>114</v>
+      </c>
       <c r="I78" s="14"/>
-      <c r="J78" s="130"/>
+      <c r="J78" s="130" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="79" spans="3:10" ht="15">
       <c r="C79" s="99"/>
-      <c r="D79" s="131"/>
-      <c r="E79" s="132"/>
-      <c r="F79" s="54"/>
-      <c r="G79" s="45">
-        <f>SUM(G70:G77)</f>
-        <v>8668700</v>
-      </c>
-      <c r="H79" s="26"/>
-      <c r="I79" s="26"/>
-      <c r="J79" s="27" t="s">
-        <v>7</v>
-      </c>
+      <c r="D79" s="128"/>
+      <c r="E79" s="116"/>
+      <c r="F79" s="120"/>
+      <c r="G79" s="129"/>
+      <c r="H79" s="14"/>
+      <c r="I79" s="14"/>
+      <c r="J79" s="130"/>
     </row>
     <row r="80" spans="3:10" ht="15">
       <c r="C80" s="99"/>
       <c r="D80" s="131"/>
       <c r="E80" s="132"/>
       <c r="F80" s="54"/>
-      <c r="G80" s="54"/>
-      <c r="H80" s="55"/>
-      <c r="I80" s="55"/>
-      <c r="J80" s="56"/>
+      <c r="G80" s="45">
+        <f>SUM(G71:G78)</f>
+        <v>8668700</v>
+      </c>
+      <c r="H80" s="26"/>
+      <c r="I80" s="26"/>
+      <c r="J80" s="27" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="81" spans="3:10" ht="15">
       <c r="C81" s="99"/>
-      <c r="D81" s="165" t="s">
-        <v>115</v>
-      </c>
-      <c r="E81" s="165"/>
-      <c r="F81" s="165"/>
-      <c r="G81" s="165"/>
-      <c r="H81" s="127"/>
-      <c r="I81" s="103"/>
-      <c r="J81" s="99"/>
+      <c r="D81" s="131"/>
+      <c r="E81" s="132"/>
+      <c r="F81" s="54"/>
+      <c r="G81" s="54"/>
+      <c r="H81" s="55"/>
+      <c r="I81" s="55"/>
+      <c r="J81" s="56"/>
     </row>
     <row r="82" spans="3:10" ht="15">
       <c r="C82" s="99"/>
-      <c r="D82" s="116" t="s">
-        <v>116</v>
-      </c>
-      <c r="E82" s="119">
-        <v>1</v>
-      </c>
-      <c r="F82" s="118">
-        <v>7174000</v>
-      </c>
-      <c r="G82" s="129">
-        <f>F82*E82</f>
-        <v>7174000</v>
-      </c>
-      <c r="H82" s="133" t="s">
-        <v>21</v>
-      </c>
-      <c r="I82" s="14"/>
-      <c r="J82" s="130"/>
+      <c r="D82" s="165" t="s">
+        <v>115</v>
+      </c>
+      <c r="E82" s="165"/>
+      <c r="F82" s="165"/>
+      <c r="G82" s="165"/>
+      <c r="H82" s="127"/>
+      <c r="I82" s="103"/>
+      <c r="J82" s="99"/>
     </row>
     <row r="83" spans="3:10" ht="15">
       <c r="C83" s="99"/>
-      <c r="D83" s="108"/>
-      <c r="E83" s="119"/>
-      <c r="F83" s="120"/>
-      <c r="G83" s="129"/>
-      <c r="H83" s="134"/>
+      <c r="D83" s="116" t="s">
+        <v>116</v>
+      </c>
+      <c r="E83" s="119">
+        <v>1</v>
+      </c>
+      <c r="F83" s="118">
+        <v>7174000</v>
+      </c>
+      <c r="G83" s="129">
+        <f>F83*E83</f>
+        <v>7174000</v>
+      </c>
+      <c r="H83" s="133" t="s">
+        <v>21</v>
+      </c>
       <c r="I83" s="14"/>
       <c r="J83" s="130"/>
     </row>
     <row r="84" spans="3:10" ht="15">
       <c r="C84" s="99"/>
-      <c r="D84" s="128"/>
-      <c r="E84" s="116"/>
+      <c r="D84" s="108"/>
+      <c r="E84" s="119"/>
       <c r="F84" s="120"/>
       <c r="G84" s="129"/>
-      <c r="H84" s="14"/>
+      <c r="H84" s="134"/>
       <c r="I84" s="14"/>
       <c r="J84" s="130"/>
     </row>
     <row r="85" spans="3:10" ht="15">
       <c r="C85" s="99"/>
-      <c r="D85" s="131"/>
-      <c r="E85" s="132"/>
-      <c r="F85" s="54"/>
-      <c r="G85" s="45">
-        <f>SUM(G82:G83)</f>
-        <v>7174000</v>
-      </c>
-      <c r="H85" s="26"/>
-      <c r="I85" s="26"/>
-      <c r="J85" s="27" t="s">
-        <v>7</v>
-      </c>
+      <c r="D85" s="128"/>
+      <c r="E85" s="116"/>
+      <c r="F85" s="120"/>
+      <c r="G85" s="129"/>
+      <c r="H85" s="14"/>
+      <c r="I85" s="14"/>
+      <c r="J85" s="130"/>
     </row>
     <row r="86" spans="3:10" ht="15">
       <c r="C86" s="99"/>
-      <c r="D86" s="15"/>
-      <c r="E86" s="98"/>
-      <c r="F86" s="101"/>
-      <c r="G86" s="135"/>
-      <c r="H86" s="99"/>
-      <c r="I86" s="99"/>
-      <c r="J86" s="99"/>
+      <c r="D86" s="131"/>
+      <c r="E86" s="132"/>
+      <c r="F86" s="54"/>
+      <c r="G86" s="45">
+        <f>SUM(G83:G84)</f>
+        <v>7174000</v>
+      </c>
+      <c r="H86" s="26"/>
+      <c r="I86" s="26"/>
+      <c r="J86" s="27" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="87" spans="3:10" ht="15">
       <c r="C87" s="99"/>
       <c r="D87" s="15"/>
       <c r="E87" s="98"/>
       <c r="F87" s="101"/>
-      <c r="G87" s="43">
-        <f>G8-G21-G60-G67-G79-G85</f>
+      <c r="G87" s="135"/>
+      <c r="H87" s="99"/>
+      <c r="I87" s="99"/>
+      <c r="J87" s="99"/>
+    </row>
+    <row r="88" spans="3:10" ht="15">
+      <c r="C88" s="99"/>
+      <c r="D88" s="15"/>
+      <c r="E88" s="98"/>
+      <c r="F88" s="101"/>
+      <c r="G88" s="43">
+        <f>G8-G21-G61-G68-G80-G86</f>
         <v>-38960700</v>
       </c>
-      <c r="H87" s="12"/>
-      <c r="I87" s="12"/>
-      <c r="J87" s="136" t="s">
+      <c r="H88" s="12"/>
+      <c r="I88" s="12"/>
+      <c r="J88" s="136" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="D69:G69"/>
-    <mergeCell ref="D81:G81"/>
+    <mergeCell ref="D70:G70"/>
+    <mergeCell ref="D82:G82"/>
     <mergeCell ref="C2:J2"/>
     <mergeCell ref="D4:G4"/>
     <mergeCell ref="D9:G9"/>
     <mergeCell ref="D22:G22"/>
-    <mergeCell ref="D61:G61"/>
+    <mergeCell ref="D62:G62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Giai ngan 160 zeus + 270 hecquyn
</commit_message>
<xml_diff>
--- a/Project/TongHopQuy2.xlsx
+++ b/Project/TongHopQuy2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ViTechSolution_LTD\04.Team_Log\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6943354F-121E-4685-AC3F-81E12C7DAF1A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{785AF069-E286-4714-ADAC-065929D40969}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tổng hợp quỹ công ty" sheetId="6" r:id="rId1"/>
@@ -68,7 +68,7 @@
     <definedName name="sport1_p1.5" localSheetId="5">'270_Hecquyn'!$G$26</definedName>
     <definedName name="sport1_p1.5" localSheetId="11">SoM_Dev!$G$47</definedName>
     <definedName name="sport1_p1.5">SPORT1_P1.5!$G$57</definedName>
-    <definedName name="sport1_p2">SPORT1_P2!$G$32</definedName>
+    <definedName name="sport1_p2">SPORT1_P2!$G$34</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="273">
   <si>
     <t>STT</t>
   </si>
@@ -892,6 +892,15 @@
   </si>
   <si>
     <t>Ngày 7/11, tài khoản cá nhân ACB Tuấn</t>
+  </si>
+  <si>
+    <t>Gửi xe tháng 10</t>
+  </si>
+  <si>
+    <t>Đã ck ngày 9/11 từ tk ACB cá nhân</t>
+  </si>
+  <si>
+    <t>Nợ 3tr</t>
   </si>
 </sst>
 </file>
@@ -1087,7 +1096,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="168">
+  <cellXfs count="169">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1510,6 +1519,9 @@
     </xf>
     <xf numFmtId="4" fontId="12" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1853,12 +1865,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="8:11" ht="20.25">
-      <c r="H2" s="163" t="s">
+      <c r="H2" s="164" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="163"/>
-      <c r="J2" s="163"/>
-      <c r="K2" s="163"/>
+      <c r="I2" s="164"/>
+      <c r="J2" s="164"/>
+      <c r="K2" s="164"/>
     </row>
     <row r="3" spans="8:11" ht="15.75">
       <c r="H3" s="6" t="s">
@@ -1894,7 +1906,7 @@
       </c>
       <c r="J5" s="11">
         <f>Pega</f>
-        <v>-22004586</v>
+        <v>-22104586</v>
       </c>
       <c r="K5" s="9"/>
     </row>
@@ -1916,7 +1928,7 @@
       </c>
       <c r="J7" s="11">
         <f>sport1_p2</f>
-        <v>-6035000</v>
+        <v>-11215000</v>
       </c>
       <c r="K7" s="9"/>
     </row>
@@ -1954,7 +1966,7 @@
       <c r="I12" s="9"/>
       <c r="J12" s="12">
         <f>SUM(J4:J11)</f>
-        <v>-73996966.400000006</v>
+        <v>-79276966.400000006</v>
       </c>
       <c r="K12" s="13" t="s">
         <v>7</v>
@@ -2487,16 +2499,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:10" ht="20.25">
-      <c r="C2" s="163" t="s">
+      <c r="C2" s="164" t="s">
         <v>191</v>
       </c>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="163"/>
-      <c r="H2" s="163"/>
-      <c r="I2" s="163"/>
-      <c r="J2" s="163"/>
+      <c r="D2" s="164"/>
+      <c r="E2" s="164"/>
+      <c r="F2" s="164"/>
+      <c r="G2" s="164"/>
+      <c r="H2" s="164"/>
+      <c r="I2" s="164"/>
+      <c r="J2" s="164"/>
     </row>
     <row r="3" spans="3:10" ht="15.75">
       <c r="C3" s="6" t="s">
@@ -2526,12 +2538,12 @@
     </row>
     <row r="4" spans="3:10" ht="15.75" customHeight="1">
       <c r="C4" s="7"/>
-      <c r="D4" s="166" t="s">
+      <c r="D4" s="167" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="166"/>
-      <c r="F4" s="166"/>
-      <c r="G4" s="166"/>
+      <c r="E4" s="167"/>
+      <c r="F4" s="167"/>
+      <c r="G4" s="167"/>
       <c r="H4" s="77"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
@@ -2588,12 +2600,12 @@
     </row>
     <row r="10" spans="3:10" ht="15">
       <c r="C10" s="8"/>
-      <c r="D10" s="166" t="s">
+      <c r="D10" s="167" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="166"/>
-      <c r="F10" s="166"/>
-      <c r="G10" s="166"/>
+      <c r="E10" s="167"/>
+      <c r="F10" s="167"/>
+      <c r="G10" s="167"/>
       <c r="H10" s="77"/>
       <c r="I10" s="14"/>
       <c r="J10" s="15"/>
@@ -2714,12 +2726,12 @@
     </row>
     <row r="18" spans="3:10" ht="15">
       <c r="C18" s="8"/>
-      <c r="D18" s="166" t="s">
+      <c r="D18" s="167" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="166"/>
-      <c r="F18" s="166"/>
-      <c r="G18" s="166"/>
+      <c r="E18" s="167"/>
+      <c r="F18" s="167"/>
+      <c r="G18" s="167"/>
       <c r="H18" s="77"/>
       <c r="I18" s="11"/>
       <c r="J18" s="9"/>
@@ -2921,12 +2933,12 @@
     </row>
     <row r="38" spans="3:10" ht="15">
       <c r="C38" s="8"/>
-      <c r="D38" s="166" t="s">
+      <c r="D38" s="167" t="s">
         <v>26</v>
       </c>
-      <c r="E38" s="166"/>
-      <c r="F38" s="166"/>
-      <c r="G38" s="166"/>
+      <c r="E38" s="167"/>
+      <c r="F38" s="167"/>
+      <c r="G38" s="167"/>
       <c r="H38" s="51"/>
       <c r="I38" s="11"/>
       <c r="J38" s="8"/>
@@ -3065,7 +3077,7 @@
   <dimension ref="C2:J49"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3083,16 +3095,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:10" ht="15">
-      <c r="C2" s="164" t="s">
+      <c r="C2" s="165" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="164"/>
-      <c r="E2" s="164"/>
-      <c r="F2" s="164"/>
-      <c r="G2" s="164"/>
-      <c r="H2" s="164"/>
-      <c r="I2" s="164"/>
-      <c r="J2" s="164"/>
+      <c r="D2" s="165"/>
+      <c r="E2" s="165"/>
+      <c r="F2" s="165"/>
+      <c r="G2" s="165"/>
+      <c r="H2" s="165"/>
+      <c r="I2" s="165"/>
+      <c r="J2" s="165"/>
     </row>
     <row r="3" spans="3:10" ht="15">
       <c r="C3" s="94" t="s">
@@ -3122,12 +3134,12 @@
     </row>
     <row r="4" spans="3:10" ht="15.75" customHeight="1">
       <c r="C4" s="94"/>
-      <c r="D4" s="165" t="s">
+      <c r="D4" s="166" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="165"/>
-      <c r="F4" s="165"/>
-      <c r="G4" s="165"/>
+      <c r="E4" s="166"/>
+      <c r="F4" s="166"/>
+      <c r="G4" s="166"/>
       <c r="H4" s="97"/>
       <c r="I4" s="94"/>
       <c r="J4" s="94"/>
@@ -3207,12 +3219,12 @@
     </row>
     <row r="9" spans="3:10" ht="15">
       <c r="C9" s="98"/>
-      <c r="D9" s="165" t="s">
+      <c r="D9" s="166" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="165"/>
-      <c r="F9" s="165"/>
-      <c r="G9" s="165"/>
+      <c r="E9" s="166"/>
+      <c r="F9" s="166"/>
+      <c r="G9" s="166"/>
       <c r="H9" s="97"/>
       <c r="I9" s="14"/>
       <c r="J9" s="15"/>
@@ -3555,7 +3567,7 @@
         <v>2685000</v>
       </c>
       <c r="G24" s="101">
-        <f t="shared" ref="G24:G33" si="3">E24*F24</f>
+        <f t="shared" ref="G24:G34" si="3">E24*F24</f>
         <v>2685000</v>
       </c>
       <c r="H24" s="102" t="s">
@@ -3772,12 +3784,25 @@
       <c r="J33" s="99"/>
     </row>
     <row r="34" spans="3:10">
-      <c r="C34" s="78"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="93"/>
-      <c r="F34" s="92"/>
-      <c r="G34" s="79"/>
-      <c r="H34" s="89"/>
+      <c r="C34" s="78">
+        <v>26</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="E34" s="93">
+        <v>1</v>
+      </c>
+      <c r="F34" s="92">
+        <v>100000</v>
+      </c>
+      <c r="G34" s="79">
+        <f t="shared" si="3"/>
+        <v>100000</v>
+      </c>
+      <c r="H34" s="89" t="s">
+        <v>9</v>
+      </c>
       <c r="I34" s="80"/>
       <c r="J34" s="9"/>
     </row>
@@ -3787,8 +3812,8 @@
       <c r="E35" s="93"/>
       <c r="F35" s="91"/>
       <c r="G35" s="45">
-        <f>SUM(G10:G33)</f>
-        <v>40404586</v>
+        <f>SUM(G10:G34)</f>
+        <v>40504586</v>
       </c>
       <c r="H35" s="75"/>
       <c r="I35" s="83"/>
@@ -3808,12 +3833,12 @@
     </row>
     <row r="37" spans="3:10" ht="15">
       <c r="C37" s="78"/>
-      <c r="D37" s="166" t="s">
+      <c r="D37" s="167" t="s">
         <v>12</v>
       </c>
-      <c r="E37" s="166"/>
-      <c r="F37" s="166"/>
-      <c r="G37" s="166"/>
+      <c r="E37" s="167"/>
+      <c r="F37" s="167"/>
+      <c r="G37" s="167"/>
       <c r="H37" s="88"/>
       <c r="I37" s="80"/>
       <c r="J37" s="9"/>
@@ -3848,12 +3873,12 @@
     </row>
     <row r="40" spans="3:10" ht="15">
       <c r="C40" s="78"/>
-      <c r="D40" s="166" t="s">
+      <c r="D40" s="167" t="s">
         <v>26</v>
       </c>
-      <c r="E40" s="166"/>
-      <c r="F40" s="166"/>
-      <c r="G40" s="166"/>
+      <c r="E40" s="167"/>
+      <c r="F40" s="167"/>
+      <c r="G40" s="167"/>
       <c r="H40" s="90"/>
       <c r="I40" s="80"/>
       <c r="J40" s="9"/>
@@ -3964,7 +3989,7 @@
       <c r="F49" s="79"/>
       <c r="G49" s="43">
         <f>G8-G35-G38-G46</f>
-        <v>-22004586</v>
+        <v>-22104586</v>
       </c>
       <c r="H49" s="73"/>
       <c r="I49" s="16"/>
@@ -3989,8 +4014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06BE7A19-D435-4A51-A018-E212475E8992}">
   <dimension ref="C2:M57"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="M45" sqref="M45"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4010,16 +4035,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:10" ht="15">
-      <c r="C2" s="164" t="s">
+      <c r="C2" s="165" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="164"/>
-      <c r="E2" s="164"/>
-      <c r="F2" s="164"/>
-      <c r="G2" s="164"/>
-      <c r="H2" s="164"/>
-      <c r="I2" s="164"/>
-      <c r="J2" s="164"/>
+      <c r="D2" s="165"/>
+      <c r="E2" s="165"/>
+      <c r="F2" s="165"/>
+      <c r="G2" s="165"/>
+      <c r="H2" s="165"/>
+      <c r="I2" s="165"/>
+      <c r="J2" s="165"/>
     </row>
     <row r="3" spans="3:10" ht="15">
       <c r="C3" s="94" t="s">
@@ -4049,12 +4074,12 @@
     </row>
     <row r="4" spans="3:10" ht="15.75" customHeight="1">
       <c r="C4" s="94"/>
-      <c r="D4" s="165" t="s">
+      <c r="D4" s="166" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="165"/>
-      <c r="F4" s="165"/>
-      <c r="G4" s="165"/>
+      <c r="E4" s="166"/>
+      <c r="F4" s="166"/>
+      <c r="G4" s="166"/>
       <c r="H4" s="115"/>
       <c r="I4" s="94"/>
       <c r="J4" s="94"/>
@@ -4139,12 +4164,12 @@
     </row>
     <row r="9" spans="3:10" ht="15">
       <c r="C9" s="99"/>
-      <c r="D9" s="165" t="s">
+      <c r="D9" s="166" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="165"/>
-      <c r="F9" s="165"/>
-      <c r="G9" s="165"/>
+      <c r="E9" s="166"/>
+      <c r="F9" s="166"/>
+      <c r="G9" s="166"/>
       <c r="H9" s="115"/>
       <c r="I9" s="14"/>
       <c r="J9" s="15"/>
@@ -4558,12 +4583,12 @@
     </row>
     <row r="30" spans="3:13" ht="15">
       <c r="C30" s="99"/>
-      <c r="D30" s="165" t="s">
+      <c r="D30" s="166" t="s">
         <v>29</v>
       </c>
-      <c r="E30" s="165"/>
-      <c r="F30" s="165"/>
-      <c r="G30" s="165"/>
+      <c r="E30" s="166"/>
+      <c r="F30" s="166"/>
+      <c r="G30" s="166"/>
       <c r="H30" s="115"/>
       <c r="I30" s="103"/>
       <c r="J30" s="99"/>
@@ -4926,12 +4951,12 @@
     </row>
     <row r="48" spans="3:10" ht="15">
       <c r="C48" s="99"/>
-      <c r="D48" s="165" t="s">
+      <c r="D48" s="166" t="s">
         <v>26</v>
       </c>
-      <c r="E48" s="165"/>
-      <c r="F48" s="165"/>
-      <c r="G48" s="165"/>
+      <c r="E48" s="166"/>
+      <c r="F48" s="166"/>
+      <c r="G48" s="166"/>
       <c r="H48" s="127"/>
       <c r="I48" s="103"/>
       <c r="J48" s="99"/>
@@ -5177,37 +5202,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C59F4560-1B60-4B5E-991D-A390F0A6ECED}">
   <dimension ref="C2:P40"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="5"/>
     <col min="3" max="3" width="8.42578125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="37.85546875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="45.7109375" style="5" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" style="20" customWidth="1"/>
     <col min="6" max="6" width="14.140625" style="46" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="32.42578125" style="46" customWidth="1"/>
     <col min="8" max="8" width="12.85546875" style="21" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" style="21" customWidth="1"/>
-    <col min="10" max="10" width="33.5703125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="23.5703125" style="21" customWidth="1"/>
+    <col min="10" max="10" width="20.5703125" style="5" customWidth="1"/>
     <col min="11" max="12" width="19.140625" style="5" customWidth="1"/>
     <col min="13" max="16" width="11.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="17" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:12" ht="20.25">
-      <c r="C2" s="163" t="s">
+      <c r="C2" s="164" t="s">
         <v>191</v>
       </c>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="163"/>
-      <c r="H2" s="163"/>
-      <c r="I2" s="163"/>
-      <c r="J2" s="163"/>
+      <c r="D2" s="164"/>
+      <c r="E2" s="164"/>
+      <c r="F2" s="164"/>
+      <c r="G2" s="164"/>
+      <c r="H2" s="164"/>
+      <c r="I2" s="164"/>
+      <c r="J2" s="164"/>
     </row>
     <row r="3" spans="3:12" ht="15.75">
       <c r="C3" s="6" t="s">
@@ -5237,12 +5262,12 @@
     </row>
     <row r="4" spans="3:12" ht="15.75" customHeight="1">
       <c r="C4" s="7"/>
-      <c r="D4" s="166" t="s">
+      <c r="D4" s="167" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="166"/>
-      <c r="F4" s="166"/>
-      <c r="G4" s="166"/>
+      <c r="E4" s="167"/>
+      <c r="F4" s="167"/>
+      <c r="G4" s="167"/>
       <c r="H4" s="60"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
@@ -5318,7 +5343,7 @@
       <c r="I7" s="11"/>
       <c r="J7" s="9"/>
     </row>
-    <row r="8" spans="3:12" ht="15">
+    <row r="8" spans="3:12" ht="30">
       <c r="C8" s="8"/>
       <c r="D8" s="9"/>
       <c r="E8" s="10"/>
@@ -5350,12 +5375,12 @@
     </row>
     <row r="10" spans="3:12" ht="15">
       <c r="C10" s="8"/>
-      <c r="D10" s="166" t="s">
+      <c r="D10" s="167" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="166"/>
-      <c r="F10" s="166"/>
-      <c r="G10" s="166"/>
+      <c r="E10" s="167"/>
+      <c r="F10" s="167"/>
+      <c r="G10" s="167"/>
       <c r="H10" s="59"/>
       <c r="I10" s="14"/>
       <c r="J10" s="15"/>
@@ -5492,12 +5517,12 @@
     </row>
     <row r="18" spans="3:16" ht="15">
       <c r="C18" s="8"/>
-      <c r="D18" s="166" t="s">
+      <c r="D18" s="167" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="166"/>
-      <c r="F18" s="166"/>
-      <c r="G18" s="166"/>
+      <c r="E18" s="167"/>
+      <c r="F18" s="167"/>
+      <c r="G18" s="167"/>
       <c r="H18" s="59"/>
       <c r="I18" s="11"/>
       <c r="J18" s="9"/>
@@ -5605,9 +5630,17 @@
       </c>
       <c r="I21" s="11"/>
       <c r="J21" s="9"/>
+      <c r="K21" s="156">
+        <f>K20+G33</f>
+        <v>24668762</v>
+      </c>
+      <c r="L21" s="156">
+        <f>L20+G32</f>
+        <v>9192418</v>
+      </c>
       <c r="N21" s="156"/>
     </row>
-    <row r="22" spans="3:16" ht="28.5">
+    <row r="22" spans="3:16" ht="15">
       <c r="C22" s="8"/>
       <c r="D22" s="1" t="s">
         <v>228</v>
@@ -5629,8 +5662,11 @@
       <c r="J22" s="35" t="s">
         <v>240</v>
       </c>
-      <c r="M22" s="5" t="s">
-        <v>259</v>
+      <c r="K22" s="18" t="s">
+        <v>272</v>
+      </c>
+      <c r="M22" s="163">
+        <v>0.1</v>
       </c>
       <c r="N22" s="156">
         <f>N20*0.1</f>
@@ -5661,6 +5697,10 @@
       </c>
       <c r="I23" s="11"/>
       <c r="J23" s="9"/>
+      <c r="K23" s="156">
+        <f>K21-3000000</f>
+        <v>21668762</v>
+      </c>
     </row>
     <row r="24" spans="3:16" ht="15">
       <c r="C24" s="8"/>
@@ -5728,7 +5768,7 @@
       <c r="I26" s="24"/>
       <c r="J26" s="15"/>
     </row>
-    <row r="27" spans="3:16" ht="30">
+    <row r="27" spans="3:16" ht="15">
       <c r="C27" s="8"/>
       <c r="D27" s="22" t="s">
         <v>249</v>
@@ -5812,17 +5852,17 @@
     </row>
     <row r="31" spans="3:16" ht="15">
       <c r="C31" s="8"/>
-      <c r="D31" s="166" t="s">
+      <c r="D31" s="167" t="s">
         <v>26</v>
       </c>
-      <c r="E31" s="166"/>
-      <c r="F31" s="166"/>
-      <c r="G31" s="166"/>
+      <c r="E31" s="167"/>
+      <c r="F31" s="167"/>
+      <c r="G31" s="167"/>
       <c r="H31" s="51"/>
       <c r="I31" s="11"/>
       <c r="J31" s="8"/>
     </row>
-    <row r="32" spans="3:16" ht="15">
+    <row r="32" spans="3:16" ht="30">
       <c r="C32" s="8">
         <v>1</v>
       </c>
@@ -5841,10 +5881,12 @@
         <v>6789418</v>
       </c>
       <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
+      <c r="I32" s="14" t="s">
+        <v>271</v>
+      </c>
       <c r="J32" s="28"/>
     </row>
-    <row r="33" spans="3:10" ht="15">
+    <row r="33" spans="3:10" ht="30">
       <c r="C33" s="8">
         <v>2</v>
       </c>
@@ -5863,10 +5905,11 @@
         <v>6789418</v>
       </c>
       <c r="H33" s="14"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="18"/>
-    </row>
-    <row r="34" spans="3:10" ht="15">
+      <c r="I33" s="14" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="34" spans="3:10" ht="30">
       <c r="C34" s="8">
         <v>3</v>
       </c>
@@ -5885,10 +5928,12 @@
         <v>8147301.6000000006</v>
       </c>
       <c r="H34" s="14"/>
-      <c r="I34" s="11"/>
+      <c r="I34" s="14" t="s">
+        <v>271</v>
+      </c>
       <c r="J34" s="18"/>
     </row>
-    <row r="35" spans="3:10" ht="15">
+    <row r="35" spans="3:10" ht="45">
       <c r="C35" s="8">
         <v>4</v>
       </c>
@@ -5907,7 +5952,9 @@
         <v>5431534.4000000004</v>
       </c>
       <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
+      <c r="I35" s="14" t="s">
+        <v>271</v>
+      </c>
       <c r="J35" s="18"/>
     </row>
     <row r="36" spans="3:10" ht="15">
@@ -5987,8 +6034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A00FBF6-6528-4077-97A8-E7F8FA86DD30}">
   <dimension ref="C2:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11:P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -6010,16 +6057,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:16" ht="20.25">
-      <c r="C2" s="163" t="s">
+      <c r="C2" s="164" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="163"/>
-      <c r="H2" s="163"/>
-      <c r="I2" s="163"/>
-      <c r="J2" s="163"/>
+      <c r="D2" s="164"/>
+      <c r="E2" s="164"/>
+      <c r="F2" s="164"/>
+      <c r="G2" s="164"/>
+      <c r="H2" s="164"/>
+      <c r="I2" s="164"/>
+      <c r="J2" s="164"/>
     </row>
     <row r="3" spans="3:16" ht="15.75">
       <c r="C3" s="6" t="s">
@@ -6049,24 +6096,24 @@
     </row>
     <row r="4" spans="3:16" ht="15.75" customHeight="1">
       <c r="C4" s="7"/>
-      <c r="D4" s="166" t="s">
+      <c r="D4" s="167" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="166"/>
-      <c r="F4" s="166"/>
-      <c r="G4" s="166"/>
+      <c r="E4" s="167"/>
+      <c r="F4" s="167"/>
+      <c r="G4" s="167"/>
       <c r="H4" s="57"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="3:16" ht="20.25">
       <c r="C5" s="7"/>
-      <c r="D5" s="166" t="s">
+      <c r="D5" s="167" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="166"/>
-      <c r="F5" s="166"/>
-      <c r="G5" s="166"/>
+      <c r="E5" s="167"/>
+      <c r="F5" s="167"/>
+      <c r="G5" s="167"/>
       <c r="H5" s="60"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
@@ -6168,12 +6215,12 @@
     </row>
     <row r="11" spans="3:16" ht="15">
       <c r="C11" s="8"/>
-      <c r="D11" s="166" t="s">
+      <c r="D11" s="167" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="166"/>
-      <c r="F11" s="166"/>
-      <c r="G11" s="166"/>
+      <c r="E11" s="167"/>
+      <c r="F11" s="167"/>
+      <c r="G11" s="167"/>
       <c r="H11" s="57"/>
       <c r="I11" s="11"/>
       <c r="J11" s="9"/>
@@ -6296,7 +6343,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="15" spans="3:16" ht="15">
+    <row r="15" spans="3:16" ht="28.5">
       <c r="C15" s="8"/>
       <c r="D15" s="1" t="s">
         <v>248</v>
@@ -6322,7 +6369,7 @@
       <c r="L15" s="5">
         <v>20000000</v>
       </c>
-      <c r="M15" s="62" t="s">
+      <c r="N15" s="62" t="s">
         <v>259</v>
       </c>
       <c r="O15" s="156">
@@ -6369,12 +6416,12 @@
     </row>
     <row r="18" spans="3:10" ht="15">
       <c r="C18" s="8"/>
-      <c r="D18" s="166" t="s">
+      <c r="D18" s="167" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="166"/>
-      <c r="F18" s="166"/>
-      <c r="G18" s="166"/>
+      <c r="E18" s="167"/>
+      <c r="F18" s="167"/>
+      <c r="G18" s="167"/>
       <c r="H18" s="51"/>
       <c r="I18" s="11"/>
       <c r="J18" s="8"/>
@@ -6526,10 +6573,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F413B64-656B-492A-8F7D-8434699F234E}">
-  <dimension ref="C2:J32"/>
+  <dimension ref="C2:J34"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -6547,16 +6594,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:10" ht="20.25">
-      <c r="C2" s="163" t="s">
+      <c r="C2" s="164" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="163"/>
-      <c r="H2" s="163"/>
-      <c r="I2" s="163"/>
-      <c r="J2" s="163"/>
+      <c r="D2" s="164"/>
+      <c r="E2" s="164"/>
+      <c r="F2" s="164"/>
+      <c r="G2" s="164"/>
+      <c r="H2" s="164"/>
+      <c r="I2" s="164"/>
+      <c r="J2" s="164"/>
     </row>
     <row r="3" spans="3:10" ht="15.75">
       <c r="C3" s="6" t="s">
@@ -6586,12 +6633,12 @@
     </row>
     <row r="4" spans="3:10" ht="15.75" customHeight="1">
       <c r="C4" s="7"/>
-      <c r="D4" s="166" t="s">
+      <c r="D4" s="167" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="166"/>
-      <c r="F4" s="166"/>
-      <c r="G4" s="166"/>
+      <c r="E4" s="167"/>
+      <c r="F4" s="167"/>
+      <c r="G4" s="167"/>
       <c r="H4" s="48"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
@@ -6649,12 +6696,12 @@
     </row>
     <row r="9" spans="3:10" ht="15">
       <c r="C9" s="8"/>
-      <c r="D9" s="166" t="s">
+      <c r="D9" s="167" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="166"/>
-      <c r="F9" s="166"/>
-      <c r="G9" s="166"/>
+      <c r="E9" s="167"/>
+      <c r="F9" s="167"/>
+      <c r="G9" s="167"/>
       <c r="H9" s="48"/>
       <c r="I9" s="14"/>
       <c r="J9" s="15"/>
@@ -6666,7 +6713,7 @@
       <c r="D10" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="24">
+      <c r="E10" s="32">
         <v>1</v>
       </c>
       <c r="F10" s="23">
@@ -6688,7 +6735,7 @@
       <c r="D11" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="E11" s="24">
+      <c r="E11" s="32">
         <v>1</v>
       </c>
       <c r="F11" s="23">
@@ -6710,7 +6757,7 @@
       <c r="D12" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="24">
+      <c r="E12" s="32">
         <v>2</v>
       </c>
       <c r="F12" s="23">
@@ -6732,7 +6779,7 @@
       <c r="D13" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="24">
+      <c r="E13" s="32">
         <v>1</v>
       </c>
       <c r="F13" s="23">
@@ -6754,7 +6801,7 @@
       <c r="D14" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="24">
+      <c r="E14" s="32">
         <v>2</v>
       </c>
       <c r="F14" s="23">
@@ -6776,7 +6823,7 @@
       <c r="D15" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="E15" s="24">
+      <c r="E15" s="32">
         <v>1</v>
       </c>
       <c r="F15" s="23">
@@ -6861,25 +6908,18 @@
       <c r="D19" s="24"/>
       <c r="E19" s="32"/>
       <c r="F19" s="23"/>
-      <c r="G19" s="49">
-        <f>SUM(G10:G16)</f>
-        <v>2435000</v>
-      </c>
-      <c r="H19" s="50"/>
-      <c r="I19" s="29"/>
-      <c r="J19" s="27" t="s">
-        <v>7</v>
-      </c>
+      <c r="G19" s="23"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="9"/>
     </row>
     <row r="20" spans="3:10" ht="15">
       <c r="C20" s="8"/>
-      <c r="D20" s="166" t="s">
-        <v>29</v>
-      </c>
-      <c r="E20" s="166"/>
-      <c r="F20" s="166"/>
-      <c r="G20" s="166"/>
-      <c r="H20" s="48"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="24"/>
       <c r="I20" s="11"/>
       <c r="J20" s="9"/>
     </row>
@@ -6888,86 +6928,85 @@
       <c r="D21" s="24"/>
       <c r="E21" s="32"/>
       <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="24"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="9"/>
+      <c r="G21" s="49">
+        <f>SUM(G10:G18)</f>
+        <v>7615000</v>
+      </c>
+      <c r="H21" s="50"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="27" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="22" spans="3:10" ht="15">
       <c r="C22" s="8"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="49">
-        <f>SUM(G21)</f>
-        <v>0</v>
-      </c>
-      <c r="H22" s="50"/>
-      <c r="I22" s="29"/>
-      <c r="J22" s="27" t="s">
-        <v>7</v>
-      </c>
+      <c r="D22" s="167" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="167"/>
+      <c r="F22" s="167"/>
+      <c r="G22" s="167"/>
+      <c r="H22" s="48"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="9"/>
     </row>
     <row r="23" spans="3:10" ht="15">
       <c r="C23" s="8"/>
-      <c r="D23" s="166" t="s">
+      <c r="D23" s="24"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="9"/>
+    </row>
+    <row r="24" spans="3:10" ht="15">
+      <c r="C24" s="8"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="49">
+        <f>SUM(G23)</f>
+        <v>0</v>
+      </c>
+      <c r="H24" s="50"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="3:10" ht="15">
+      <c r="C25" s="8"/>
+      <c r="D25" s="167" t="s">
         <v>26</v>
       </c>
-      <c r="E23" s="166"/>
-      <c r="F23" s="166"/>
-      <c r="G23" s="166"/>
-      <c r="H23" s="51"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="8"/>
-    </row>
-    <row r="24" spans="3:10" ht="15">
-      <c r="C24" s="8">
-        <v>1</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" s="10"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="44"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="28"/>
-    </row>
-    <row r="25" spans="3:10" ht="15">
-      <c r="C25" s="8">
-        <v>2</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="E25" s="10"/>
-      <c r="F25" s="42"/>
-      <c r="G25" s="44"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="18"/>
+      <c r="E25" s="167"/>
+      <c r="F25" s="167"/>
+      <c r="G25" s="167"/>
+      <c r="H25" s="51"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="8"/>
     </row>
     <row r="26" spans="3:10" ht="15">
       <c r="C26" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E26" s="10"/>
       <c r="F26" s="42"/>
       <c r="G26" s="44"/>
       <c r="H26" s="14"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="18"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="28"/>
     </row>
     <row r="27" spans="3:10" ht="15">
       <c r="C27" s="8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E27" s="10"/>
       <c r="F27" s="42"/>
@@ -6978,69 +7017,97 @@
     </row>
     <row r="28" spans="3:10" ht="15">
       <c r="C28" s="8">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="E28" s="10"/>
       <c r="F28" s="42"/>
-      <c r="G28" s="44">
-        <v>3600000</v>
-      </c>
-      <c r="H28" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="I28" s="14"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="11"/>
       <c r="J28" s="18"/>
     </row>
     <row r="29" spans="3:10" ht="15">
-      <c r="C29" s="8"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="47"/>
-      <c r="G29" s="45">
-        <f>SUM(G24:G28)</f>
-        <v>3600000</v>
-      </c>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="27" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="3:10">
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
+      <c r="C29" s="8">
+        <v>4</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="10"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="18"/>
+    </row>
+    <row r="30" spans="3:10" ht="15">
+      <c r="C30" s="8">
+        <v>5</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>64</v>
+      </c>
       <c r="E30" s="10"/>
       <c r="F30" s="42"/>
-      <c r="G30" s="42"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="8"/>
+      <c r="G30" s="44">
+        <v>3600000</v>
+      </c>
+      <c r="H30" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I30" s="14"/>
+      <c r="J30" s="18"/>
     </row>
     <row r="31" spans="3:10" ht="15">
       <c r="C31" s="8"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="42"/>
-      <c r="G31" s="52"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-    </row>
-    <row r="32" spans="3:10" ht="15">
+      <c r="D31" s="30"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="45">
+        <f>SUM(G26:G30)</f>
+        <v>3600000</v>
+      </c>
+      <c r="H31" s="26"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="3:10">
       <c r="C32" s="8"/>
-      <c r="D32" s="17"/>
+      <c r="D32" s="8"/>
       <c r="E32" s="10"/>
       <c r="F32" s="42"/>
-      <c r="G32" s="43">
-        <f>G8-G19-G22-G29</f>
-        <v>-6035000</v>
-      </c>
-      <c r="H32" s="12"/>
-      <c r="I32" s="16"/>
-      <c r="J32" s="25" t="s">
+      <c r="G32" s="42"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="8"/>
+    </row>
+    <row r="33" spans="3:10" ht="15">
+      <c r="C33" s="8"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="42"/>
+      <c r="G33" s="52"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+    </row>
+    <row r="34" spans="3:10" ht="15">
+      <c r="C34" s="8"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="42"/>
+      <c r="G34" s="43">
+        <f>G8-G21-G24-G31</f>
+        <v>-11215000</v>
+      </c>
+      <c r="H34" s="12"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="25" t="s">
         <v>25</v>
       </c>
     </row>
@@ -7049,8 +7116,8 @@
     <mergeCell ref="C2:J2"/>
     <mergeCell ref="D4:G4"/>
     <mergeCell ref="D9:G9"/>
-    <mergeCell ref="D20:G20"/>
-    <mergeCell ref="D23:G23"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="D25:G25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7062,7 +7129,7 @@
   <dimension ref="C2:J32"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D10" sqref="D10:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -7080,16 +7147,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:10" ht="20.25">
-      <c r="C2" s="163" t="s">
+      <c r="C2" s="164" t="s">
         <v>71</v>
       </c>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="163"/>
-      <c r="H2" s="163"/>
-      <c r="I2" s="163"/>
-      <c r="J2" s="163"/>
+      <c r="D2" s="164"/>
+      <c r="E2" s="164"/>
+      <c r="F2" s="164"/>
+      <c r="G2" s="164"/>
+      <c r="H2" s="164"/>
+      <c r="I2" s="164"/>
+      <c r="J2" s="164"/>
     </row>
     <row r="3" spans="3:10" ht="15.75">
       <c r="C3" s="6" t="s">
@@ -7119,12 +7186,12 @@
     </row>
     <row r="4" spans="3:10" ht="15.75" customHeight="1">
       <c r="C4" s="7"/>
-      <c r="D4" s="166" t="s">
+      <c r="D4" s="167" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="166"/>
-      <c r="F4" s="166"/>
-      <c r="G4" s="166"/>
+      <c r="E4" s="167"/>
+      <c r="F4" s="167"/>
+      <c r="G4" s="167"/>
       <c r="H4" s="48"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
@@ -7182,12 +7249,12 @@
     </row>
     <row r="9" spans="3:10" ht="15">
       <c r="C9" s="8"/>
-      <c r="D9" s="166" t="s">
+      <c r="D9" s="167" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="166"/>
-      <c r="F9" s="166"/>
-      <c r="G9" s="166"/>
+      <c r="E9" s="167"/>
+      <c r="F9" s="167"/>
+      <c r="G9" s="167"/>
       <c r="H9" s="48"/>
       <c r="I9" s="14"/>
       <c r="J9" s="15"/>
@@ -7359,12 +7426,12 @@
     </row>
     <row r="20" spans="3:10" ht="15">
       <c r="C20" s="8"/>
-      <c r="D20" s="166" t="s">
+      <c r="D20" s="167" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="166"/>
-      <c r="F20" s="166"/>
-      <c r="G20" s="166"/>
+      <c r="E20" s="167"/>
+      <c r="F20" s="167"/>
+      <c r="G20" s="167"/>
       <c r="H20" s="48"/>
       <c r="I20" s="11"/>
       <c r="J20" s="9"/>
@@ -7396,12 +7463,12 @@
     </row>
     <row r="23" spans="3:10" ht="15">
       <c r="C23" s="8"/>
-      <c r="D23" s="166" t="s">
+      <c r="D23" s="167" t="s">
         <v>26</v>
       </c>
-      <c r="E23" s="166"/>
-      <c r="F23" s="166"/>
-      <c r="G23" s="166"/>
+      <c r="E23" s="167"/>
+      <c r="F23" s="167"/>
+      <c r="G23" s="167"/>
       <c r="H23" s="51"/>
       <c r="I23" s="11"/>
       <c r="J23" s="8"/>
@@ -7539,8 +7606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73990C79-75DF-434D-B272-2581D279AD79}">
   <dimension ref="C2:M88"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H61" sqref="H61"/>
+    <sheetView topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -7560,16 +7627,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:10" ht="20.25">
-      <c r="C2" s="167" t="s">
+      <c r="C2" s="168" t="s">
         <v>73</v>
       </c>
-      <c r="D2" s="167"/>
-      <c r="E2" s="167"/>
-      <c r="F2" s="167"/>
-      <c r="G2" s="167"/>
-      <c r="H2" s="167"/>
-      <c r="I2" s="167"/>
-      <c r="J2" s="167"/>
+      <c r="D2" s="168"/>
+      <c r="E2" s="168"/>
+      <c r="F2" s="168"/>
+      <c r="G2" s="168"/>
+      <c r="H2" s="168"/>
+      <c r="I2" s="168"/>
+      <c r="J2" s="168"/>
     </row>
     <row r="3" spans="3:10" ht="15.75">
       <c r="C3" s="112" t="s">
@@ -7599,12 +7666,12 @@
     </row>
     <row r="4" spans="3:10" ht="15.75" customHeight="1">
       <c r="C4" s="114"/>
-      <c r="D4" s="165" t="s">
+      <c r="D4" s="166" t="s">
         <v>81</v>
       </c>
-      <c r="E4" s="165"/>
-      <c r="F4" s="165"/>
-      <c r="G4" s="165"/>
+      <c r="E4" s="166"/>
+      <c r="F4" s="166"/>
+      <c r="G4" s="166"/>
       <c r="H4" s="115"/>
       <c r="I4" s="114"/>
       <c r="J4" s="114"/>
@@ -7662,12 +7729,12 @@
     </row>
     <row r="9" spans="3:10" ht="15">
       <c r="C9" s="99"/>
-      <c r="D9" s="165" t="s">
+      <c r="D9" s="166" t="s">
         <v>74</v>
       </c>
-      <c r="E9" s="165"/>
-      <c r="F9" s="165"/>
-      <c r="G9" s="165"/>
+      <c r="E9" s="166"/>
+      <c r="F9" s="166"/>
+      <c r="G9" s="166"/>
       <c r="H9" s="115"/>
       <c r="I9" s="14"/>
       <c r="J9" s="15"/>
@@ -7921,12 +7988,12 @@
     </row>
     <row r="22" spans="3:10" ht="15">
       <c r="C22" s="99"/>
-      <c r="D22" s="165" t="s">
+      <c r="D22" s="166" t="s">
         <v>82</v>
       </c>
-      <c r="E22" s="165"/>
-      <c r="F22" s="165"/>
-      <c r="G22" s="165"/>
+      <c r="E22" s="166"/>
+      <c r="F22" s="166"/>
+      <c r="G22" s="166"/>
       <c r="H22" s="115"/>
       <c r="I22" s="103"/>
       <c r="J22" s="99"/>
@@ -8804,12 +8871,12 @@
     </row>
     <row r="62" spans="3:13" ht="15">
       <c r="C62" s="99"/>
-      <c r="D62" s="165" t="s">
+      <c r="D62" s="166" t="s">
         <v>104</v>
       </c>
-      <c r="E62" s="165"/>
-      <c r="F62" s="165"/>
-      <c r="G62" s="165"/>
+      <c r="E62" s="166"/>
+      <c r="F62" s="166"/>
+      <c r="G62" s="166"/>
       <c r="H62" s="127"/>
       <c r="I62" s="103"/>
       <c r="J62" s="99"/>
@@ -8941,12 +9008,12 @@
     </row>
     <row r="70" spans="3:10" ht="15">
       <c r="C70" s="99"/>
-      <c r="D70" s="165" t="s">
+      <c r="D70" s="166" t="s">
         <v>108</v>
       </c>
-      <c r="E70" s="165"/>
-      <c r="F70" s="165"/>
-      <c r="G70" s="165"/>
+      <c r="E70" s="166"/>
+      <c r="F70" s="166"/>
+      <c r="G70" s="166"/>
       <c r="H70" s="127"/>
       <c r="I70" s="103"/>
       <c r="J70" s="99"/>
@@ -9168,12 +9235,12 @@
     </row>
     <row r="82" spans="3:10" ht="15">
       <c r="C82" s="99"/>
-      <c r="D82" s="165" t="s">
+      <c r="D82" s="166" t="s">
         <v>115</v>
       </c>
-      <c r="E82" s="165"/>
-      <c r="F82" s="165"/>
-      <c r="G82" s="165"/>
+      <c r="E82" s="166"/>
+      <c r="F82" s="166"/>
+      <c r="G82" s="166"/>
       <c r="H82" s="127"/>
       <c r="I82" s="103"/>
       <c r="J82" s="99"/>

</xml_diff>

<commit_message>
Update sau khi chuyển sang chỗ ở mới
</commit_message>
<xml_diff>
--- a/Project/TongHopQuy2.xlsx
+++ b/Project/TongHopQuy2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\03.ViTechSolution_LTD\04.Team_Log\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71EA1803-E9FF-49A2-92D7-C4D17DEB159A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E384D2-DED1-4051-A8A3-5AA8DBF6B902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tổng hợp quỹ công ty" sheetId="6" r:id="rId1"/>
@@ -73,7 +73,7 @@
     <definedName name="sport1_p1.5" localSheetId="12">SoM_Dev!$G$47</definedName>
     <definedName name="sport1_p1.5">SPORT1_P1.5!$G$57</definedName>
     <definedName name="sport1_p2" localSheetId="7">BaoTangQS!$G$37</definedName>
-    <definedName name="sport1_p2">SPORT1_P2!$G$38</definedName>
+    <definedName name="sport1_p2">SPORT1_P2!$G$40</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="314">
   <si>
     <t>STT</t>
   </si>
@@ -1028,6 +1028,15 @@
   </si>
   <si>
     <t>Chuyển đồ sang văn phòng mới</t>
+  </si>
+  <si>
+    <t>chuyển bàn sang Khởi Nguồn</t>
+  </si>
+  <si>
+    <t>Đặt 2 board test</t>
+  </si>
+  <si>
+    <t>Tuấn chuyển anh Khơ 2tr</t>
   </si>
 </sst>
 </file>
@@ -2025,7 +2034,7 @@
       </c>
       <c r="J4" s="11">
         <f>chi_phi_cong_ty</f>
-        <v>-65906700</v>
+        <v>-66256700</v>
       </c>
       <c r="K4" s="8"/>
     </row>
@@ -2096,7 +2105,7 @@
       <c r="I12" s="9"/>
       <c r="J12" s="12">
         <f>SUM(J4:J11)</f>
-        <v>-106222966.40000001</v>
+        <v>-106572966.40000001</v>
       </c>
       <c r="K12" s="13" t="s">
         <v>7</v>
@@ -2114,8 +2123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73990C79-75DF-434D-B272-2581D279AD79}">
   <dimension ref="C2:M119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H84" sqref="H84"/>
+    <sheetView topLeftCell="A79" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I98" sqref="I98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4014,7 +4023,7 @@
         <v>750000</v>
       </c>
       <c r="G94" s="44">
-        <f t="shared" ref="G94:G97" si="4">E94*F94</f>
+        <f t="shared" ref="G94:G98" si="4">E94*F94</f>
         <v>750000</v>
       </c>
       <c r="H94" s="14" t="s">
@@ -4088,11 +4097,22 @@
     </row>
     <row r="98" spans="3:10" ht="15">
       <c r="C98" s="99"/>
-      <c r="D98" s="15"/>
-      <c r="E98" s="98"/>
-      <c r="F98" s="101"/>
-      <c r="G98" s="44"/>
-      <c r="H98" s="14"/>
+      <c r="D98" s="15" t="s">
+        <v>311</v>
+      </c>
+      <c r="E98" s="98">
+        <v>1</v>
+      </c>
+      <c r="F98" s="101">
+        <v>350000</v>
+      </c>
+      <c r="G98" s="44">
+        <f t="shared" si="4"/>
+        <v>350000</v>
+      </c>
+      <c r="H98" s="14" t="s">
+        <v>9</v>
+      </c>
       <c r="I98" s="14"/>
       <c r="J98" s="130"/>
     </row>
@@ -4102,8 +4122,8 @@
       <c r="E99" s="132"/>
       <c r="F99" s="54"/>
       <c r="G99" s="45">
-        <f>SUM(G89:G97)</f>
-        <v>12866000</v>
+        <f>SUM(G89:G98)</f>
+        <v>13216000</v>
       </c>
       <c r="H99" s="26"/>
       <c r="I99" s="26"/>
@@ -4444,7 +4464,7 @@
       <c r="F119" s="101"/>
       <c r="G119" s="43">
         <f>G8-G33-G87-G99-G111-G117</f>
-        <v>-65906700</v>
+        <v>-66256700</v>
       </c>
       <c r="H119" s="12"/>
       <c r="I119" s="12"/>
@@ -9066,10 +9086,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F413B64-656B-492A-8F7D-8434699F234E}">
-  <dimension ref="C2:J38"/>
+  <dimension ref="C2:J40"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -9345,7 +9365,7 @@
         <v>15000</v>
       </c>
       <c r="G16" s="23">
-        <f t="shared" ref="G16:G23" si="0">F16*E16</f>
+        <f t="shared" ref="G16:G24" si="0">F16*E16</f>
         <v>150000</v>
       </c>
       <c r="H16" s="34" t="s">
@@ -9505,38 +9525,44 @@
     </row>
     <row r="24" spans="3:10" ht="15">
       <c r="C24" s="8"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="24"/>
+      <c r="D24" s="24" t="s">
+        <v>312</v>
+      </c>
+      <c r="E24" s="32">
+        <v>1</v>
+      </c>
+      <c r="F24" s="23">
+        <v>2000000</v>
+      </c>
+      <c r="G24" s="23">
+        <f t="shared" si="0"/>
+        <v>2000000</v>
+      </c>
+      <c r="H24" s="24" t="s">
+        <v>9</v>
+      </c>
       <c r="I24" s="11"/>
-      <c r="J24" s="9"/>
+      <c r="J24" s="9" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="25" spans="3:10" ht="15">
       <c r="C25" s="8"/>
       <c r="D25" s="24"/>
       <c r="E25" s="32"/>
       <c r="F25" s="23"/>
-      <c r="G25" s="49">
-        <f>SUM(G10:G18)</f>
-        <v>7615000</v>
-      </c>
-      <c r="H25" s="50"/>
-      <c r="I25" s="29"/>
-      <c r="J25" s="27" t="s">
-        <v>7</v>
-      </c>
+      <c r="G25" s="23"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="9"/>
     </row>
     <row r="26" spans="3:10" ht="15">
       <c r="C26" s="8"/>
-      <c r="D26" s="168" t="s">
-        <v>29</v>
-      </c>
-      <c r="E26" s="168"/>
-      <c r="F26" s="168"/>
-      <c r="G26" s="168"/>
-      <c r="H26" s="48"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="24"/>
       <c r="I26" s="11"/>
       <c r="J26" s="9"/>
     </row>
@@ -9545,86 +9571,85 @@
       <c r="D27" s="24"/>
       <c r="E27" s="32"/>
       <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="9"/>
+      <c r="G27" s="49">
+        <f>SUM(G10:G18)</f>
+        <v>7615000</v>
+      </c>
+      <c r="H27" s="50"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="27" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="28" spans="3:10" ht="15">
       <c r="C28" s="8"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="49">
-        <f>SUM(G27)</f>
-        <v>0</v>
-      </c>
-      <c r="H28" s="50"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="27" t="s">
-        <v>7</v>
-      </c>
+      <c r="D28" s="168" t="s">
+        <v>29</v>
+      </c>
+      <c r="E28" s="168"/>
+      <c r="F28" s="168"/>
+      <c r="G28" s="168"/>
+      <c r="H28" s="48"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="9"/>
     </row>
     <row r="29" spans="3:10" ht="15">
       <c r="C29" s="8"/>
-      <c r="D29" s="168" t="s">
+      <c r="D29" s="24"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="9"/>
+    </row>
+    <row r="30" spans="3:10" ht="15">
+      <c r="C30" s="8"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="49">
+        <f>SUM(G29)</f>
+        <v>0</v>
+      </c>
+      <c r="H30" s="50"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="3:10" ht="15">
+      <c r="C31" s="8"/>
+      <c r="D31" s="168" t="s">
         <v>26</v>
       </c>
-      <c r="E29" s="168"/>
-      <c r="F29" s="168"/>
-      <c r="G29" s="168"/>
-      <c r="H29" s="51"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="8"/>
-    </row>
-    <row r="30" spans="3:10" ht="15">
-      <c r="C30" s="8">
-        <v>1</v>
-      </c>
-      <c r="D30" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30" s="10"/>
-      <c r="F30" s="42"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="28"/>
-    </row>
-    <row r="31" spans="3:10" ht="15">
-      <c r="C31" s="8">
-        <v>2</v>
-      </c>
-      <c r="D31" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="10"/>
-      <c r="F31" s="42"/>
-      <c r="G31" s="44"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="18"/>
+      <c r="E31" s="168"/>
+      <c r="F31" s="168"/>
+      <c r="G31" s="168"/>
+      <c r="H31" s="51"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="8"/>
     </row>
     <row r="32" spans="3:10" ht="15">
       <c r="C32" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E32" s="10"/>
       <c r="F32" s="42"/>
       <c r="G32" s="44"/>
       <c r="H32" s="14"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="18"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="28"/>
     </row>
     <row r="33" spans="3:10" ht="15">
       <c r="C33" s="8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E33" s="10"/>
       <c r="F33" s="42"/>
@@ -9635,69 +9660,97 @@
     </row>
     <row r="34" spans="3:10" ht="15">
       <c r="C34" s="8">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="E34" s="10"/>
       <c r="F34" s="42"/>
-      <c r="G34" s="44">
-        <v>3600000</v>
-      </c>
-      <c r="H34" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="I34" s="14"/>
+      <c r="G34" s="44"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="11"/>
       <c r="J34" s="18"/>
     </row>
     <row r="35" spans="3:10" ht="15">
-      <c r="C35" s="8"/>
-      <c r="D35" s="30"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="47"/>
-      <c r="G35" s="45">
-        <f>SUM(G30:G34)</f>
-        <v>3600000</v>
-      </c>
-      <c r="H35" s="26"/>
-      <c r="I35" s="26"/>
-      <c r="J35" s="27" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="3:10">
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
+      <c r="C35" s="8">
+        <v>4</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="10"/>
+      <c r="F35" s="42"/>
+      <c r="G35" s="44"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="18"/>
+    </row>
+    <row r="36" spans="3:10" ht="15">
+      <c r="C36" s="8">
+        <v>5</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>64</v>
+      </c>
       <c r="E36" s="10"/>
       <c r="F36" s="42"/>
-      <c r="G36" s="42"/>
-      <c r="H36" s="19"/>
-      <c r="I36" s="19"/>
-      <c r="J36" s="8"/>
+      <c r="G36" s="44">
+        <v>3600000</v>
+      </c>
+      <c r="H36" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I36" s="14"/>
+      <c r="J36" s="18"/>
     </row>
     <row r="37" spans="3:10" ht="15">
       <c r="C37" s="8"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="42"/>
-      <c r="G37" s="52"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
-    </row>
-    <row r="38" spans="3:10" ht="15">
+      <c r="D37" s="30"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="47"/>
+      <c r="G37" s="45">
+        <f>SUM(G32:G36)</f>
+        <v>3600000</v>
+      </c>
+      <c r="H37" s="26"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="3:10">
       <c r="C38" s="8"/>
-      <c r="D38" s="17"/>
+      <c r="D38" s="8"/>
       <c r="E38" s="10"/>
       <c r="F38" s="42"/>
-      <c r="G38" s="43">
-        <f>G8-G25-G28-G35</f>
+      <c r="G38" s="42"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="8"/>
+    </row>
+    <row r="39" spans="3:10" ht="15">
+      <c r="C39" s="8"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="42"/>
+      <c r="G39" s="52"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+    </row>
+    <row r="40" spans="3:10" ht="15">
+      <c r="C40" s="8"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="42"/>
+      <c r="G40" s="43">
+        <f>G8-G27-G30-G37</f>
         <v>-11215000</v>
       </c>
-      <c r="H38" s="12"/>
-      <c r="I38" s="16"/>
-      <c r="J38" s="25" t="s">
+      <c r="H40" s="12"/>
+      <c r="I40" s="16"/>
+      <c r="J40" s="25" t="s">
         <v>25</v>
       </c>
     </row>
@@ -9706,8 +9759,8 @@
     <mergeCell ref="C2:J2"/>
     <mergeCell ref="D4:G4"/>
     <mergeCell ref="D9:G9"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="D29:G29"/>
+    <mergeCell ref="D28:G28"/>
+    <mergeCell ref="D31:G31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9718,7 +9771,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B76B0C4E-BB10-4A27-93F6-ECDC21CDE865}">
   <dimension ref="C2:J37"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update sau khi gửi màn hình sang TQ
</commit_message>
<xml_diff>
--- a/Project/TongHopQuy2.xlsx
+++ b/Project/TongHopQuy2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\03.ViTechSolution_LTD\04.Team_Log\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E384D2-DED1-4051-A8A3-5AA8DBF6B902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF270E14-8F7A-414D-BF81-5A413A5D8CE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="315">
   <si>
     <t>STT</t>
   </si>
@@ -1037,6 +1037,9 @@
   </si>
   <si>
     <t>Tuấn chuyển anh Khơ 2tr</t>
+  </si>
+  <si>
+    <t>Gửi màn hình + cảm ứng sang TQ</t>
   </si>
 </sst>
 </file>
@@ -2067,7 +2070,7 @@
       </c>
       <c r="J7" s="11">
         <f>sport1_p2</f>
-        <v>-11215000</v>
+        <v>-17813741</v>
       </c>
       <c r="K7" s="9"/>
     </row>
@@ -2105,7 +2108,7 @@
       <c r="I12" s="9"/>
       <c r="J12" s="12">
         <f>SUM(J4:J11)</f>
-        <v>-106572966.40000001</v>
+        <v>-113171707.40000001</v>
       </c>
       <c r="K12" s="13" t="s">
         <v>7</v>
@@ -9088,8 +9091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F413B64-656B-492A-8F7D-8434699F234E}">
   <dimension ref="C2:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28:G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -9365,7 +9368,7 @@
         <v>15000</v>
       </c>
       <c r="G16" s="23">
-        <f t="shared" ref="G16:G24" si="0">F16*E16</f>
+        <f t="shared" ref="G16:G25" si="0">F16*E16</f>
         <v>150000</v>
       </c>
       <c r="H16" s="34" t="s">
@@ -9548,11 +9551,22 @@
     </row>
     <row r="25" spans="3:10" ht="15">
       <c r="C25" s="8"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="24"/>
+      <c r="D25" s="24" t="s">
+        <v>314</v>
+      </c>
+      <c r="E25" s="32">
+        <v>1</v>
+      </c>
+      <c r="F25" s="23">
+        <v>1670000</v>
+      </c>
+      <c r="G25" s="23">
+        <f t="shared" si="0"/>
+        <v>1670000</v>
+      </c>
+      <c r="H25" s="24" t="s">
+        <v>9</v>
+      </c>
       <c r="I25" s="11"/>
       <c r="J25" s="9"/>
     </row>
@@ -9572,8 +9586,8 @@
       <c r="E27" s="32"/>
       <c r="F27" s="23"/>
       <c r="G27" s="49">
-        <f>SUM(G10:G18)</f>
-        <v>7615000</v>
+        <f>SUM(G10:G25)</f>
+        <v>14213741</v>
       </c>
       <c r="H27" s="50"/>
       <c r="I27" s="29"/>
@@ -9746,7 +9760,7 @@
       <c r="F40" s="42"/>
       <c r="G40" s="43">
         <f>G8-G27-G30-G37</f>
-        <v>-11215000</v>
+        <v>-17813741</v>
       </c>
       <c r="H40" s="12"/>
       <c r="I40" s="16"/>

</xml_diff>